<commit_message>
Update main.py, and csv_to_txt_converter.py with demo TXT file
</commit_message>
<xml_diff>
--- a/quantum_articles.xlsx
+++ b/quantum_articles.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C178"/>
+  <dimension ref="A1:C232"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -878,7 +878,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>InterQnet: a heterogeneous full-stack approach to co-designing scalable quantum networks</t>
+          <t>US Restricts Exports to Top Quantum Labs in China</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -888,14 +888,14 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiaWh0dHBzOi8vd3d3LmFubC5nb3YvaW50ZXJxbmV0LWEtaGV0ZXJvZ2VuZW91cy1mdWxsc3RhY2stYXBwcm9hY2gtdG8tY29kZXNpZ25pbmctc2NhbGFibGUtcXVhbnR1bS1uZXR3b3Jrc9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiSWh0dHBzOi8vd3cyLmFpcC5vcmcvZnlpL3VzLXJlc3RyaWN0cy1leHBvcnRzLXRvLXRvcC1xdWFudHVtLWxhYnMtaW4tY2hpbmHSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>US Restricts Exports to Top Quantum Labs in China</t>
+          <t>InterQnet: a heterogeneous full-stack approach to co-designing scalable quantum networks</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -905,14 +905,14 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiSWh0dHBzOi8vd3cyLmFpcC5vcmcvZnlpL3VzLXJlc3RyaWN0cy1leHBvcnRzLXRvLXRvcC1xdWFudHVtLWxhYnMtaW4tY2hpbmHSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiaWh0dHBzOi8vd3d3LmFubC5nb3YvaW50ZXJxbmV0LWEtaGV0ZXJvZ2VuZW91cy1mdWxsc3RhY2stYXBwcm9hY2gtdG8tY29kZXNpZ25pbmctc2NhbGFibGUtcXVhbnR1bS1uZXR3b3Jrc9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>First Quantum Minerals Ltd. stock rises Monday, outperforms market</t>
+          <t>How a quantum scientist, a nurse, and an economist are joining the fight against global poverty</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -922,14 +922,14 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMijgFodHRwczovL3d3dy5tYXJrZXR3YXRjaC5jb20vZGF0YS1uZXdzL2ZpcnN0LXF1YW50dW0tbWluZXJhbHMtbHRkLXN0b2NrLXJpc2VzLW1vbmRheS1vdXRwZXJmb3Jtcy1tYXJrZXQtNDU2YzAzNTMtZjI0ZTI5MDI3OTk3P21vZD1td19xdW90ZV9uZXdz0gGAAWh0dHBzOi8vd3d3Lm1hcmtldHdhdGNoLmNvbS9hbXAvZGF0YS1uZXdzL2ZpcnN0LXF1YW50dW0tbWluZXJhbHMtbHRkLXN0b2NrLXJpc2VzLW1vbmRheS1vdXRwZXJmb3Jtcy1tYXJrZXQtNDU2YzAzNTMtZjI0ZTI5MDI3OTk3?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiaWh0dHBzOi8vbmV3cy5taXQuZWR1LzIwMjQvaG93LXF1YW50dW0tc2NpZW50aXN0LW51cnNlLWVjb25vbWlzdC1qb2luaW5nLWZpZ2h0LWFnYWluc3QtZ2xvYmFsLXBvdmVydHktMDYxMNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>How a quantum scientist, a nurse, and an economist are joining the fight against global poverty</t>
+          <t>First Quantum Minerals Ltd. stock rises Monday, outperforms market</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -939,7 +939,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiaWh0dHBzOi8vbmV3cy5taXQuZWR1LzIwMjQvaG93LXF1YW50dW0tc2NpZW50aXN0LW51cnNlLWVjb25vbWlzdC1qb2luaW5nLWZpZ2h0LWFnYWluc3QtZ2xvYmFsLXBvdmVydHktMDYxMNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMijgFodHRwczovL3d3dy5tYXJrZXR3YXRjaC5jb20vZGF0YS1uZXdzL2ZpcnN0LXF1YW50dW0tbWluZXJhbHMtbHRkLXN0b2NrLXJpc2VzLW1vbmRheS1vdXRwZXJmb3Jtcy1tYXJrZXQtNDU2YzAzNTMtZjI0ZTI5MDI3OTk3P21vZD1td19xdW90ZV9uZXdz0gGAAWh0dHBzOi8vd3d3Lm1hcmtldHdhdGNoLmNvbS9hbXAvZGF0YS1uZXdzL2ZpcnN0LXF1YW50dW0tbWluZXJhbHMtbHRkLXN0b2NrLXJpc2VzLW1vbmRheS1vdXRwZXJmb3Jtcy1tYXJrZXQtNDU2YzAzNTMtZjI0ZTI5MDI3OTk3?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
@@ -1065,7 +1065,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Experimental quantum computational chemistry with optimized unitary coupled cluster ansatz</t>
+          <t>When quantum physicists met Freud and Jung</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1075,7 +1075,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiMmh0dHBzOi8vd3d3Lm5hdHVyZS5jb20vYXJ0aWNsZXMvczQxNTY3LTAyNC0wMjUzMC160gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiTGh0dHBzOi8vaWFpLnR2L2FydGljbGVzL3doZW4tcXVhbnR1bS1waHlzaWNpc3RzLW1ldC1mcmV1ZC1hbmQtanVuZy1hdWlkLTI4NTfSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
@@ -1099,7 +1099,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>When quantum physicists met Freud and Jung</t>
+          <t>Experimental quantum computational chemistry with optimized unitary coupled cluster ansatz</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1109,7 +1109,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiTGh0dHBzOi8vaWFpLnR2L2FydGljbGVzL3doZW4tcXVhbnR1bS1waHlzaWNpc3RzLW1ldC1mcmV1ZC1hbmQtanVuZy1hdWlkLTI4NTfSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiMmh0dHBzOi8vd3d3Lm5hdHVyZS5jb20vYXJ0aWNsZXMvczQxNTY3LTAyNC0wMjUzMC160gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
@@ -1133,7 +1133,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Riverlane, the company making quantum computing useful far sooner than anticipated</t>
+          <t>New technique could help build quantum computers of the future</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1143,14 +1143,14 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiemh0dHBzOi8vd3d3Lm1hZGR5bmVzcy5jb20vdWsvMjAyNC8wNi8xMS9yaXZlcmxhbmUtdGhlLWNvbXBhbnktbWFraW5nLXF1YW50dW0tY29tcHV0aW5nLXVzZWZ1bC1mYXItc29vbmVyLXRoYW4tYW50aWNpcGF0ZWQv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiO2h0dHBzOi8vcGh5cy5vcmcvbmV3cy8yMDI0LTA2LXRlY2huaXF1ZS1xdWFudHVtLWZ1dHVyZS5odG1s0gE6aHR0cHM6Ly9waHlzLm9yZy9uZXdzLzIwMjQtMDYtdGVjaG5pcXVlLXF1YW50dW0tZnV0dXJlLmFtcA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>New technique could help build quantum computers of the future</t>
+          <t>Riverlane, the company making quantum computing useful far sooner than anticipated</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1160,7 +1160,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiO2h0dHBzOi8vcGh5cy5vcmcvbmV3cy8yMDI0LTA2LXRlY2huaXF1ZS1xdWFudHVtLWZ1dHVyZS5odG1s0gE6aHR0cHM6Ly9waHlzLm9yZy9uZXdzLzIwMjQtMDYtdGVjaG5pcXVlLXF1YW50dW0tZnV0dXJlLmFtcA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiemh0dHBzOi8vd3d3Lm1hZGR5bmVzcy5jb20vdWsvMjAyNC8wNi8xMS9yaXZlcmxhbmUtdGhlLWNvbXBhbnktbWFraW5nLXF1YW50dW0tY29tcHV0aW5nLXVzZWZ1bC1mYXItc29vbmVyLXRoYW4tYW50aWNpcGF0ZWQv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
@@ -1303,7 +1303,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>D-Wave Quantum director sells warrants worth over $529k By Investing.com</t>
+          <t>Analogous electronic states in graphene and planer metallic quantum dots | Scientific Reports</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1313,14 +1313,14 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMibmh0dHBzOi8vd3d3LmludmVzdGluZy5jb20vbmV3cy9jb21wYW55LW5ld3MvZHdhdmUtcXVhbnR1bS1kaXJlY3Rvci1zZWxscy13YXJyYW50cy13b3J0aC1vdmVyLTUyOWstOTNDSC0zNDgyMjU20gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiMmh0dHBzOi8vd3d3Lm5hdHVyZS5jb20vYXJ0aWNsZXMvczQxNTk4LTAyNC02MzQ2NS0y0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Analogous electronic states in graphene and planer metallic quantum dots | Scientific Reports</t>
+          <t>Diraq, GlobalFoundries to Make Quantum Chips With Standard Tools</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1330,14 +1330,14 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiMmh0dHBzOi8vd3d3Lm5hdHVyZS5jb20vYXJ0aWNsZXMvczQxNTk4LTAyNC02MzQ2NS0y0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMicmh0dHBzOi8vd3d3LmJsb29tYmVyZy5jb20vbmV3cy9hcnRpY2xlcy8yMDI0LTA2LTEyL2RpcmFxLWdsb2JhbGZvdW5kcmllcy10by1tYWtlLXF1YW50dW0tY2hpcHMtd2l0aC1zdGFuZGFyZC10b29sc9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Diraq, GlobalFoundries to Make Quantum Chips With Standard Tools</t>
+          <t>D-Wave Quantum director sells warrants worth over $529k By Investing.com</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -1347,7 +1347,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMicmh0dHBzOi8vd3d3LmJsb29tYmVyZy5jb20vbmV3cy9hcnRpY2xlcy8yMDI0LTA2LTEyL2RpcmFxLWdsb2JhbGZvdW5kcmllcy10by1tYWtlLXF1YW50dW0tY2hpcHMtd2l0aC1zdGFuZGFyZC10b29sc9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMibmh0dHBzOi8vd3d3LmludmVzdGluZy5jb20vbmV3cy9jb21wYW55LW5ld3MvZHdhdmUtcXVhbnR1bS1kaXJlY3Rvci1zZWxscy13YXJyYW50cy13b3J0aC1vdmVyLTUyOWstOTNDSC0zNDgyMjU20gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
@@ -1371,7 +1371,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Vatican convenes astrophysicists to discuss black holes, quantum theory</t>
+          <t>Quantum Cybersecurity 'Must Be Priority' for Next Administration</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1381,7 +1381,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMib2h0dHBzOi8vd3d3Lm5jcm9ubGluZS5vcmcvZWFydGhiZWF0L3NjaWVuY2UvdmF0aWNhbi1jb252ZW5lcy1hc3Ryb3BoeXNpY2lzdHMtZGlzY3Vzcy1ibGFjay1ob2xlcy1xdWFudHVtLXRoZW9yedIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiaGh0dHBzOi8vdGhlcXVhbnR1bWluc2lkZXIuY29tLzIwMjQvMDYvMTIvcXVhbnR1bS1jeWJlcnNlY3VyaXR5LW11c3QtYmUtcHJpb3JpdHktZm9yLW5leHQtYWRtaW5pc3RyYXRpb24v0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
@@ -1405,7 +1405,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Quantum Cybersecurity 'Must Be Priority' for Next Administration</t>
+          <t>Vatican convenes astrophysicists to discuss black holes, quantum theory</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1415,7 +1415,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiaGh0dHBzOi8vdGhlcXVhbnR1bWluc2lkZXIuY29tLzIwMjQvMDYvMTIvcXVhbnR1bS1jeWJlcnNlY3VyaXR5LW11c3QtYmUtcHJpb3JpdHktZm9yLW5leHQtYWRtaW5pc3RyYXRpb24v0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMib2h0dHBzOi8vd3d3Lm5jcm9ubGluZS5vcmcvZWFydGhiZWF0L3NjaWVuY2UvdmF0aWNhbi1jb252ZW5lcy1hc3Ryb3BoeXNpY2lzdHMtZGlzY3Vzcy1ibGFjay1ob2xlcy1xdWFudHVtLXRoZW9yedIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
@@ -1524,7 +1524,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>CERN welcomes International Year of Quantum Science and Technology</t>
+          <t>Liquid crystals could improve quantum communication devices</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1534,14 +1534,14 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMibWh0dHBzOi8vaG9tZS5jZXJuL25ld3MvbmV3cy9rbm93bGVkZ2Utc2hhcmluZy9jZXJuLXdlbGNvbWVzLWludGVybmF0aW9uYWwteWVhci1xdWFudHVtLXNjaWVuY2UtYW5kLXRlY2hub2xvZ3nSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiaWh0dHBzOi8vd3d3Lm5ld3NjaWVudGlzdC5jb20vYXJ0aWNsZS8yNDM1MDEwLWxpcXVpZC1jcnlzdGFscy1jb3VsZC1pbXByb3ZlLXF1YW50dW0tY29tbXVuaWNhdGlvbi1kZXZpY2VzL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>DARPA's military-grade 'quantum laser' will use entangled photons to outshine conventional laser beams</t>
+          <t>Nu Quantum CEO: “The UK is Today a World Leader on Quantum”</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1551,14 +1551,14 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMilgFodHRwczovL3d3dy5saXZlc2NpZW5jZS5jb20vdGVjaG5vbG9neS9lbmdpbmVlcmluZy9kYXJwYXMtbWlsaXRhcnktZ3JhZGUtcXVhbnR1bS1sYXNlci13aWxsLXVzZS1lbnRhbmdsZWQtcGhvdG9ucy10by1vdXRzaGluZS1jb252ZW50aW9uYWwtbGFzZXItYmVhbXPSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiYmh0dHBzOi8vdGhlcXVhbnR1bWluc2lkZXIuY29tLzIwMjQvMDYvMTIvbnUtcXVhbnR1bS1jZW8tdGhlLXVrLWlzLXRvZGF5LWEtd29ybGQtbGVhZGVyLW9uLXF1YW50dW0v0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>OTI Lumionics Selects Nord Quantique to Test New Quantum Computing Applications for Materials Science</t>
+          <t>New theory links quantum geometry to electron-phonon coupling</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -1568,14 +1568,14 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMijwFodHRwczovL3RoZXF1YW50dW1pbnNpZGVyLmNvbS8yMDI0LzA2LzEyL290aS1sdW1pb25pY3Mtc2VsZWN0cy1ub3JkLXF1YW50aXF1ZS10by10ZXN0LW5ldy1xdWFudHVtLWNvbXB1dGluZy1hcHBsaWNhdGlvbnMtZm9yLW1hdGVyaWFscy1zY2llbmNlL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiSWh0dHBzOi8vcGh5cy5vcmcvbmV3cy8yMDI0LTA2LXRoZW9yeS1saW5rcy1xdWFudHVtLWdlb21ldHJ5LWVsZWN0cm9uLmh0bWzSAUhodHRwczovL3BoeXMub3JnL25ld3MvMjAyNC0wNi10aGVvcnktbGlua3MtcXVhbnR1bS1nZW9tZXRyeS1lbGVjdHJvbi5hbXA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>New theory links quantum geometry to electron-phonon coupling</t>
+          <t>Finalists Named for the Airbus-BMW Group Quantum Computing Challenge</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -1585,14 +1585,14 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiSWh0dHBzOi8vcGh5cy5vcmcvbmV3cy8yMDI0LTA2LXRoZW9yeS1saW5rcy1xdWFudHVtLWdlb21ldHJ5LWVsZWN0cm9uLmh0bWzSAUhodHRwczovL3BoeXMub3JnL25ld3MvMjAyNC0wNi10aGVvcnktbGlua3MtcXVhbnR1bS1nZW9tZXRyeS1lbGVjdHJvbi5hbXA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMibmh0dHBzOi8vdGhlcXVhbnR1bWluc2lkZXIuY29tLzIwMjQvMDYvMTIvZmluYWxpc3RzLW5hbWVkLWZvci10aGUtYWlyYnVzLWJtdy1ncm91cC1xdWFudHVtLWNvbXB1dGluZy1jaGFsbGVuZ2Uv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Nu Quantum CEO: “The UK is Today a World Leader on Quantum”</t>
+          <t>DARPA's military-grade 'quantum laser' will use entangled photons to outshine conventional laser beams</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -1602,14 +1602,14 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiYmh0dHBzOi8vdGhlcXVhbnR1bWluc2lkZXIuY29tLzIwMjQvMDYvMTIvbnUtcXVhbnR1bS1jZW8tdGhlLXVrLWlzLXRvZGF5LWEtd29ybGQtbGVhZGVyLW9uLXF1YW50dW0v0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMilgFodHRwczovL3d3dy5saXZlc2NpZW5jZS5jb20vdGVjaG5vbG9neS9lbmdpbmVlcmluZy9kYXJwYXMtbWlsaXRhcnktZ3JhZGUtcXVhbnR1bS1sYXNlci13aWxsLXVzZS1lbnRhbmdsZWQtcGhvdG9ucy10by1vdXRzaGluZS1jb252ZW50aW9uYWwtbGFzZXItYmVhbXPSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>New method integrates quantum dots with metasurfaces for enhanced luminescence</t>
+          <t>CERN welcomes International Year of Quantum Science and Technology</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -1619,14 +1619,14 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiUGh0dHBzOi8vcGh5cy5vcmcvbmV3cy8yMDI0LTA2LW1ldGhvZC1xdWFudHVtLWRvdHMtbWV0YXN1cmZhY2VzLWx1bWluZXNjZW5jZS5odG1s0gFPaHR0cHM6Ly9waHlzLm9yZy9uZXdzLzIwMjQtMDYtbWV0aG9kLXF1YW50dW0tZG90cy1tZXRhc3VyZmFjZXMtbHVtaW5lc2NlbmNlLmFtcA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMibWh0dHBzOi8vaG9tZS5jZXJuL25ld3MvbmV3cy9rbm93bGVkZ2Utc2hhcmluZy9jZXJuLXdlbGNvbWVzLWludGVybmF0aW9uYWwteWVhci1xdWFudHVtLXNjaWVuY2UtYW5kLXRlY2hub2xvZ3nSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Liquid crystals could improve quantum communication devices</t>
+          <t>New method integrates quantum dots with metasurfaces for enhanced luminescence</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -1636,14 +1636,14 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiaWh0dHBzOi8vd3d3Lm5ld3NjaWVudGlzdC5jb20vYXJ0aWNsZS8yNDM1MDEwLWxpcXVpZC1jcnlzdGFscy1jb3VsZC1pbXByb3ZlLXF1YW50dW0tY29tbXVuaWNhdGlvbi1kZXZpY2VzL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiUGh0dHBzOi8vcGh5cy5vcmcvbmV3cy8yMDI0LTA2LW1ldGhvZC1xdWFudHVtLWRvdHMtbWV0YXN1cmZhY2VzLWx1bWluZXNjZW5jZS5odG1s0gFPaHR0cHM6Ly9waHlzLm9yZy9uZXdzLzIwMjQtMDYtbWV0aG9kLXF1YW50dW0tZG90cy1tZXRhc3VyZmFjZXMtbHVtaW5lc2NlbmNlLmFtcA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Finalists Named for the Airbus-BMW Group Quantum Computing Challenge</t>
+          <t>OTI Lumionics Selects Nord Quantique to Test New Quantum Computing Applications for Materials Science</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -1653,7 +1653,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMibmh0dHBzOi8vdGhlcXVhbnR1bWluc2lkZXIuY29tLzIwMjQvMDYvMTIvZmluYWxpc3RzLW5hbWVkLWZvci10aGUtYWlyYnVzLWJtdy1ncm91cC1xdWFudHVtLWNvbXB1dGluZy1jaGFsbGVuZ2Uv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMijwFodHRwczovL3RoZXF1YW50dW1pbnNpZGVyLmNvbS8yMDI0LzA2LzEyL290aS1sdW1pb25pY3Mtc2VsZWN0cy1ub3JkLXF1YW50aXF1ZS10by10ZXN0LW5ldy1xdWFudHVtLWNvbXB1dGluZy1hcHBsaWNhdGlvbnMtZm9yLW1hdGVyaWFscy1zY2llbmNlL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
@@ -1694,7 +1694,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Simulator Lights the Way to Quantum Gravity Trial</t>
+          <t>Quantum sensor gets a read on tiny worm implanted with nanodiamonds</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -1704,14 +1704,14 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiZGh0dHA6Ly93d3cub3B0aWNhLW9wbi5vcmcvaG9tZS9uZXdzcm9vbS8yMDI0L2p1bmUvc2ltdWxhdG9yX2xpZ2h0c190aGVfd2F5X3RvX3F1YW50dW1fZ3Jhdml0eV90cmlhbC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMicWh0dHBzOi8vd3d3Lm5ld3NjaWVudGlzdC5jb20vYXJ0aWNsZS8yNDM1MTQwLXF1YW50dW0tc2Vuc29yLWdldHMtYS1yZWFkLW9uLXRpbnktd29ybS1pbXBsYW50ZWQtd2l0aC1uYW5vZGlhbW9uZHMv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Quantum sensor gets a read on tiny worm implanted with nanodiamonds</t>
+          <t>Simulator Lights the Way to Quantum Gravity Trial</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -1721,7 +1721,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMicWh0dHBzOi8vd3d3Lm5ld3NjaWVudGlzdC5jb20vYXJ0aWNsZS8yNDM1MTQwLXF1YW50dW0tc2Vuc29yLWdldHMtYS1yZWFkLW9uLXRpbnktd29ybS1pbXBsYW50ZWQtd2l0aC1uYW5vZGlhbW9uZHMv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiZGh0dHA6Ly93d3cub3B0aWNhLW9wbi5vcmcvaG9tZS9uZXdzcm9vbS8yMDI0L2p1bmUvc2ltdWxhdG9yX2xpZ2h0c190aGVfd2F5X3RvX3F1YW50dW1fZ3Jhdml0eV90cmlhbC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
@@ -1779,7 +1779,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Liquid crystal source of photon pairs opens path to new generation of quantum sources</t>
+          <t>First Quantum Minerals Ltd. stock falls Thursday, underperforms market</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -1789,14 +1789,14 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiRWh0dHBzOi8vcGh5cy5vcmcvbmV3cy8yMDI0LTA2LWxpcXVpZC1jcnlzdGFsLXNvdXJjZS1waG90b24tcGFpcnMuaHRtbNIBRGh0dHBzOi8vcGh5cy5vcmcvbmV3cy8yMDI0LTA2LWxpcXVpZC1jcnlzdGFsLXNvdXJjZS1waG90b24tcGFpcnMuYW1w?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMigAFodHRwczovL3d3dy5tYXJrZXR3YXRjaC5jb20vZGF0YS1uZXdzL2ZpcnN0LXF1YW50dW0tbWluZXJhbHMtbHRkLXN0b2NrLWZhbGxzLXRodXJzZGF5LXVuZGVycGVyZm9ybXMtbWFya2V0LWRjNjU1MmU5LTUwOWQyMjE0ZDUwZdIBhAFodHRwczovL3d3dy5tYXJrZXR3YXRjaC5jb20vYW1wL2RhdGEtbmV3cy9maXJzdC1xdWFudHVtLW1pbmVyYWxzLWx0ZC1zdG9jay1mYWxscy10aHVyc2RheS11bmRlcnBlcmZvcm1zLW1hcmtldC1kYzY1NTJlOS01MDlkMjIxNGQ1MGU?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Quantum Tech Sector Hiring Stays Soft</t>
+          <t>Semiconductor Quantum Light Sources</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -1806,7 +1806,7 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiSWh0dHBzOi8vd3d3LmhwY3dpcmUuY29tLzIwMjQvMDYvMTMvcXVhbnR1bS10ZWNoLXNlY3Rvci1oaXJpbmctc3RheXMtc29mdC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMigAFodHRwOi8vd3d3Lm9wdGljYS1vcG4ub3JnL2hvbWUvYm9va19yZXZpZXdzLzIwMjQvMDYyNC9zZW1pY29uZHVjdG9yX3F1YW50dW1fbGlnaHRfc291cmNlc19mdW5kYW1lbnRhbHNfdGVjaG5vbG9naWVzX2FuZF9kZXZpY2VzL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
@@ -1830,7 +1830,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Semiconductor Quantum Light Sources</t>
+          <t>Quantum Tech Sector Hiring Stays Soft</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -1840,48 +1840,48 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMigAFodHRwOi8vd3d3Lm9wdGljYS1vcG4ub3JnL2hvbWUvYm9va19yZXZpZXdzLzIwMjQvMDYyNC9zZW1pY29uZHVjdG9yX3F1YW50dW1fbGlnaHRfc291cmNlc19mdW5kYW1lbnRhbHNfdGVjaG5vbG9naWVzX2FuZF9kZXZpY2VzL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiSWh0dHBzOi8vd3d3LmhwY3dpcmUuY29tLzIwMjQvMDYvMTMvcXVhbnR1bS10ZWNoLXNlY3Rvci1oaXJpbmctc3RheXMtc29mdC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>First Quantum Minerals Ltd. stock falls Thursday, underperforms market</t>
+          <t>Underground quantum criticality is hot right now</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>2024-06-13 13:31:21.545640</t>
+          <t>2024-06-13 13:31:21.548155</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMigAFodHRwczovL3d3dy5tYXJrZXR3YXRjaC5jb20vZGF0YS1uZXdzL2ZpcnN0LXF1YW50dW0tbWluZXJhbHMtbHRkLXN0b2NrLWZhbGxzLXRodXJzZGF5LXVuZGVycGVyZm9ybXMtbWFya2V0LWRjNjU1MmU5LTUwOWQyMjE0ZDUwZdIBhAFodHRwczovL3d3dy5tYXJrZXR3YXRjaC5jb20vYW1wL2RhdGEtbmV3cy9maXJzdC1xdWFudHVtLW1pbmVyYWxzLWx0ZC1zdG9jay1mYWxscy10aHVyc2RheS11bmRlcnBlcmZvcm1zLW1hcmtldC1kYzY1NTJlOS01MDlkMjIxNGQ1MGU?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiMmh0dHBzOi8vd3d3Lm5hdHVyZS5jb20vYXJ0aWNsZXMvczQxNTY3LTAyNC0wMjU2OS150gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Underground quantum criticality is hot right now</t>
+          <t>Fascinating behavior of 'super photons' in the quantum realm</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>2024-06-13 13:31:21.548155</t>
+          <t>2024-06-13 13:31:21.548290</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiMmh0dHBzOi8vd3d3Lm5hdHVyZS5jb20vYXJ0aWNsZXMvczQxNTY3LTAyNC0wMjU2OS150gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiT2h0dHBzOi8vd3d3LmVhcnRoLmNvbS9uZXdzL3N1cGVyLXBob3RvbnMtZmFzY2luYXRpbmctYmVoYXZpb3ItaW4tcXVhbnR1bS1yZWFsbS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>United Nations Declares 2025 as International Year of Quantum Science and Technology</t>
+          <t>Diraq Achieves Record Accuracy For Quantum Computing Device Manufactured by Existing Semiconductor Infrastructure</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -1891,14 +1891,14 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMieGh0dHBzOi8vcXVhbnR1bWNvbXB1dGluZ3JlcG9ydC5jb20vdW5pdGVkLW5hdGlvbnMtZGVjbGFyZXMtMjAyNS1hcy1pbnRlcm5hdGlvbmFsLXllYXItb2YtcXVhbnR1bS1zY2llbmNlLWFuZC10ZWNobm9sb2d5L9IBfGh0dHBzOi8vcXVhbnR1bWNvbXB1dGluZ3JlcG9ydC5jb20vdW5pdGVkLW5hdGlvbnMtZGVjbGFyZXMtMjAyNS1hcy1pbnRlcm5hdGlvbmFsLXllYXItb2YtcXVhbnR1bS1zY2llbmNlLWFuZC10ZWNobm9sb2d5L2FtcC8?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMimwFodHRwczovL3RoZXF1YW50dW1pbnNpZGVyLmNvbS8yMDI0LzA2LzEzL2RpcmFxLWFjaGlldmVzLXJlY29yZC1hY2N1cmFjeS1mb3ItcXVhbnR1bS1jb21wdXRpbmctZGV2aWNlLW1hbnVmYWN0dXJlZC1ieS1leGlzdGluZy1zZW1pY29uZHVjdG9yLWluZnJhc3RydWN0dXJlL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Quantum data assimilation: A quantum leap in weather prediction</t>
+          <t>Quantum Teleportation Just Got Real: Achieving 90% Fidelity Amidst Noise</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -1908,14 +1908,14 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiMGh0dHBzOi8vd3d3LmV1cmVrYWxlcnQub3JnL25ld3MtcmVsZWFzZXMvMTA0Nzk1NNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiYGh0dHBzOi8vc2NpdGVjaGRhaWx5LmNvbS9xdWFudHVtLXRlbGVwb3J0YXRpb24tanVzdC1nb3QtcmVhbC1hY2hpZXZpbmctOTAtZmlkZWxpdHktYW1pZHN0LW5vaXNlL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Diraq Achieves Record Accuracy For Quantum Computing Device Manufactured by Existing Semiconductor Infrastructure</t>
+          <t>Recurrent quantum embedding neural network and its application in vulnerability detection | Scientific Reports</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -1925,14 +1925,14 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMimwFodHRwczovL3RoZXF1YW50dW1pbnNpZGVyLmNvbS8yMDI0LzA2LzEzL2RpcmFxLWFjaGlldmVzLXJlY29yZC1hY2N1cmFjeS1mb3ItcXVhbnR1bS1jb21wdXRpbmctZGV2aWNlLW1hbnVmYWN0dXJlZC1ieS1leGlzdGluZy1zZW1pY29uZHVjdG9yLWluZnJhc3RydWN0dXJlL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiMmh0dHBzOi8vd3d3Lm5hdHVyZS5jb20vYXJ0aWNsZXMvczQxNTk4LTAyNC02MzAyMS150gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Fascinating behavior of 'super photons' in the quantum realm</t>
+          <t>The Sphere in Las Vegas really is a 'quantum leap' for live music: Inside the first shows</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -1942,14 +1942,14 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiT2h0dHBzOi8vd3d3LmVhcnRoLmNvbS9uZXdzL3N1cGVyLXBob3RvbnMtZmFzY2luYXRpbmctYmVoYXZpb3ItaW4tcXVhbnR1bS1yZWFsbS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiSGh0dHBzOi8vY2EubmV3cy55YWhvby5jb20vc3BoZXJlLWxhcy12ZWdhcy1yZWFsbHktcXVhbnR1bS0xNDIwMjYzNTcuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>The Sphere in Las Vegas really is a 'quantum leap' for live music: Inside the first shows</t>
+          <t>United Nations Declares 2025 as International Year of Quantum Science and Technology</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -1959,7 +1959,7 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiSGh0dHBzOi8vY2EubmV3cy55YWhvby5jb20vc3BoZXJlLWxhcy12ZWdhcy1yZWFsbHktcXVhbnR1bS0xNDIwMjYzNTcuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMieGh0dHBzOi8vcXVhbnR1bWNvbXB1dGluZ3JlcG9ydC5jb20vdW5pdGVkLW5hdGlvbnMtZGVjbGFyZXMtMjAyNS1hcy1pbnRlcm5hdGlvbmFsLXllYXItb2YtcXVhbnR1bS1zY2llbmNlLWFuZC10ZWNobm9sb2d5L9IBfGh0dHBzOi8vcXVhbnR1bWNvbXB1dGluZ3JlcG9ydC5jb20vdW5pdGVkLW5hdGlvbnMtZGVjbGFyZXMtMjAyNS1hcy1pbnRlcm5hdGlvbmFsLXllYXItb2YtcXVhbnR1bS1zY2llbmNlLWFuZC10ZWNobm9sb2d5L2FtcC8?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
@@ -1983,7 +1983,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Recurrent quantum embedding neural network and its application in vulnerability detection | Scientific Reports</t>
+          <t>Riverlane Joins the Quantum Energy Initiative</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -1993,7 +1993,7 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiMmh0dHBzOi8vd3d3Lm5hdHVyZS5jb20vYXJ0aWNsZXMvczQxNTk4LTAyNC02MzAyMS150gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiV2h0dHBzOi8vdGhlcXVhbnR1bWluc2lkZXIuY29tLzIwMjQvMDYvMTMvcml2ZXJsYW5lLWpvaW5zLXRoZS1xdWFudHVtLWVuZXJneS1pbml0aWF0aXZlL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
@@ -2017,7 +2017,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Riverlane Joins the Quantum Energy Initiative</t>
+          <t>Unlock Generous Growth With These 3 Top Quantum Computing Stocks</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -2027,7 +2027,7 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiV2h0dHBzOi8vdGhlcXVhbnR1bWluc2lkZXIuY29tLzIwMjQvMDYvMTMvcml2ZXJsYW5lLWpvaW5zLXRoZS1xdWFudHVtLWVuZXJneS1pbml0aWF0aXZlL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMie2h0dHBzOi8vbWFya2V0cy5idXNpbmVzc2luc2lkZXIuY29tL25ld3Mvc3RvY2tzL3VubG9jay1nZW5lcm91cy1ncm93dGgtd2l0aC10aGVzZS0zLXRvcC1xdWFudHVtLWNvbXB1dGluZy1zdG9ja3MtMTAzMzQ3NzY0MNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
@@ -2051,7 +2051,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Quantum Teleportation Just Got Real: Achieving 90% Fidelity Amidst Noise</t>
+          <t>Estonia's Roadmap for Encryption in the Age of Quantum Computing</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -2061,14 +2061,14 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiYGh0dHBzOi8vc2NpdGVjaGRhaWx5LmNvbS9xdWFudHVtLXRlbGVwb3J0YXRpb24tanVzdC1nb3QtcmVhbC1hY2hpZXZpbmctOTAtZmlkZWxpdHktYW1pZHN0LW5vaXNlL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiaWh0dHBzOi8vdGhlcXVhbnR1bWluc2lkZXIuY29tLzIwMjQvMDYvMTMvZXN0b25pYXMtcm9hZG1hcC1mb3ItZW5jcnlwdGlvbi1pbi10aGUtYWdlLW9mLXF1YW50dW0tY29tcHV0aW5nL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Estonia's Roadmap for Encryption in the Age of Quantum Computing</t>
+          <t>Quantum data assimilation: A quantum leap in weather prediction</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -2078,24 +2078,24 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiaWh0dHBzOi8vdGhlcXVhbnR1bWluc2lkZXIuY29tLzIwMjQvMDYvMTMvZXN0b25pYXMtcm9hZG1hcC1mb3ItZW5jcnlwdGlvbi1pbi10aGUtYWdlLW9mLXF1YW50dW0tY29tcHV0aW5nL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiMGh0dHBzOi8vd3d3LmV1cmVrYWxlcnQub3JnL25ld3MtcmVsZWFzZXMvMTA0Nzk1NNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Unlock Generous Growth With These 3 Top Quantum Computing Stocks</t>
+          <t>Diraq Reports 99.9% Qubit Control Accuracy with imec-Produced Silicon Quantum Dot</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>2024-06-13 13:31:21.548290</t>
+          <t>2024-06-13 13:31:21.553304</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMie2h0dHBzOi8vbWFya2V0cy5idXNpbmVzc2luc2lkZXIuY29tL25ld3Mvc3RvY2tzL3VubG9jay1nZW5lcm91cy1ncm93dGgtd2l0aC10aGVzZS0zLXRvcC1xdWFudHVtLWNvbXB1dGluZy1zdG9ja3MtMTAzMzQ3NzY0MNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMidmh0dHBzOi8vd3d3LmhwY3dpcmUuY29tL29mZi10aGUtd2lyZS9kaXJhcS1yZXBvcnRzLTk5LTktcXViaXQtY29udHJvbC1hY2N1cmFjeS13aXRoLWltZWMtcHJvZHVjZWQtc2lsaWNvbi1xdWFudHVtLWRvdC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
@@ -2204,7 +2204,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Diraq Reports 99.9% Qubit Control Accuracy with imec-Produced Silicon Quantum Dot</t>
+          <t>Chip-Scale Visible Sources Aim to Release Quantum Technology from the Lab</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -2214,7 +2214,7 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMidmh0dHBzOi8vd3d3LmhwY3dpcmUuY29tL29mZi10aGUtd2lyZS9kaXJhcS1yZXBvcnRzLTk5LTktcXViaXQtY29udHJvbC1hY2N1cmFjeS13aXRoLWltZWMtcHJvZHVjZWQtc2lsaWNvbi1xdWFudHVtLWRvdC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiXmh0dHBzOi8vd3d3LnBob3Rvbmljcy5jb20vQXJ0aWNsZXMvQ2hpcC1TY2FsZV9WaXNpYmxlX1NvdXJjZXNfQWltX3RvX1JlbGVhc2VfUXVhbnR1bS9wNS9hNjk5NjPSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
@@ -2238,7 +2238,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Quantum, AI Combine to Transform Energy Generation, AI Summit London</t>
+          <t>IBM thinks it's ready to turn quantum computing into an actual business</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -2248,14 +2248,14 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiaGh0dHBzOi8vd3d3LmlvdHdvcmxkdG9kYXkuY29tL3F1YW50dW0vcXVhbnR1bS1haS1jb21iaW5lLXRvLXRyYW5zZm9ybS1lbmVyZ3ktZ2VuZXJhdGlvbi1haS1zdW1taXQtbG9uZG9u0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiRmh0dHBzOi8vbnoubmV3cy55YWhvby5jb20vaWJtLXRoaW5rcy1yZWFkeS10dXJuLXF1YW50dW0tMDUwMTAwNTc0Lmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Chip-Scale Visible Sources Aim to Release Quantum Technology from the Lab</t>
+          <t>Microsoft CEO says Azure Quantum will address the big challenges in computing</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -2265,14 +2265,14 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiXmh0dHBzOi8vd3d3LnBob3Rvbmljcy5jb20vQXJ0aWNsZXMvQ2hpcC1TY2FsZV9WaXNpYmxlX1NvdXJjZXNfQWltX3RvX1JlbGVhc2VfUXVhbnR1bS9wNS9hNjk5NjPSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiUGh0dHBzOi8vdWsuc3R5bGUueWFob28uY29tL3N0eWxlL21pY3Jvc29mdC1jZW8tc2F5cy1henVyZS1xdWFudHVtLTE2MjYwMTAxOC5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>IBM thinks it's ready to turn quantum computing into an actual business</t>
+          <t>Quantum Revolution “Living up to Hype,” Quantum Summit London</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -2282,14 +2282,14 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiRmh0dHBzOi8vbnoubmV3cy55YWhvby5jb20vaWJtLXRoaW5rcy1yZWFkeS10dXJuLXF1YW50dW0tMDUwMTAwNTc0Lmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiYGh0dHBzOi8vd3d3LmlvdHdvcmxkdG9kYXkuY29tL3F1YW50dW0vcXVhbnR1bS1yZXZvbHV0aW9uLWxpdmluZy11cC10by1oeXBlLXF1YW50dW0tc3VtbWl0LWxvbmRvbtIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Microsoft CEO says Azure Quantum will address the big challenges in computing</t>
+          <t>The Techy ASICS GEL-Quantum 360 VIII Mints Two “Digitune” Pack Pairs</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -2299,14 +2299,14 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiUGh0dHBzOi8vdWsuc3R5bGUueWFob28uY29tL3N0eWxlL21pY3Jvc29mdC1jZW8tc2F5cy1henVyZS1xdWFudHVtLTE2MjYwMTAxOC5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiVGh0dHBzOi8vc25lYWtlcm5ld3MuY29tLzIwMjQvMDYvMTMvYXNpY3MtZ2VsLXF1YW50dW0tMzYwLXZpaWktZGlnaXR1bmUtcmVsZWFzZS1kYXRlL9IBVGh0dHBzOi8vc25lYWtlcm5ld3MuY29tLzIwMjQvMDYvMTMvYXNpY3MtZ2VsLXF1YW50dW0tMzYwLXZpaWktZGlnaXR1bmUtcmVsZWFzZS1kYXRlLw?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Quantum Revolution “Living up to Hype,” Quantum Summit London</t>
+          <t>Quantum, AI Combine to Transform Energy Generation, AI Summit London</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -2316,14 +2316,14 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiYGh0dHBzOi8vd3d3LmlvdHdvcmxkdG9kYXkuY29tL3F1YW50dW0vcXVhbnR1bS1yZXZvbHV0aW9uLWxpdmluZy11cC10by1oeXBlLXF1YW50dW0tc3VtbWl0LWxvbmRvbtIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiaGh0dHBzOi8vd3d3LmlvdHdvcmxkdG9kYXkuY29tL3F1YW50dW0vcXVhbnR1bS1haS1jb21iaW5lLXRvLXRyYW5zZm9ybS1lbmVyZ3ktZ2VuZXJhdGlvbi1haS1zdW1taXQtbG9uZG9u0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>The Techy ASICS GEL-Quantum 360 VIII Mints Two “Digitune” Pack Pairs</t>
+          <t>Fermilab Opens Underground Facility for Quantum Information Science Research</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -2333,7 +2333,7 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiVGh0dHBzOi8vc25lYWtlcm5ld3MuY29tLzIwMjQvMDYvMTMvYXNpY3MtZ2VsLXF1YW50dW0tMzYwLXZpaWktZGlnaXR1bmUtcmVsZWFzZS1kYXRlL9IBVGh0dHBzOi8vc25lYWtlcm5ld3MuY29tLzIwMjQvMDYvMTMvYXNpY3MtZ2VsLXF1YW50dW0tMzYwLXZpaWktZGlnaXR1bmUtcmVsZWFzZS1kYXRlLw?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMibmh0dHBzOi8vZXhlY3V0aXZlZ292LmNvbS8yMDI0LzA2L2Zlcm1pbGFiLW9wZW5zLXVuZGVyZ3JvdW5kLWZhY2lsaXR5LWZvci1xdWFudHVtLWluZm9ybWF0aW9uLXNjaWVuY2UtcmVzZWFyY2gv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
@@ -2357,58 +2357,58 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Fermilab Opens Underground Facility for Quantum Information Science Research</t>
+          <t>Quantinuum AI Team's Advance Quickens Pace Toward Merging Quantum Computing And AI</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>2024-06-13 13:31:21.553304</t>
+          <t>2024-06-14 13:06:43.366610</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMibmh0dHBzOi8vZXhlY3V0aXZlZ292LmNvbS8yMDI0LzA2L2Zlcm1pbGFiLW9wZW5zLXVuZGVyZ3JvdW5kLWZhY2lsaXR5LWZvci1xdWFudHVtLWluZm9ybWF0aW9uLXNjaWVuY2UtcmVzZWFyY2gv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMie2h0dHBzOi8vdGhlcXVhbnR1bWluc2lkZXIuY29tLzIwMjQvMDYvMTQvcXVhbnRpbnV1bS1haS10ZWFtcy1hZHZhbmNlLXF1aWNrZW5zLXBhY2UtdG93YXJkLW1lcmdpbmctcXVhbnR1bS1jb21wdXRpbmctYW5kLWFpL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Quantinuum AI Team's Advance Quickens Pace Toward Merging Quantum Computing And AI</t>
+          <t>Quantum entanglement measures Earth rotation</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>2024-06-14 13:06:43.366610</t>
+          <t>2024-06-14 13:06:43.373729</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMie2h0dHBzOi8vdGhlcXVhbnR1bWluc2lkZXIuY29tLzIwMjQvMDYvMTQvcXVhbnRpbnV1bS1haS10ZWFtcy1hZHZhbmNlLXF1aWNrZW5zLXBhY2UtdG93YXJkLW1lcmdpbmctcXVhbnR1bS1jb21wdXRpbmctYW5kLWFpL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiMGh0dHBzOi8vd3d3LmV1cmVrYWxlcnQub3JnL25ld3MtcmVsZWFzZXMvMTA0ODA5NdIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Quantum entanglement measures Earth rotation</t>
+          <t>Closing Bell: First Quantum Minerals Ltd up on Monday (FM)</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>2024-06-14 13:06:43.373729</t>
+          <t>2024-06-14 13:31:21.538115</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiMGh0dHBzOi8vd3d3LmV1cmVrYWxlcnQub3JnL25ld3MtcmVsZWFzZXMvMTA0ODA5NdIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMijQFodHRwczovL3d3dy50aGVnbG9iZWFuZG1haWwuY29tL2ludmVzdGluZy9tYXJrZXRzL3N0b2Nrcy9GTS1UL3ByZXNzcmVsZWFzZXMvMjY3MzQ1MTkvY2xvc2luZy1iZWxsLWZpcnN0LXF1YW50dW0tbWluZXJhbHMtbHRkLXVwLW9uLW1vbmRheS1mbS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Physicists confirm quantum entanglement persists between top quarks, the heaviest known fundamental particles</t>
+          <t>No Small Thing: The U.K.'s Other Quantum Startups</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
@@ -2418,7 +2418,7 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiUmh0dHBzOi8vcGh5cy5vcmcvbmV3cy8yMDI0LTA2LXBoeXNpY2lzdHMtcXVhbnR1bS1lbnRhbmdsZW1lbnQtcGVyc2lzdHMtcXVhcmtzLmh0bWzSAVFodHRwczovL3BoeXMub3JnL25ld3MvMjAyNC0wNi1waHlzaWNpc3RzLXF1YW50dW0tZW50YW5nbGVtZW50LXBlcnNpc3RzLXF1YXJrcy5hbXA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMia2h0dHBzOi8vd3d3LmZvcmJlcy5jb20vc2l0ZXMvdHJldm9yY2xhd3Nvbi8yMDI0LzA2LzE0L25vLXNtYWxsLXRoaW5nLXF1YW50dW0tc3RhcnR1cHMtZm9yLXRoZS1oZXJlLWFuZC1ub3cv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
@@ -2442,41 +2442,41 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>No Small Thing: The U.K.'s Other Quantum Startups</t>
+          <t>D-Wave (NYSE: QBTS) Extends Partnership with Aramco Research Center to Help Maximize Quantum’s Positive Impact</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>2024-06-14 13:31:21.538115</t>
+          <t>2024-06-14 13:31:21.543127</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMia2h0dHBzOi8vd3d3LmZvcmJlcy5jb20vc2l0ZXMvdHJldm9yY2xhd3Nvbi8yMDI0LzA2LzE0L25vLXNtYWxsLXRoaW5nLXF1YW50dW0tc3RhcnR1cHMtZm9yLXRoZS1oZXJlLWFuZC1ub3cv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiwgFodHRwczovL3d3dy50aGVnbG9iZWFuZG1haWwuY29tL2ludmVzdGluZy9tYXJrZXRzL3N0b2Nrcy9RQlRTLU4vcHJlc3NyZWxlYXNlcy8yNjgyOTk2My9kLXdhdmUtbnlzZS1xYnRzLWV4dGVuZHMtcGFydG5lcnNoaXAtd2l0aC1hcmFtY28tcmVzZWFyY2gtY2VudGVyLXRvLWhlbHAtbWF4aW1pemUtcXVhbnR1bXMtcG9zaXRpdmUtaW1wYWN0L9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Closing Bell: First Quantum Minerals Ltd up on Monday (FM)</t>
+          <t>Midnight Sun Mining partners with KoBold Metals; First Quantum - MINING.COM</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>2024-06-14 13:31:21.538115</t>
+          <t>2024-06-14 13:31:21.543127</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMijQFodHRwczovL3d3dy50aGVnbG9iZWFuZG1haWwuY29tL2ludmVzdGluZy9tYXJrZXRzL3N0b2Nrcy9GTS1UL3ByZXNzcmVsZWFzZXMvMjY3MzQ1MTkvY2xvc2luZy1iZWxsLWZpcnN0LXF1YW50dW0tbWluZXJhbHMtbHRkLXVwLW9uLW1vbmRheS1mbS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiZ2h0dHBzOi8vd3d3Lm1pbmluZy5jb20vc3BvbnNvcmVkLWNvbnRlbnQvbWlkbmlnaHQtc3VuLW1pbmluZy1wYXJ0bmVycy13aXRoLWtvYm9sZC1tZXRhbHMtZmlyc3QtcXVhbnR1bS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Quantum entangled photons react to Earth's spin</t>
+          <t>Experimental observation of Earth's rotation with quantum entanglement</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
@@ -2486,14 +2486,14 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiSGh0dHBzOi8vcGh5cy5vcmcvbmV3cy8yMDI0LTA2LXF1YW50dW0tZW50YW5nbGVkLXBob3RvbnMtcmVhY3QtZWFydGguaHRtbNIBR2h0dHBzOi8vcGh5cy5vcmcvbmV3cy8yMDI0LTA2LXF1YW50dW0tZW50YW5nbGVkLXBob3RvbnMtcmVhY3QtZWFydGguYW1w?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiMmh0dHBzOi8vd3d3LnNjaWVuY2Uub3JnL2RvaS8xMC4xMTI2L3NjaWFkdi5hZG8wMjE10gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>When quantum dots meet blue phase liquid crystal elastomers</t>
+          <t>Physicists measured Earth's rotation using quantum entanglement</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -2503,14 +2503,14 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiQWh0dHBzOi8vcGh5cy5vcmcvbmV3cy8yMDI0LTA2LXF1YW50dW0tZG90cy1ibHVlLXBoYXNlLWxpcXVpZC5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiR2h0dHBzOi8vd3d3LnNjaWVuY2VuZXdzLm9yZy9hcnRpY2xlL2VhcnRoLXJvdGF0aW9uLXF1YW50dW0tZW50YW5nbGVtZW500gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>European quantum computing startup takes its funding to €32M with fresh raise</t>
+          <t>How Classical AI is 'Saving' Quantum Computing: A Talk with IBM's Ismael Faro</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -2520,347 +2520,347 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiWmh0dHBzOi8vY2EubW92aWVzLnlhaG9vLmNvbS9tb3ZpZXMvZXVyb3BlYW4tcXVhbnR1bS1jb21wdXRpbmctc3RhcnR1cC10YWtlcy0xMjMyNTEzNTIuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMic2h0dHBzOi8vdGhlcXVhbnR1bWluc2lkZXIuY29tLzIwMjQvMDYvMTQvaG93LWNsYXNzaWNhbC1haS1pcy1zYXZpbmctcXVhbnR1bS1jb21wdXRpbmctYS10YWxrLXdpdGgtaWJtcy1pc21hZWwtZmFyby_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Unlocking the Future of Quantum Computing: Insights from Paul Terry, CEO of Photonic Inc.</t>
+          <t>SpaceX launches 'zero fuel' engine into space</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>2024-06-14 13:31:21.543127</t>
+          <t>2024-06-14 13:31:21.545640</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMigAFodHRwczovL3RoZXF1YW50dW1pbnNpZGVyLmNvbS8yMDI0LzA2LzE0L3VubG9ja2luZy10aGUtZnV0dXJlLW9mLXF1YW50dW0tY29tcHV0aW5nLWluc2lnaHRzLWZyb20tcGF1bC10ZXJyeS1jZW8tb2YtcGhvdG9uaWMtaW5jL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiT2h0dHBzOi8vY2Euc3R5bGUueWFob28uY29tL25ld3Mvc3BhY2V4LWxhdW5jaGVzLXplcm8tZnVlbC1lbmdpbmUtMTQ1NDAzODYyLmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>D-Wave (NYSE: QBTS) Extends Partnership with Aramco Research Center to Help Maximize Quantum’s Positive Impact</t>
+          <t>'Escape From Shadow Physics' Review: Quantum Weirdness</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>2024-06-14 13:31:21.543127</t>
+          <t>2024-06-14 13:31:21.548290</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiwgFodHRwczovL3d3dy50aGVnbG9iZWFuZG1haWwuY29tL2ludmVzdGluZy9tYXJrZXRzL3N0b2Nrcy9RQlRTLU4vcHJlc3NyZWxlYXNlcy8yNjgyOTk2My9kLXdhdmUtbnlzZS1xYnRzLWV4dGVuZHMtcGFydG5lcnNoaXAtd2l0aC1hcmFtY28tcmVzZWFyY2gtY2VudGVyLXRvLWhlbHAtbWF4aW1pemUtcXVhbnR1bXMtcG9zaXRpdmUtaW1wYWN0L9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiaWh0dHBzOi8vd3d3Lm1zbi5jb20vZW4tdXMvbmV3cy90ZWNobm9sb2d5L2VzY2FwZS1mcm9tLXNoYWRvdy1waHlzaWNzLXJldmlldy1xdWFudHVtLXdlaXJkbmVzcy9hci1CQjFvZU5wUNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Midnight Sun Mining partners with KoBold Metals; First Quantum - MINING.COM</t>
+          <t>The Growing Interest in On-Prem Quantum Computing - High-Performance Computing News Analysis</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>2024-06-14 13:31:21.543127</t>
+          <t>2024-06-14 13:31:21.548290</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiZ2h0dHBzOi8vd3d3Lm1pbmluZy5jb20vc3BvbnNvcmVkLWNvbnRlbnQvbWlkbmlnaHQtc3VuLW1pbmluZy1wYXJ0bmVycy13aXRoLWtvYm9sZC1tZXRhbHMtZmlyc3QtcXVhbnR1bS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiUGh0dHBzOi8vaW5zaWRlaHBjLmNvbS8yMDI0LzA2L3RoZS1ncm93aW5nLWludGVyZXN0LWluLW9uLXByZW0tcXVhbnR1bS1jb21wdXRpbmcv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Quantum computers are like kaleidoscopes − why unusual metaphors help illustrate science and technology</t>
+          <t>Scott Bakula Addresses 'Quantum Leap' Reboot Involvement Speculation, Says It Was “Very Difficult Decision” To Pass ...</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>2024-06-14 13:31:21.543127</t>
+          <t>2024-06-14 13:31:21.548290</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiiAFodHRwczovL3RoZWNvbnZlcnNhdGlvbi5jb20vcXVhbnR1bS1jb21wdXRlcnMtYXJlLWxpa2Uta2FsZWlkb3Njb3Blcy13aHktdW51c3VhbC1tZXRhcGhvcnMtaGVscC1pbGx1c3RyYXRlLXNjaWVuY2UtYW5kLXRlY2hub2xvZ3ktMjI4MTc40gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiTmh0dHBzOi8vY2EubW92aWVzLnlhaG9vLmNvbS9zY290dC1iYWt1bGEtYWRkcmVzc2VzLXF1YW50dW0tbGVhcC0yMjA5NDUzNzMuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Physicists Measure Earth’s Rotation Using Quantum Entanglement</t>
+          <t>Diraq is going to make a hybrid chip combining quantum and classical processors</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>2024-06-14 13:31:21.543127</t>
+          <t>2024-06-14 13:31:21.553304</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiWGh0dHBzOi8vd3d3LnNjaS5uZXdzL3BoeXNpY3MvZWFydGhzLXJvdGF0aW9uLXF1YW50dW0tZW50YW5nbGVtZW50LW1lYXN1cmVtZW50LTEzMDIwLmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMihQFodHRwczovL3d3dy5zdGFydHVwZGFpbHkubmV0L3RvcGljL3F1YW50dW0tY29tcHV0aW5nL2RpcmFxLWlzLWdvaW5nLXRvLW1ha2UtYS1oeWJyaWQtY2hpcC1jb21iaW5pbmctcXVhbnR1bS1hbmQtY2xhc3NpY2FsLXByb2Nlc3NvcnMv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Experimental observation of Earth's rotation with quantum entanglement</t>
+          <t>Physicists confirm quantum entanglement persists between top quarks, the heaviest known fundamental particles</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>2024-06-14 13:31:21.543127</t>
+          <t>2024-06-14 14:00:59.908773</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiMmh0dHBzOi8vd3d3LnNjaWVuY2Uub3JnL2RvaS8xMC4xMTI2L3NjaWFkdi5hZG8wMjE10gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiUmh0dHBzOi8vcGh5cy5vcmcvbmV3cy8yMDI0LTA2LXBoeXNpY2lzdHMtcXVhbnR1bS1lbnRhbmdsZW1lbnQtcGVyc2lzdHMtcXVhcmtzLmh0bWzSAVFodHRwczovL3BoeXMub3JnL25ld3MvMjAyNC0wNi1waHlzaWNpc3RzLXF1YW50dW0tZW50YW5nbGVtZW50LXBlcnNpc3RzLXF1YXJrcy5hbXA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Physicists measured Earth's rotation using quantum entanglement</t>
+          <t>IQC celebrates latest Dean of Science Award winners</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>2024-06-14 13:31:21.543127</t>
+          <t>2024-06-14 14:00:59.908773</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiR2h0dHBzOi8vd3d3LnNjaWVuY2VuZXdzLm9yZy9hcnRpY2xlL2VhcnRoLXJvdGF0aW9uLXF1YW50dW0tZW50YW5nbGVtZW500gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiamh0dHBzOi8vdXdhdGVybG9vLmNhL2luc3RpdHV0ZS1mb3ItcXVhbnR1bS1jb21wdXRpbmcvbmV3cy9pcWMtY2VsZWJyYXRlcy1sYXRlc3QtZGVhbi1zY2llbmNlLWF3YXJkLXdpbm5lcnPSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>How Classical AI is 'Saving' Quantum Computing: A Talk with IBM's Ismael Faro</t>
+          <t>First Quantum Minerals Ltd (FM-T) Quote - Press Release</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>2024-06-14 13:31:21.543127</t>
+          <t>2024-06-14 14:00:59.908773</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMic2h0dHBzOi8vdGhlcXVhbnR1bWluc2lkZXIuY29tLzIwMjQvMDYvMTQvaG93LWNsYXNzaWNhbC1haS1pcy1zYXZpbmctcXVhbnR1bS1jb21wdXRpbmctYS10YWxrLXdpdGgtaWJtcy1pc21hZWwtZmFyby_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMijQFodHRwczovL3d3dy50aGVnbG9iZWFuZG1haWwuY29tL2ludmVzdGluZy9tYXJrZXRzL3N0b2Nrcy9GTS1UL3ByZXNzcmVsZWFzZXMvMjY3MzQ1MTkvY2xvc2luZy1iZWxsLWZpcnN0LXF1YW50dW0tbWluZXJhbHMtbHRkLXVwLW9uLW1vbmRheS1mbS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>First Quantum Minerals Ltd. stock rises Friday, outperforms market</t>
+          <t>Experimental observation of Earth’s rotation with quantum entanglement</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>2024-06-14 13:31:21.545640</t>
+          <t>2024-06-14 14:00:59.908773</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMijgFodHRwczovL3d3dy5tYXJrZXR3YXRjaC5jb20vZGF0YS1uZXdzL2ZpcnN0LXF1YW50dW0tbWluZXJhbHMtbHRkLXN0b2NrLXJpc2VzLWZyaWRheS1vdXRwZXJmb3Jtcy1tYXJrZXQtNDIwMWM3NGEtZTk4OTFkYjhlNTBjP21vZD1td19xdW90ZV9uZXdz0gGAAWh0dHBzOi8vd3d3Lm1hcmtldHdhdGNoLmNvbS9hbXAvZGF0YS1uZXdzL2ZpcnN0LXF1YW50dW0tbWluZXJhbHMtbHRkLXN0b2NrLXJpc2VzLWZyaWRheS1vdXRwZXJmb3Jtcy1tYXJrZXQtNDIwMWM3NGEtZTk4OTFkYjhlNTBj?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiMmh0dHBzOi8vd3d3LnNjaWVuY2Uub3JnL2RvaS8xMC4xMTI2L3NjaWFkdi5hZG8wMjE10gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>Purified Silicon Makes Bigger, Faster Quantum Computers</t>
+          <t>Quantum computers are like kaleidoscopes − why unusual metaphors help illustrate science and technology</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>2024-06-14 13:31:21.545640</t>
+          <t>2024-06-14 14:00:59.908773</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiP2h0dHBzOi8vc3BlY3RydW0uaWVlZS5vcmcvc2lsaWNvbi1xdWFudHVtLWNvbXB1dGluZy1wdXJpZmllZC1zadIBTmh0dHBzOi8vc3BlY3RydW0uaWVlZS5vcmcvYW1wL3NpbGljb24tcXVhbnR1bS1jb21wdXRpbmctcHVyaWZpZWQtc2ktMjY2ODQ4NzY3Mw?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiiAFodHRwczovL3RoZWNvbnZlcnNhdGlvbi5jb20vcXVhbnR1bS1jb21wdXRlcnMtYXJlLWxpa2Uta2FsZWlkb3Njb3Blcy13aHktdW51c3VhbC1tZXRhcGhvcnMtaGVscC1pbGx1c3RyYXRlLXNjaWVuY2UtYW5kLXRlY2hub2xvZ3ktMjI4MTc40gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Innovation Lightbulb: Private Investment in Quantum Technology</t>
+          <t>Physicists measured Earth’s rotation using quantum entanglement</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>2024-06-14 13:31:21.545640</t>
+          <t>2024-06-14 14:00:59.908773</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiWGh0dHBzOi8vd3d3LmNzaXMub3JnL2FuYWx5c2lzL2lubm92YXRpb24tbGlnaHRidWxiLXByaXZhdGUtaW52ZXN0bWVudC1xdWFudHVtLXRlY2hub2xvZ3nSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiR2h0dHBzOi8vd3d3LnNjaWVuY2VuZXdzLm9yZy9hcnRpY2xlL2VhcnRoLXJvdGF0aW9uLXF1YW50dW0tZW50YW5nbGVtZW500gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>SpaceX launches 'zero fuel' engine into space</t>
+          <t>No Small Thing: Quantum Startups For The Here And Now</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>2024-06-14 13:31:21.545640</t>
+          <t>2024-06-14 14:00:59.908773</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiT2h0dHBzOi8vY2Euc3R5bGUueWFob28uY29tL25ld3Mvc3BhY2V4LWxhdW5jaGVzLXplcm8tZnVlbC1lbmdpbmUtMTQ1NDAzODYyLmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMia2h0dHBzOi8vd3d3LmZvcmJlcy5jb20vc2l0ZXMvdHJldm9yY2xhd3Nvbi8yMDI0LzA2LzE0L25vLXNtYWxsLXRoaW5nLXF1YW50dW0tc3RhcnR1cHMtZm9yLXRoZS1oZXJlLWFuZC1ub3cv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>Many-excitation removal of a transmon qubit using a single-junction quantum-circuit refrigerator and a two-tone ...</t>
+          <t>Midnight Sun Mining partners with KoBold Metals; First Quantum</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>2024-06-14 13:31:21.548290</t>
+          <t>2024-06-14 14:00:59.908773</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiMmh0dHBzOi8vd3d3Lm5hdHVyZS5jb20vYXJ0aWNsZXMvczQxNTk4LTAyNC02NDQ5Ni010gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiZ2h0dHBzOi8vd3d3Lm1pbmluZy5jb20vc3BvbnNvcmVkLWNvbnRlbnQvbWlkbmlnaHQtc3VuLW1pbmluZy1wYXJ0bmVycy13aXRoLWtvYm9sZC1tZXRhbHMtZmlyc3QtcXVhbnR1bS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>A portable quantum simulator on a silicon chip</t>
+          <t>Innovation Lightbulb: Private Investment in Quantum Technology</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>2024-06-14 13:31:21.548290</t>
+          <t>2024-06-14 14:00:59.912386</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiY2h0dHBzOi8vd3d3Lm9wZW5hY2Nlc3Nnb3Zlcm5tZW50Lm9yZy9hcnRpY2xlL2EtcG9ydGFibGUtcXVhbnR1bS1zaW11bGF0b3Itb24tYS1zaWxpY29uLWNoaXAvMTc4MTYxL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiWGh0dHBzOi8vd3d3LmNzaXMub3JnL2FuYWx5c2lzL2lubm92YXRpb24tbGlnaHRidWxiLXByaXZhdGUtaW52ZXN0bWVudC1xdWFudHVtLXRlY2hub2xvZ3nSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>The Growing Interest in On-Prem Quantum Computing - High-Performance Computing News Analysis</t>
+          <t>Physicists Measure Earth’s Rotation Using Quantum Entanglement</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>2024-06-14 13:31:21.548290</t>
+          <t>2024-06-14 14:00:59.912386</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiUGh0dHBzOi8vaW5zaWRlaHBjLmNvbS8yMDI0LzA2L3RoZS1ncm93aW5nLWludGVyZXN0LWluLW9uLXByZW0tcXVhbnR1bS1jb21wdXRpbmcv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiWGh0dHBzOi8vd3d3LnNjaS5uZXdzL3BoeXNpY3MvZWFydGhzLXJvdGF0aW9uLXF1YW50dW0tZW50YW5nbGVtZW50LW1lYXN1cmVtZW50LTEzMDIwLmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>Scott Bakula Addresses 'Quantum Leap' Reboot Involvement Speculation, Says It Was “Very Difficult Decision” To Pass ...</t>
+          <t>When quantum dots meet blue phase liquid crystal elastomers</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>2024-06-14 13:31:21.548290</t>
+          <t>2024-06-14 14:00:59.912386</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiTmh0dHBzOi8vY2EubW92aWVzLnlhaG9vLmNvbS9zY290dC1iYWt1bGEtYWRkcmVzc2VzLXF1YW50dW0tbGVhcC0yMjA5NDUzNzMuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiQWh0dHBzOi8vcGh5cy5vcmcvbmV3cy8yMDI0LTA2LXF1YW50dW0tZG90cy1ibHVlLXBoYXNlLWxpcXVpZC5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>Quantum Defies Fossil Fuel Flight with $5.8B Target</t>
+          <t>D-Wave Quantum Inc (QBTS-N) Quote - Press Release</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>2024-06-14 13:31:21.548290</t>
+          <t>2024-06-14 14:00:59.912386</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiYGh0dHBzOi8vd3d3LnRoZW1pZGRsZW1hcmtldC5jb20vbmV3cy1hbmFseXNpcy9xdWFudHVtLWRlZmllcy1mb3NzaWwtZnVlbC1mbGlnaHQtd2l0aC01LThiLXRhcmdldNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiwgFodHRwczovL3d3dy50aGVnbG9iZWFuZG1haWwuY29tL2ludmVzdGluZy9tYXJrZXRzL3N0b2Nrcy9RQlRTLU4vcHJlc3NyZWxlYXNlcy8yNjgyOTk2My9kLXdhdmUtbnlzZS1xYnRzLWV4dGVuZHMtcGFydG5lcnNoaXAtd2l0aC1hcmFtY28tcmVzZWFyY2gtY2VudGVyLXRvLWhlbHAtbWF4aW1pemUtcXVhbnR1bXMtcG9zaXRpdmUtaW1wYWN0L9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>'Escape From Shadow Physics' Review: Quantum Weirdness</t>
+          <t>Quantum Computing Revolutionizes Data Assimilation</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>2024-06-14 13:31:21.548290</t>
+          <t>2024-06-14 14:00:59.912386</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiaWh0dHBzOi8vd3d3Lm1zbi5jb20vZW4tdXMvbmV3cy90ZWNobm9sb2d5L2VzY2FwZS1mcm9tLXNoYWRvdy1waHlzaWNzLXJldmlldy1xdWFudHVtLXdlaXJkbmVzcy9hci1CQjFvZU5wUNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiMWh0dHBzOi8vd3d3LmF6b3F1YW50dW0uY29tL05ld3MuYXNweD9uZXdzSUQ9MTAzMjHSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>When quantum dots meet blue phase liquid crystal elastomers: visualized full-color and mechanically-switchable ...</t>
+          <t>How Classical AI is ‘Saving’ Quantum Computing: A Talk with IBM’s Ismael Faro</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>2024-06-14 13:31:21.548290</t>
+          <t>2024-06-14 14:00:59.912386</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiMmh0dHBzOi8vd3d3Lm5hdHVyZS5jb20vYXJ0aWNsZXMvczQxMzc3LTAyNC0wMTQ3OS0x0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMic2h0dHBzOi8vdGhlcXVhbnR1bWluc2lkZXIuY29tLzIwMjQvMDYvMTQvaG93LWNsYXNzaWNhbC1haS1pcy1zYXZpbmctcXVhbnR1bS1jb21wdXRpbmctYS10YWxrLXdpdGgtaWJtcy1pc21hZWwtZmFyby_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>Quantum technologies take off!</t>
+          <t>The Growing Interest in On-Prem Quantum Computing</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>2024-06-14 13:31:21.548290</t>
+          <t>2024-06-14 14:00:59.912386</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiVmh0dHBzOi8vd3d3Lmxhc2VyZm9jdXN3b3JsZC5jb20vcXVhbnR1bS9hcnRpY2xlLzU1MDg4MzY2L3F1YW50dW0tdGVjaG5vbG9naWVzLXRha2Utb2Zm0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiUGh0dHBzOi8vaW5zaWRlaHBjLmNvbS8yMDI0LzA2L3RoZS1ncm93aW5nLWludGVyZXN0LWluLW9uLXByZW0tcXVhbnR1bS1jb21wdXRpbmcv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
@@ -2872,7 +2872,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>2024-06-14 13:31:21.548290</t>
+          <t>2024-06-14 14:00:59.912386</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
@@ -2884,17 +2884,17 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>Earth's rotation measured 1000x better with quantum entanglement</t>
+          <t>Unlocking the Future of Quantum Computing: Insights from Paul Terry, CEO of Photonic Inc.</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>2024-06-14 13:31:21.548290</t>
+          <t>2024-06-14 14:00:59.912386</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiVmh0dHBzOi8vaW50ZXJlc3RpbmdlbmdpbmVlcmluZy5jb20vc2NpZW5jZS9xdWFudHVtLWVudGFuZ2xlbWVudC1tZWFzdXJlLWVhcnRoLXJvdGF0aW9u0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMigAFodHRwczovL3RoZXF1YW50dW1pbnNpZGVyLmNvbS8yMDI0LzA2LzE0L3VubG9ja2luZy10aGUtZnV0dXJlLW9mLXF1YW50dW0tY29tcHV0aW5nLWluc2lnaHRzLWZyb20tcGF1bC10ZXJyeS1jZW8tb2YtcGhvdG9uaWMtaW5jL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
@@ -2906,7 +2906,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>2024-06-14 13:31:21.548290</t>
+          <t>2024-06-14 14:00:59.912386</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
@@ -2918,544 +2918,1462 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>Quantum Computing Revolutionizes Data Assimilation</t>
+          <t>First Quantum Minerals Ltd. stock rises Friday, outperforms market</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>2024-06-14 13:31:21.548290</t>
+          <t>2024-06-14 14:00:59.912386</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiMWh0dHBzOi8vd3d3LmF6b3F1YW50dW0uY29tL05ld3MuYXNweD9uZXdzSUQ9MTAzMjHSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMijgFodHRwczovL3d3dy5tYXJrZXR3YXRjaC5jb20vZGF0YS1uZXdzL2ZpcnN0LXF1YW50dW0tbWluZXJhbHMtbHRkLXN0b2NrLXJpc2VzLWZyaWRheS1vdXRwZXJmb3Jtcy1tYXJrZXQtNDIwMWM3NGEtZTk4OTFkYjhlNTBjP21vZD1td19xdW90ZV9uZXdz0gGAAWh0dHBzOi8vd3d3Lm1hcmtldHdhdGNoLmNvbS9hbXAvZGF0YS1uZXdzL2ZpcnN0LXF1YW50dW0tbWluZXJhbHMtbHRkLXN0b2NrLXJpc2VzLWZyaWRheS1vdXRwZXJmb3Jtcy1tYXJrZXQtNDIwMWM3NGEtZTk4OTFkYjhlNTBj?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>Quantum Computing Inc. Releases Preliminary Financial Results for Q1 2024</t>
+          <t>European quantum computing startup takes its funding to €32M with fresh raise</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>2024-06-14 13:31:21.548290</t>
+          <t>2024-06-14 14:00:59.912386</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMia2h0dHBzOi8vcXVhbnR1bWNvbXB1dGluZ3JlcG9ydC5jb20vcXVhbnR1bS1jb21wdXRpbmctaW5jLXJlbGVhc2UtcHJlbGltaW5hcnktZmluYW5jaWFsLXJlc3VsdHMtZm9yLXExLTIwMjQv0gFvaHR0cHM6Ly9xdWFudHVtY29tcHV0aW5ncmVwb3J0LmNvbS9xdWFudHVtLWNvbXB1dGluZy1pbmMtcmVsZWFzZS1wcmVsaW1pbmFyeS1maW5hbmNpYWwtcmVzdWx0cy1mb3ItcTEtMjAyNC9hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiWmh0dHBzOi8vY2EubW92aWVzLnlhaG9vLmNvbS9tb3ZpZXMvZXVyb3BlYW4tcXVhbnR1bS1jb21wdXRpbmctc3RhcnR1cC10YWtlcy0xMjMyNTEzNTIuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>Diraq is going to make a hybrid chip combining quantum and classical processors</t>
+          <t>Quantum Computing Inc. Releases Preliminary Financial Results for Q1 2024</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>2024-06-14 13:31:21.553304</t>
+          <t>2024-06-14 14:00:59.912386</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMihQFodHRwczovL3d3dy5zdGFydHVwZGFpbHkubmV0L3RvcGljL3F1YW50dW0tY29tcHV0aW5nL2RpcmFxLWlzLWdvaW5nLXRvLW1ha2UtYS1oeWJyaWQtY2hpcC1jb21iaW5pbmctcXVhbnR1bS1hbmQtY2xhc3NpY2FsLXByb2Nlc3NvcnMv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMia2h0dHBzOi8vcXVhbnR1bWNvbXB1dGluZ3JlcG9ydC5jb20vcXVhbnR1bS1jb21wdXRpbmctaW5jLXJlbGVhc2UtcHJlbGltaW5hcnktZmluYW5jaWFsLXJlc3VsdHMtZm9yLXExLTIwMjQv0gFvaHR0cHM6Ly9xdWFudHVtY29tcHV0aW5ncmVwb3J0LmNvbS9xdWFudHVtLWNvbXB1dGluZy1pbmMtcmVsZWFzZS1wcmVsaW1pbmFyeS1maW5hbmNpYWwtcmVzdWx0cy1mb3ItcTEtMjAyNC9hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>Lantronix Wins 2024 IoT Evolution Asset Tracking Award for FOX3 Telematic Gateway</t>
+          <t>Quantum technologies take off!</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>2024-06-14 13:31:21.553304</t>
+          <t>2024-06-14 14:00:59.912386</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMinAFodHRwczovL3d3dy5nbG9iZW5ld3N3aXJlLmNvbS9lbi9uZXdzLXJlbGVhc2UvMjAyNC8wNi8xMy8yODk4MTQ0LzAvZW4vTGFudHJvbml4LVdpbnMtMjAyNC1Jb1QtRXZvbHV0aW9uLUFzc2V0LVRyYWNraW5nLUF3YXJkLWZvci1GT1gzLVRlbGVtYXRpYy1HYXRld2F5Lmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiVmh0dHBzOi8vd3d3Lmxhc2VyZm9jdXN3b3JsZC5jb20vcXVhbnR1bS9hcnRpY2xlLzU1MDg4MzY2L3F1YW50dW0tdGVjaG5vbG9naWVzLXRha2Utb2Zm0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>Bizarre device uses 'blind quantum computing' to let you access quantum computers from home</t>
+          <t>Many-excitation removal of a transmon qubit using a single-junction quantum-circuit refrigerator and a two-tone ...</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>2024-06-14 13:31:21.553304</t>
+          <t>2024-06-14 14:00:59.912386</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMirQFodHRwczovL3d3dy5tc24uY29tL2VuLXVzL25ld3MvdGVjaG5vbG9neS9iaXphcnJlLWRldmljZS11c2VzLWJsaW5kLXF1YW50dW0tY29tcHV0aW5nLXRvLWxldC15b3UtYWNjZXNzLXF1YW50dW0tY29tcHV0ZXJzLWZyb20taG9tZS9hci1CQjFtekNwNT9pdGVtPWZsaWdodHNwcmctdGlwc3Vic2MtdjFhL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiMmh0dHBzOi8vd3d3Lm5hdHVyZS5jb20vYXJ0aWNsZXMvczQxNTk4LTAyNC02NDQ5Ni010gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>New Dimensions in Quantum Computing: Majorana Particles Go 2D</t>
+          <t>A portable quantum simulator on a silicon chip</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>2024-06-14 13:31:21.553304</t>
+          <t>2024-06-14 14:00:59.912386</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiVmh0dHBzOi8vc2NpdGVjaGRhaWx5LmNvbS9uZXctZGltZW5zaW9ucy1pbi1xdWFudHVtLWNvbXB1dGluZy1tYWpvcmFuYS1wYXJ0aWNsZXMtZ28tMmQv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiY2h0dHBzOi8vd3d3Lm9wZW5hY2Nlc3Nnb3Zlcm5tZW50Lm9yZy9hcnRpY2xlL2EtcG9ydGFibGUtcXVhbnR1bS1zaW11bGF0b3Itb24tYS1zaWxpY29uLWNoaXAvMTc4MTYxL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>Soon, QDEL Screens Could Perfect What OLED Couldn't</t>
+          <t>Earth's rotation measured 1000x better with quantum entanglement</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>2024-06-14 13:31:21.553304</t>
+          <t>2024-06-14 14:00:59.912386</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiTGh0dHBzOi8vd3d3Lmhvd3RvZ2Vlay5jb20vc29vbi1xZGVsLXNjcmVlbnMtY291bGQtcGVyZmVjdC13aGF0LW9sZWQtY291bGRudC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiVmh0dHBzOi8vaW50ZXJlc3RpbmdlbmdpbmVlcmluZy5jb20vc2NpZW5jZS9xdWFudHVtLWVudGFuZ2xlbWVudC1tZWFzdXJlLWVhcnRoLXJvdGF0aW9u0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>D-Wave quantum director Emil Michael sells over $27 million in warrants</t>
+          <t>Daniel Oi</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>2024-06-14 13:31:21.553304</t>
+          <t>2024-06-14 14:00:59.916918</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMifWh0dHBzOi8vaW4uaW52ZXN0aW5nLmNvbS9uZXdzL2NvbXBhbnktbmV3cy9kd2F2ZS1xdWFudHVtLWRpcmVjdG9yLWVtaWwtbWljaGFlbC1zZWxscy1vdmVyLTI3LW1pbGxpb24taW4td2FycmFudHMtOTNDSC00MjU1MTI00gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiP2h0dHBzOi8vd3d3Lmxhc2VyZm9jdXN3b3JsZC5jb20vaG9tZS9jb250YWN0LzU1MDg4Mjk2L2RhbmllbC1vadIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>Femtosecond Lasers Spearhead the Quantum Computing Revolution</t>
+          <t>Lantronix Wins 2024 IoT Evolution Asset Tracking Award for FOX3 Telematic Gateway</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>2024-06-14 13:31:21.553304</t>
+          <t>2024-06-14 14:00:59.916918</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiV2h0dHBzOi8vc2NpdGVjaGRhaWx5LmNvbS9mZW10b3NlY29uZC1sYXNlcnMtc3BlYXJoZWFkLXRoZS1xdWFudHVtLWNvbXB1dGluZy1yZXZvbHV0aW9uL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMinAFodHRwczovL3d3dy5nbG9iZW5ld3N3aXJlLmNvbS9lbi9uZXdzLXJlbGVhc2UvMjAyNC8wNi8xMy8yODk4MTQ0LzAvZW4vTGFudHJvbml4LVdpbnMtMjAyNC1Jb1QtRXZvbHV0aW9uLUFzc2V0LVRyYWNraW5nLUF3YXJkLWZvci1GT1gzLVRlbGVtYXRpYy1HYXRld2F5Lmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>‘It’s the perfect place’: London Underground hosts tests for ‘quantum compass’ that could replace GPS</t>
+          <t>D-Wave quantum director Emil Michael sells over $27 million in warrants</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>2024-06-15 13:31:21.538115</t>
+          <t>2024-06-14 14:00:59.916918</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMifWh0dHBzOi8vd3d3LnRoZWd1YXJkaWFuLmNvbS9zY2llbmNlL2FydGljbGUvMjAyNC9qdW4vMTUvbG9uZG9uLXVuZGVyZ3JvdW5kLXF1YW50dW0tY29tcGFzcy1ncHMtc3ViYXRvbWljLWluc3RydW1lbnQtbG9jYXRpb25z0gF9aHR0cHM6Ly9hbXAudGhlZ3VhcmRpYW4uY29tL3NjaWVuY2UvYXJ0aWNsZS8yMDI0L2p1bi8xNS9sb25kb24tdW5kZXJncm91bmQtcXVhbnR1bS1jb21wYXNzLWdwcy1zdWJhdG9taWMtaW5zdHJ1bWVudC1sb2NhdGlvbnM?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMifWh0dHBzOi8vaW4uaW52ZXN0aW5nLmNvbS9uZXdzL2NvbXBhbnktbmV3cy9kd2F2ZS1xdWFudHVtLWRpcmVjdG9yLWVtaWwtbWljaGFlbC1zZWxscy1vdmVyLTI3LW1pbGxpb24taW4td2FycmFudHMtOTNDSC00MjU1MTI00gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>Panama and Canada's First Quantum agree details for copper mine contract</t>
+          <t>Financial regulators need a ‘quantum’ leap</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>2024-06-15 13:31:21.538115</t>
+          <t>2024-06-14 14:00:59.916918</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiWmh0dHBzOi8vY2EubW92aWVzLnlhaG9vLmNvbS9maW5hbmNlL25ld3MvcGFuYW1hLWNhbmFkYXMtZmlyc3QtcXVhbnR1bS1hZ3JlZS0xNTI2MTgxNzQuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMieWh0dHBzOi8vd3d3Lm1zbi5jb20vZW4taW4vbW9uZXkvdG9wc3Rvcmllcy9maW5hbmNpYWwtcmVndWxhdG9ycy1uZWVkLWEtcXVhbnR1bS1sZWFwL2FyLUJCMW9nNHhPP29jaWQ9ZmluYW5jZS12ZXJ0aHAtZmVlZHPSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>Zero Point Cryogenics Secures $2.67 Million (CAD) in Funding to Fuel Growth</t>
+          <t>Advancements in Quantum Computing and Their Influence on</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>2024-06-15 13:31:21.543127</t>
+          <t>2024-06-14 14:00:59.916918</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMicmh0dHBzOi8vdGhlcXVhbnR1bWluc2lkZXIuY29tLzIwMjQvMDYvMTUvemVyby1wb2ludC1jcnlvZ2VuaWNzLXNlY3VyZXMtMi02Ny1taWxsaW9uLWNhZC1pbi1mdW5kaW5nLXRvLWZ1ZWwtZ3Jvd3RoL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiXGh0dHBzOi8vd3d3Lm9wZW5wci5jb20vbmV3cy8zNTM5NjkyL2FkdmFuY2VtZW50cy1pbi1xdWFudHVtLWNvbXB1dGluZy1hbmQtdGhlaXItaW5mbHVlbmNlLW9u0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>Huge fault-tolerant quantum computers on the agenda at Commercialising Quantum 2024 conference – Physics World</t>
+          <t>Government plans to work with TCS, HCL and other IT giants for quantum technology</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>2024-06-15 13:31:21.543127</t>
+          <t>2024-06-14 14:00:59.916918</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiemh0dHBzOi8vcGh5c2ljc3dvcmxkLmNvbS9hL2h1Z2UtZmF1bHQtdG9sZXJhbnQtcXVhbnR1bS1jb21wdXRlcnMtb24tdGhlLWFnZW5kYS1hdC1jb21tZXJjaWFsaXNpbmctcXVhbnR1bS0yMDI0LWNvbmZlcmVuY2Uv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiowFodHRwczovL3RpbWVzb2ZpbmRpYS5pbmRpYXRpbWVzLmNvbS90ZWNobm9sb2d5L3RlY2gtbmV3cy9nb3Zlcm5tZW50LXBsYW5zLXRvLXdvcmstd2l0aC10Y3MtaGNsLWFuZC1vdGhlci1pdC1naWFudHMtZm9yLXF1YW50dW0tdGVjaG5vbG9neS9hcnRpY2xlc2hvdy8xMTEwMDMwNDEuY21z0gGnAWh0dHBzOi8vdGltZXNvZmluZGlhLmluZGlhdGltZXMuY29tL3RlY2hub2xvZ3kvdGVjaC1uZXdzL2dvdmVybm1lbnQtcGxhbnMtdG8td29yay13aXRoLXRjcy1oY2wtYW5kLW90aGVyLWl0LWdpYW50cy1mb3ItcXVhbnR1bS10ZWNobm9sb2d5L2FtcF9hcnRpY2xlc2hvdy8xMTEwMDMwNDEuY21z?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>Anyon quantum dimensions from an arbitrary ground state wave function</t>
+          <t>African traditional spirituality parallels quantum physics: Implications development</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>2024-06-15 13:31:21.543127</t>
+          <t>2024-06-14 14:00:59.916918</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiMmh0dHBzOi8vd3d3Lm5hdHVyZS5jb20vYXJ0aWNsZXMvczQxNDY3LTAyNC00Nzg1Ni030gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiiwFodHRwczovL3d3dy5naGFuYXdlYi5jb20vR2hhbmFIb21lUGFnZS9mZWF0dXJlcy9BZnJpY2FuLXRyYWRpdGlvbmFsLXNwaXJpdHVhbGl0eS1wYXJhbGxlbHMtcXVhbnR1bS1waHlzaWNzLUltcGxpY2F0aW9ucy1kZXZlbG9wbWVudC0xOTM1NjM50gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>Guest Post -- The Road to the Proclamation of IYQ2025</t>
+          <t>Indian Government To Collaborate With IT Giants For Quantum Technology Development</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>2024-06-15 13:31:21.545640</t>
+          <t>2024-06-14 14:00:59.916918</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiXGh0dHBzOi8vdGhlcXVhbnR1bWluc2lkZXIuY29tLzIwMjQvMDYvMTUvZ3Vlc3QtcG9zdC10aGUtcm9hZC10by10aGUtcHJvY2xhbWF0aW9uLW9mLWl5cTIwMjUv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMilAFodHRwczovL3d3dy50aW1lc25vd25ld3MuY29tL3RlY2hub2xvZ3ktc2NpZW5jZS9pbmRpYW4tZ292ZXJubWVudC10by1jb2xsYWJvcmF0ZS13aXRoLWl0LWdpYW50cy1mb3ItcXVhbnR1bS10ZWNobm9sb2d5LWRldmVsb3BtZW50LWFydGljbGUtMTExMDAzNzkz0gGYAWh0dHBzOi8vd3d3LnRpbWVzbm93bmV3cy5jb20vdGVjaG5vbG9neS1zY2llbmNlL2luZGlhbi1nb3Zlcm5tZW50LXRvLWNvbGxhYm9yYXRlLXdpdGgtaXQtZ2lhbnRzLWZvci1xdWFudHVtLXRlY2hub2xvZ3ktZGV2ZWxvcG1lbnQtYXJ0aWNsZS0xMTEwMDM3OTMvYW1w?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>Superposition Guy's Podcast -- Dominik Ulmer, Chief Quantum Solutions officer at ParTec The Superposition Guy's ...</t>
+          <t>Bizarre device uses 'blind quantum computing' to let you access quantum computers from home</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>2024-06-15 13:31:21.545640</t>
+          <t>2024-06-14 14:00:59.916918</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMifGh0dHBzOi8vdGhlcXVhbnR1bWluc2lkZXIuY29tLzIwMjQvMDYvMTUvc3VwZXJwb3NpdGlvbi1ndXlzLXBvZGNhc3QtZG9taW5pay11bG1lci1jaGllZi1xdWFudHVtLXNvbHV0aW9ucy1vZmZpY2VyLWF0LXBhcnRlYy_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMirQFodHRwczovL3d3dy5tc24uY29tL2VuLXVzL25ld3MvdGVjaG5vbG9neS9iaXphcnJlLWRldmljZS11c2VzLWJsaW5kLXF1YW50dW0tY29tcHV0aW5nLXRvLWxldC15b3UtYWNjZXNzLXF1YW50dW0tY29tcHV0ZXJzLWZyb20taG9tZS9hci1CQjFtekNwNT9pdGVtPWZsaWdodHNwcmctdGlwc3Vic2MtdjFhL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>Nonlocal correlations transmitted between quantum dots via short topological superconductor | Scientific Reports</t>
+          <t>Fraunhofer, EV team for 300mm 3D quantum chip ...</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>2024-06-15 13:31:21.545640</t>
+          <t>2024-06-14 14:00:59.916918</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiMmh0dHBzOi8vd3d3Lm5hdHVyZS5jb20vYXJ0aWNsZXMvczQxNTk4LTAyNC02NDU3OC000gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiTWh0dHBzOi8vd3d3LmVlbmV3c2V1cm9wZS5jb20vZW4vZnJhdW5ob2Zlci1ldi10ZWFtLWZvci0zMDBtbS0zZC1xdWFudHVtLWNoaXAv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>What Is a Quantum Battery? And When Will It Power My Laptop?</t>
+          <t>Best Internet Providers in Seattle, Washington</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>2024-06-15 13:31:21.545640</t>
+          <t>2024-06-14 14:00:59.916918</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiVWh0dHBzOi8vZ2l6bW9kby5jb20vd2hhdC1pcy1hLXF1YW50dW0tYmF0dGVyeS1hbmQtd2hlbi13aWxsLWl0LXBvd2VyLW15LWxhLTE4NTE1MjIwNjLSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiSWh0dHBzOi8vd3d3LmNuZXQuY29tL2hvbWUvaW50ZXJuZXQvYmVzdC1pbnRlcm5ldC1wcm92aWRlcnMtaW4tc2VhdHRsZS13YS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>What if a nonmagnetic material could be magnetic?</t>
+          <t>Femtosecond Lasers Spearhead the Quantum Computing Revolution</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>2024-06-15 13:31:21.548290</t>
+          <t>2024-06-14 14:00:59.916918</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiMGh0dHBzOi8vd3d3LmV1cmVrYWxlcnQub3JnL25ld3MtcmVsZWFzZXMvMTA0ODM1MtIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiV2h0dHBzOi8vc2NpdGVjaGRhaWx5LmNvbS9mZW10b3NlY29uZC1sYXNlcnMtc3BlYXJoZWFkLXRoZS1xdWFudHVtLWNvbXB1dGluZy1yZXZvbHV0aW9uL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>An Improved Method for Quantum Matrix Multiplication: Main Procedure</t>
+          <t>Soon, QDEL Screens Could Perfect What OLED Couldn't</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>2024-06-15 13:31:21.548290</t>
+          <t>2024-06-14 14:00:59.916918</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiWmh0dHBzOi8vaGFja2Vybm9vbi5jb20vYW4taW1wcm92ZWQtbWV0aG9kLWZvci1xdWFudHVtLW1hdHJpeC1tdWx0aXBsaWNhdGlvbi1tYWluLXByb2NlZHVyZdIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiTGh0dHBzOi8vd3d3Lmhvd3RvZ2Vlay5jb20vc29vbi1xZGVsLXNjcmVlbnMtY291bGQtcGVyZmVjdC13aGF0LW9sZWQtY291bGRudC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>Everyone Missed 1 Detail In The MCU's Most Recent Movie, But I Can't Wait To See What It Means</t>
+          <t>When quantum dots meet blue phase liquid crystal elastomers: visualized full-color and mechanically-switchable ...</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>2024-06-15 13:31:21.548290</t>
+          <t>2024-06-14 14:00:59.916918</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiTWh0dHBzOi8vc2NyZWVucmFudC5jb20vdGhlLW1hcnZlbHMtbWlzc2VkLWRldGFpbC1xdWFudHVtLWJhbmRzLW1hcmlhLXJhbWJlYXUv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiMmh0dHBzOi8vd3d3Lm5hdHVyZS5jb20vYXJ0aWNsZXMvczQxMzc3LTAyNC0wMTQ3OS0x0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>Quantum entanglement measures Earth's spin with never-before-seen accuracy</t>
+          <t>First topological quantum simulator device in strong light-matter interaction regime to operate at room temperatures</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>2024-06-15 13:31:21.553304</t>
+          <t>2024-06-14 14:00:59.916918</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMingFodHRwczovL3d3dy5tc24uY29tL2VuLXVzL25ld3MvdGVjaG5vbG9neS9xdWFudHVtLWVudGFuZ2xlbWVudC1tZWFzdXJlcy1lYXJ0aC1zLXNwaW4td2l0aC1uZXZlci1iZWZvcmUtc2Vlbi1hY2N1cmFjeS9hci1CQjFvZjZWZj9pdGVtPWZsaWdodHNwcmctdGlwc3Vic2MtdjFhL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMi0wFodHRwczovL3d3dy5tc24uY29tL2VuLXVzL25ld3MvdGVjaG5vbG9neS9maXJzdC10b3BvbG9naWNhbC1xdWFudHVtLXNpbXVsYXRvci1kZXZpY2UtaW4tc3Ryb25nLWxpZ2h0LW1hdHRlci1pbnRlcmFjdGlvbi1yZWdpbWUtdG8tb3BlcmF0ZS1hdC1yb29tLXRlbXBlcmF0dXJlcy9hci1CQjFtWm5pYT9pdGVtPWZsaWdodHNwcmctdGlwc3Vic2MtdjFhP3NlYXNvbj0yMDI00gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>Quantum Encryption &amp; the Rise of Cybersecuritys Superhero ‍♂️ | Tech News with Comed-AI-n</t>
+          <t>‘Escape From Shadow Physics’ Review: Quantum Weirdness</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>2024-06-15 13:31:21.553304</t>
+          <t>2024-06-14 14:00:59.916918</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMirwFodHRwczovL21lZGl1bS5jb20vQENvbWVkX0FJX24vcXVhbnR1bS1lbmNyeXB0aW9uLXRoZS1yaXNlLW9mLWN5YmVyc2VjdXJpdHlzLXN1cGVyaGVyby0lRUYlQjglOEYtdGVjaC1uZXdzLXdpdGgtY29tZWQtYWktbi01ZTUxODc1YzRmYzA_cmVzcG9uc2VzT3Blbj10cnVlJnNvcnRCeT1SRVZFUlNFX0NIUk9O0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiaWh0dHBzOi8vd3d3Lm1zbi5jb20vZW4tdXMvbmV3cy90ZWNobm9sb2d5L2VzY2FwZS1mcm9tLXNoYWRvdy1waHlzaWNzLXJldmlldy1xdWFudHVtLXdlaXJkbmVzcy9hci1CQjFvZU5wUNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>Gemma Arterton Says She Gets 'Criticism' for Quantum of Solace : There's 'So Much Wrong with Bond Women'</t>
+          <t>High-tech highway: US 36 corridor emerging as hotspot for quantum, aerospace, biotech – BizWest</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>2024-06-15 14:31:21.548290</t>
+          <t>2024-06-14 14:00:59.916918</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiR2h0dHBzOi8vdWsubW92aWVzLnlhaG9vLmNvbS9nZW1tYS1hcnRlcnRvbi1zYXlzLXNoZS1nZXRzLTE2MTkzMDYzNy5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMicmh0dHBzOi8vYml6d2VzdC5jb20vMjAyNC8wNi8xNC9oaWdoLXRlY2gtaGlnaHdheS11cy0zNi1jb3JyaWRvci1lbWVyZ2luZy1hcy1ob3RzcG90LWZvci1xdWFudHVtLWFlcm9zcGFjZS1iaW90ZWNoL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>IBM and Japan institute team up to develop next-gen quantum computer</t>
+          <t>Quantum Defies Fossil Fuel Flight with $5.8B Target</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>2024-06-15 14:31:21.548290</t>
+          <t>2024-06-14 14:00:59.916918</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMicGh0dHBzOi8vYXNpYS5uaWtrZWkuY29tL0J1c2luZXNzL1RlY2hub2xvZ3kvSUJNLWFuZC1KYXBhbi1pbnN0aXR1dGUtdGVhbS11cC10by1kZXZlbG9wLW5leHQtZ2VuLXF1YW50dW0tY29tcHV0ZXLSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiYGh0dHBzOi8vd3d3LnRoZW1pZGRsZW1hcmtldC5jb20vbmV3cy1hbmFseXNpcy9xdWFudHVtLWRlZmllcy1mb3NzaWwtZnVlbC1mbGlnaHQtd2l0aC01LThiLXRhcmdldNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>Quantum Technology Flourishes in India with 40 New Startups in Two Years</t>
+          <t>New Dimensions in Quantum Computing: Majorana Particles Go 2D</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>2024-06-15 14:31:21.553304</t>
+          <t>2024-06-14 14:00:59.916918</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiZWh0dHBzOi8vd3d3LnRlY2hpZXhwZXJ0LmNvbS9xdWFudHVtLXRlY2hub2xvZ3ktZmxvdXJpc2hlcy1pbi1pbmRpYS13aXRoLTQwLW5ldy1zdGFydHVwcy1pbi10d28teWVhcnMv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiVmh0dHBzOi8vc2NpdGVjaGRhaWx5LmNvbS9uZXctZGltZW5zaW9ucy1pbi1xdWFudHVtLWNvbXB1dGluZy1tYWpvcmFuYS1wYXJ0aWNsZXMtZ28tMmQv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>"Spooky action at a distance" confirmed in heaviest particles</t>
+          <t>Indian Govt Mulls Working With TCS, HCL and Tech Mahindra to Develop Quantum Tech Software Under Rs 6000 ...</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>2024-06-15 20:31:21.545640</t>
+          <t>2024-06-14 14:00:59.922033</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiaGh0dHBzOi8vd3d3LmVhcnRoLmNvbS9uZXdzL3F1YW50dW0tZW50YW5nbGVtZW50LXNwb29reS1hY3Rpb24tYXQtYS1kaXN0YW5jZS1wZXJzaXN0cy1iZXR3ZWVuLXRvcC1xdWFya3Mv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiTmh0dHBzOi8vd3d3LmluZGlhbndlYjIuY29tLzIwMjQvMDYvaW5kaWFuLWdvdnQtbXVsbHMtd29ya2luZy13aXRoLXRjcy1oY2wuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>Development of optimization method for truss structure by quantum annealing | Scientific Reports</t>
+          <t>דף בית | Emirates News Agency</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>2024-06-15 23:31:21.538115</t>
+          <t>2024-06-14 14:00:59.922033</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiMmh0dHBzOi8vd3d3Lm5hdHVyZS5jb20vYXJ0aWNsZXMvczQxNTk4LTAyNC02NDU4OC0y0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiTmh0dHBzOi8vd3d3LndhbS5hZS9lbi9hcnRpY2xlL2IzbGZ5eW0tc29yYm9ubmUtdW5pdmVyc2l0eS1hYnUtZGhhYmktdGVjaG5vbG9nedIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>Record 99.9% quantum computing accuracy achieved on existing silicon chips</t>
+          <t>Tech3 | Navi's UPI payments surge 10x in 2 months; IT majors to join govt's quantum mission; and more</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>2024-06-16 00:31:21.545640</t>
+          <t>2024-06-14 14:00:59.922033</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMitgFodHRwczovL3d3dy5tc24uY29tL2VuLXVzL25ld3MvdGVjaG5vbG9neS9yZWNvcmQtOTktOS1xdWFudHVtLWNvbXB1dGluZy1hY2N1cmFjeS1hY2hpZXZlZC1vbi1leGlzdGluZy1zaWxpY29uLWNoaXBzL2FyLUJCMW9oN0VVP2l0ZW09dGhlbWVkX2ZlYXR1cmVkYXBwc19lbmFibGVEP2xvYWRJbj1kZWZhdWx0QnJvd3NlctIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiqwFodHRwczovL3d3dy5tb25leWNvbnRyb2wuY29tL25ld3MvdGVjaG5vbG9neS1zdGFydHVwL25ld3NsZXR0ZXJzL01DVGVjaDMvdGVjaDMtbmF2aS1zLXVwaS1wYXltZW50cy1zdXJnZS0xMHgtaW4tMi1tb250aHMtaXQtbWFqb3JzLXRvLWpvaW4tZ292dC1zLXF1YW50dW0tbWlzc2lvbi1hbmQtbW9yZS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>Jitendra Singh says over 40 quantum technology startups emerged in two years</t>
+          <t>Ripple Issues Urgent Warning on Quantum Computing's Threat to Blockchain Security</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>2024-06-16 00:31:21.548290</t>
+          <t>2024-06-14 14:00:59.922033</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMijwFodHRwczovL3d3dy50aGVoaW5kdWJ1c2luZXNzbGluZS5jb20vaW5mby10ZWNoL2ppdGVuZHJhLXNpbmdoLXNheXMtb3Zlci00MC1xdWFudHVtLXRlY2hub2xvZ3ktc3RhcnR1cHMtZW1lcmdlZC1pbi10d28teWVhcnMvYXJ0aWNsZTY4Mjk2MDI3LmVjZdIBlAFodHRwczovL3d3dy50aGVoaW5kdWJ1c2luZXNzbGluZS5jb20vaW5mby10ZWNoL2ppdGVuZHJhLXNpbmdoLXNheXMtb3Zlci00MC1xdWFudHVtLXRlY2hub2xvZ3ktc3RhcnR1cHMtZW1lcmdlZC1pbi10d28teWVhcnMvYXJ0aWNsZTY4Mjk2MDI3LmVjZS9hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMifWh0dHBzOi8vd3d3LmJpZ25ld3NuZXR3b3JrLmNvbS9uZXdzLzI3NDQxMDI2OS9yaXBwbGUtaXNzdWVzLXVyZ2VudC13YXJuaW5nLW9uLXF1YW50dW0tY29tcHV0aW5nLXRocmVhdC10by1ibG9ja2NoYWluLXNlY3VyaXR50gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>Quantum entangled photons used to measure the Earth's rotation</t>
+          <t>52 Super Series : Back to reality for Quantum, the dream continues for Vayu</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>2024-06-16 01:31:21.538115</t>
+          <t>2024-06-14 14:00:59.922033</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiV2h0dHBzOi8vd3d3LmVhcnRoLmNvbS9uZXdzL3F1YW50dW0tZW50YW5nbGVtZW50LXBob3RvbnMtdXNlZC10by1tZWFzdXJlLWVhcnRoLXJvdGF0aW9uL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiXmh0dHBzOi8vbmF1dGljYS5uZXdzLzUyLXN1cGVyLXNlcmllcy1iYWNrLXRvLXJlYWxpdHktZm9yLXF1YW50dW0tdGhlLWRyZWFtLWNvbnRpbnVlcy1mb3ItdmF5dS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
+          <t>Govt to work with TCS, HCL, others for Rs 6,000 crore quantum tech scheme</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>2024-06-14 14:00:59.922033</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMif2h0dHBzOi8vd3d3Lm1vbmV5Y29udHJvbC5jb20vdGVjaG5vbG9neS9nb3Z0LXRvLXdvcmstd2l0aC1pdC1tYWpvcnMtZm9yLXJzLTYwMDAtY3JvcmUtcXVhbnR1bS10ZWNoLXNjaGVtZS1hcnRpY2xlLTEyNzQ4NjEzLmh0bWzSAYMBaHR0cHM6Ly93d3cubW9uZXljb250cm9sLmNvbS90ZWNobm9sb2d5L2dvdnQtdG8td29yay13aXRoLWl0LW1ham9ycy1mb3ItcnMtNjAwMC1jcm9yZS1xdWFudHVtLXRlY2gtc2NoZW1lLWFydGljbGUtMTI3NDg2MTMuaHRtbC9hbXA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>TCS, HCLTech and Others Join Govt's INR 6000 Crore Quantum Tech Project – AIM</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>2024-06-14 14:00:59.922033</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiZGh0dHBzOi8vYW5hbHl0aWNzaW5kaWFtYWcuY29tL3Rjcy1oY2x0ZWNoLWFuZC1vdGhlcnMtam9pbi1nb3Z0cy1pbnItNjAwMC1jcm9yZS1xdWFudHVtLXRlY2gtcHJvamVjdC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>Former Quantum House CEO Robi Jurney to serve as Palm Beach Chamber's new board chair</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>2024-06-14 14:00:59.922033</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiQGh0dHBzOi8vd3d3LmFvbC5jb20vZm9ybWVyLXF1YW50dW0taG91c2UtY2VvLXJvYmktMDkwMjI0MTg3Lmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>Data Loading into Quantum: The Gateway to Quantum Computing Power</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>2024-06-14 14:00:59.922033</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiWWh0dHBzOi8vdGVjaGJ1bGxpb24uY29tL2RhdGEtbG9hZGluZy1pbnRvLXF1YW50dW0tdGhlLWdhdGV3YXktdG8tcXVhbnR1bS1jb21wdXRpbmctcG93ZXIv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>Govt to work with IT majors for Rs 6,000 crore quantum tech scheme</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>2024-06-14 14:00:59.922033</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMieWh0dHBzOi8vd3d3Lm1zbi5jb20vZW4taW4vbW9uZXkvdG9wc3Rvcmllcy9nb3Z0LXRvLXdvcmstd2l0aC1pdC1tYWpvcnMtZm9yLXJzLTYtMDAwLWNyb3JlLXF1YW50dW0tdGVjaC1zY2hlbWUvYXItQkIxb2NVVG3SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>Investing in the Future: 3 Top Quantum Computing Stocks for Growth</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>2024-06-14 14:00:59.924036</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiYGh0dHBzOi8vd3d3LmZlYXR1cmV3ZWVrbHkuY29tL2ludmVzdGluZy1pbi10aGUtZnV0dXJlLTMtdG9wLXF1YW50dW0tY29tcHV0aW5nLXN0b2Nrcy1mb3ItZ3Jvd3RoL9IBZGh0dHBzOi8vd3d3LmZlYXR1cmV3ZWVrbHkuY29tL2ludmVzdGluZy1pbi10aGUtZnV0dXJlLTMtdG9wLXF1YW50dW0tY29tcHV0aW5nLXN0b2Nrcy1mb3ItZ3Jvd3RoL2FtcC8?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>Fresh Insights On D-Wave Quantum Inc (QBTS)</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>2024-06-14 14:00:59.924036</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiVGh0dHBzOi8vd3d3LnN0b2Nrc3JlZ2lzdGVyLmNvbS8yMDI0LzA2LzE0L2ZyZXNoLWluc2lnaHRzLW9uLWQtd2F2ZS1xdWFudHVtLWluYy1xYnRzL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>Guest Post — The Road to the Proclamation of IYQ2025</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>2024-06-15 14:00:59.912386</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiXGh0dHBzOi8vdGhlcXVhbnR1bWluc2lkZXIuY29tLzIwMjQvMDYvMTUvZ3Vlc3QtcG9zdC10aGUtcm9hZC10by10aGUtcHJvY2xhbWF0aW9uLW9mLWl5cTIwMjUv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>Earth's rotation is measured using quantum entanglement | Globe Echo</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>2024-06-15 14:00:59.924683</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiTWh0dHBzOi8vZ2xvYmVlY2hvLmNvbS9lYXJ0aHMtcm90YXRpb24taXMtbWVhc3VyZWQtdXNpbmctcXVhbnR1bS1lbnRhbmdsZW1lbnQv0gFRaHR0cHM6Ly9nbG9iZWVjaG8uY29tL2VhcnRocy1yb3RhdGlvbi1pcy1tZWFzdXJlZC11c2luZy1xdWFudHVtLWVudGFuZ2xlbWVudC9hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>What if a nonmagnetic material could be magnetic?</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>2024-06-15 14:05:28.341672</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiMGh0dHBzOi8vd3d3LmV1cmVrYWxlcnQub3JnL25ld3MtcmVsZWFzZXMvMTA0ODM1MtIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>Anyon quantum dimensions from an arbitrary ground state wave function</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>2024-06-15 14:05:28.341672</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiMmh0dHBzOi8vd3d3Lm5hdHVyZS5jb20vYXJ0aWNsZXMvczQxNDY3LTAyNC00Nzg1Ni030gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>Superposition Guy's Podcast -- Dominik Ulmer, Chief Quantum Solutions officer at ParTec The Superposition Guy's ...</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>2024-06-15 14:05:28.341672</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMifGh0dHBzOi8vdGhlcXVhbnR1bWluc2lkZXIuY29tLzIwMjQvMDYvMTUvc3VwZXJwb3NpdGlvbi1ndXlzLXBvZGNhc3QtZG9taW5pay11bG1lci1jaGllZi1xdWFudHVtLXNvbHV0aW9ucy1vZmZpY2VyLWF0LXBhcnRlYy_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>Quantum entangled photons react to Earth's spin</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>2024-06-15 14:05:28.341672</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMieWh0dHBzOi8vd3d3Lm1zbi5jb20vZW4tdXMvbmV3cy90ZWNobm9sb2d5L3F1YW50dW0tZW50YW5nbGVkLXBob3RvbnMtcmVhY3QtdG8tZWFydGgtcy1zcGluL2FyLUJCMW9mMmpqP29jaWQ9QmluZ05ld3NTZWFyY2jSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>Gemma Arterton Says She Gets 'Criticism' for Quantum of Solace : There's 'So Much Wrong with Bond Women'</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>2024-06-15 14:05:28.341672</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiR2h0dHBzOi8vdWsubW92aWVzLnlhaG9vLmNvbS9nZW1tYS1hcnRlcnRvbi1zYXlzLXNoZS1nZXRzLTE2MTkzMDYzNy5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>Guest Post -- The Road to the Proclamation of IYQ2025</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>2024-06-15 14:05:28.341672</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiXGh0dHBzOi8vdGhlcXVhbnR1bWluc2lkZXIuY29tLzIwMjQvMDYvMTUvZ3Vlc3QtcG9zdC10aGUtcm9hZC10by10aGUtcHJvY2xhbWF0aW9uLW9mLWl5cTIwMjUv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>An Improved Method for Quantum Matrix Multiplication: Main Procedure</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>2024-06-15 14:05:28.341672</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiWmh0dHBzOi8vaGFja2Vybm9vbi5jb20vYW4taW1wcm92ZWQtbWV0aG9kLWZvci1xdWFudHVtLW1hdHJpeC1tdWx0aXBsaWNhdGlvbi1tYWluLXByb2NlZHVyZdIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>Everyone Missed 1 Detail In The MCU's Most Recent Movie, But I Can't Wait To See What It Means</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>2024-06-15 14:05:28.341672</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiTWh0dHBzOi8vc2NyZWVucmFudC5jb20vdGhlLW1hcnZlbHMtbWlzc2VkLWRldGFpbC1xdWFudHVtLWJhbmRzLW1hcmlhLXJhbWJlYXUv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>Quantum entanglement measures Earth's spin with never-before-seen accuracy</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>2024-06-15 14:05:28.341672</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMingFodHRwczovL3d3dy5tc24uY29tL2VuLXVzL25ld3MvdGVjaG5vbG9neS9xdWFudHVtLWVudGFuZ2xlbWVudC1tZWFzdXJlcy1lYXJ0aC1zLXNwaW4td2l0aC1uZXZlci1iZWZvcmUtc2Vlbi1hY2N1cmFjeS9hci1CQjFvZjZWZj9pdGVtPWZsaWdodHNwcmctdGlwc3Vic2MtdjFhL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>Nonlocal correlations transmitted between quantum dots via short topological superconductor | Scientific Reports</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>2024-06-15 14:05:28.341672</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiMmh0dHBzOi8vd3d3Lm5hdHVyZS5jb20vYXJ0aWNsZXMvczQxNTk4LTAyNC02NDU3OC000gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>What Is a Quantum Battery? And When Will It Power My Laptop?</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>2024-06-15 14:05:28.341672</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiVWh0dHBzOi8vZ2l6bW9kby5jb20vd2hhdC1pcy1hLXF1YW50dW0tYmF0dGVyeS1hbmQtd2hlbi13aWxsLWl0LXBvd2VyLW15LWxhLTE4NTE1MjIwNjLSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>Huge fault-tolerant quantum computers on the agenda at Commercialising Quantum 2024 conference – Physics World</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>2024-06-15 14:05:28.341672</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiemh0dHBzOi8vcGh5c2ljc3dvcmxkLmNvbS9hL2h1Z2UtZmF1bHQtdG9sZXJhbnQtcXVhbnR1bS1jb21wdXRlcnMtb24tdGhlLWFnZW5kYS1hdC1jb21tZXJjaWFsaXNpbmctcXVhbnR1bS0yMDI0LWNvbmZlcmVuY2Uv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>A liquid crystal source of photon pairs</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>2024-06-15 14:05:28.341672</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiMGh0dHBzOi8vd3d3LmV1cmVrYWxlcnQub3JnL25ld3MtcmVsZWFzZXMvMTA0ODMwMtIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>Quantum Encryption &amp; the Rise of Cybersecuritys Superhero ‍♂️ | Tech News with Comed-AI-n</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>2024-06-15 14:05:28.341672</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMirwFodHRwczovL21lZGl1bS5jb20vQENvbWVkX0FJX24vcXVhbnR1bS1lbmNyeXB0aW9uLXRoZS1yaXNlLW9mLWN5YmVyc2VjdXJpdHlzLXN1cGVyaGVyby0lRUYlQjglOEYtdGVjaC1uZXdzLXdpdGgtY29tZWQtYWktbi01ZTUxODc1YzRmYzA_cmVzcG9uc2VzT3Blbj10cnVlJnNvcnRCeT1SRVZFUlNFX0NIUk9O0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>Purified Silicon Makes Bigger, Faster Quantum Computers</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>2024-06-15 14:05:28.341672</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiP2h0dHBzOi8vc3BlY3RydW0uaWVlZS5vcmcvc2lsaWNvbi1xdWFudHVtLWNvbXB1dGluZy1wdXJpZmllZC1zadIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>‘It’s the perfect place’: London Underground hosts tests for ‘quantum compass’ that could replace GPS</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>2024-06-15 14:05:28.341672</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMifWh0dHBzOi8vd3d3LnRoZWd1YXJkaWFuLmNvbS9zY2llbmNlL2FydGljbGUvMjAyNC9qdW4vMTUvbG9uZG9uLXVuZGVyZ3JvdW5kLXF1YW50dW0tY29tcGFzcy1ncHMtc3ViYXRvbWljLWluc3RydW1lbnQtbG9jYXRpb25z0gF9aHR0cHM6Ly9hbXAudGhlZ3VhcmRpYW4uY29tL3NjaWVuY2UvYXJ0aWNsZS8yMDI0L2p1bi8xNS9sb25kb24tdW5kZXJncm91bmQtcXVhbnR1bS1jb21wYXNzLWdwcy1zdWJhdG9taWMtaW5zdHJ1bWVudC1sb2NhdGlvbnM?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>Panama and Canada's First Quantum agree details for copper mine contract</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>2024-06-15 14:05:28.341672</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiWmh0dHBzOi8vY2EubW92aWVzLnlhaG9vLmNvbS9maW5hbmNlL25ld3MvcGFuYW1hLWNhbmFkYXMtZmlyc3QtcXVhbnR1bS1hZ3JlZS0xNTI2MTgxNzQuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>Zero Point Cryogenics Secures $2.67 Million (CAD) in Funding to Fuel Growth</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>2024-06-15 14:05:28.341672</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMicmh0dHBzOi8vdGhlcXVhbnR1bWluc2lkZXIuY29tLzIwMjQvMDYvMTUvemVyby1wb2ludC1jcnlvZ2VuaWNzLXNlY3VyZXMtMi02Ny1taWxsaW9uLWNhZC1pbi1mdW5kaW5nLXRvLWZ1ZWwtZ3Jvd3RoL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>Other Quantum Startups in the U.K. | Globe Echo</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>2024-06-15 14:05:28.346308</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiOGh0dHBzOi8vZ2xvYmVlY2hvLmNvbS9vdGhlci1xdWFudHVtLXN0YXJ0dXBzLWluLXRoZS11LWsv0gE8aHR0cHM6Ly9nbG9iZWVjaG8uY29tL290aGVyLXF1YW50dW0tc3RhcnR1cHMtaW4tdGhlLXUtay9hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>European Telecom Industry at the Forefront of Quantum Technology Adoption</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>2024-06-15 14:05:28.346308</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiamh0dHBzOi8vd3d3Lml0c2VjdXJpdHluZXdzLmluZm8vZXVyb3BlYW4tdGVsZWNvbS1pbmR1c3RyeS1hdC10aGUtZm9yZWZyb250LW9mLXF1YW50dW0tdGVjaG5vbG9neS1hZG9wdGlvbi_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>From Uncommon White Powder to Quantum Innovation: Discovering Nearly Noiseless Qubits is a valuable resource for learning about quantum computing</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>2024-06-15 14:05:28.346308</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMigAFodHRwczovL2xpc3QyMy5jb20vMzgwMTU2NS1mcm9tLXVuY29tbW9uLXdoaXRlLXBvd2Rlci10by1xdWFudHVtLWlubm92YXRpb24tZGlzY292ZXJpbmctbmVhcmx5LW5vaXNlbGVzcy1xdWJpdHMtaXMtYS12YWx1YWJsZS1yL9IBhAFodHRwczovL2xpc3QyMy5jb20vMzgwMTU2NS1mcm9tLXVuY29tbW9uLXdoaXRlLXBvd2Rlci10by1xdWFudHVtLWlubm92YXRpb24tZGlzY292ZXJpbmctbmVhcmx5LW5vaXNlbGVzcy1xdWJpdHMtaXMtYS12YWx1YWJsZS1yL2FtcC8?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>Liquid crystal source of photon pairs opens path to new generation of quantum sources</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>2024-06-15 14:05:28.346308</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiqAFodHRwczovL3d3dy5tc24uY29tL2VuLXVzL25ld3MvdGVjaG5vbG9neS9saXF1aWQtY3J5c3RhbC1zb3VyY2Utb2YtcGhvdG9uLXBhaXJzLW9wZW5zLXBhdGgtdG8tbmV3LWdlbmVyYXRpb24tb2YtcXVhbnR1bS1zb3VyY2VzL2FyLUJCMW9hcDBrP2l0ZW09ZmxpZ2h0c3ByZy10aXBzdWJzYy12MWHSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>There's a way to lessen your chances of getting booted from an overbooked cruise: pay more</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>2024-06-15 14:05:28.346308</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiSmh0dHBzOi8vc2cubmV3cy55YWhvby5jb20vdGhlcmVzLXdheS1sZXNzZW4tY2hhbmNlcy1nZXR0aW5nLTEwMDAwMTkwMy5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>HDK questions ₹3.2 crore subsidy to chip manufacturer by Gujarat govt, then backtracks</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>2024-06-15 14:05:28.346308</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMisgFodHRwczovL3d3dy50aGVoaW5kdS5jb20vYnVzaW5lc3MvdW5pb24tbWluaXN0ZXItaGQta3VtYXJhc3dhbXktcmV0cmFjdHMtc3RhdGVtZW50LW9uLXNlbWljb25kdWN0b3ItdW5pdC1pbi1ndWphcmF0LWEtZGF5LWFmdGVyLXF1ZXN0aW9uaW5nLXF1YW50dW0tb2Ytc3Vic2lkeS9hcnRpY2xlNjgyOTI3NTUuZWNl0gG3AWh0dHBzOi8vd3d3LnRoZWhpbmR1LmNvbS9idXNpbmVzcy91bmlvbi1taW5pc3Rlci1oZC1rdW1hcmFzd2FteS1yZXRyYWN0cy1zdGF0ZW1lbnQtb24tc2VtaWNvbmR1Y3Rvci11bml0LWluLWd1amFyYXQtYS1kYXktYWZ0ZXItcXVlc3Rpb25pbmctcXVhbnR1bS1vZi1zdWJzaWR5L2FydGljbGU2ODI5Mjc1NS5lY2UvYW1wLw?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>India Produced 40 'Quantum' Startups In 2 Years, Few With Global Potential: Dr Jitendra</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>2024-06-15 14:05:28.346308</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMic2h0dHBzOi8vd3d3LmRhaWx5ZXhjZWxzaW9yLmNvbS9pbmRpYS1wcm9kdWNlZC00MC1xdWFudHVtLXN0YXJ0dXBzLWluLTIteWVhcnMtZmV3LXdpdGgtZ2xvYmFsLXBvdGVudGlhbC1kci1qaXRlbmRyYS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>Scientists Create Multi-Node Entanglement in Metropolitan Quantum Network</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>2024-06-15 14:05:28.346308</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiZWh0dHBzOi8vYW5hLmlyL2VuL25ld3MvNjIyMy9zY2llbnRpc3RzLWNyZWF0ZS1tdWx0aS1ub2RlLWVudGFuZ2xlbWVudC1pbi1tZXRyb3BvbGl0YW4tcXVhbnR1bS1uZXR3b3Jr0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>Quantum network (QSWAP), a Cutting-Edge Cross-Chain Swap Platform, to List on BitMart Exchange ...</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>2024-06-15 14:05:28.346308</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMinwFodHRwczovL21hcmtldHMuZmluYW5jaWFsY29udGVudC5jb20vc3RvY2tzL2FydGljbGUvYmluYXJ5LTIwMjQtNi0xNS1xdWFudHVtLW5ldHdvcmstcXN3YXAtYS1jdXR0aW5nLWVkZ2UtY3Jvc3MtY2hhaW4tc3dhcC1wbGF0Zm9ybS10by1saXN0LW9uLWJpdG1hcnQtZXhjaGFuZ2XSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>Modi 3.0 to team up with TCS, HCL and other IT giants – Know why</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>2024-06-15 14:05:28.346308</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMie2h0dHBzOi8vd3d3Lm1zbi5jb20vZW4taW4vbGlmZXN0eWxlL3JlbGF0aW9uc2hpcHMvbW9kaS0zLTAtdG8tdGVhbS11cC13aXRoLXRjcy1oY2wtYW5kLW90aGVyLWl0LWdpYW50cy1rbm93LXdoeS9hci1CQjFvZ1lFb9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>“India has produced over 40 Quantum Technology start-ups in 2 years, few of them with global potential,” says Dr ...</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>2024-06-15 14:05:28.346308</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiO2h0dHBzOi8vcGliLmdvdi5pbi9QcmVzc1JlbGVhc2VJZnJhbWVQYWdlLmFzcHg_UFJJRD0yMDI1NTY00gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>India Has Produced Over 40 Quantum Technology Start-Ups In Two Years: Union Minister Dr. Jitendra Singh |</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>2024-06-15 14:05:28.346308</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMimQFodHRwczovL3d3dy5qYWlzYWxtZXJuZXdzLmNvbS9uZXdzL25hdGlvbmFsL2luZGlhLWhhcy1wcm9kdWNlZC1vdmVyLTQwLXF1YW50dW0tdGVjaG5vbG9neS1zdGFydC11cHMtaW4tdHdvLXllYXJzLXVuaW9uLW1pbmlzdGVyLWRyLWppdGVuZHJhLXNpbmdoLTI0NDEyNS_SAZ0BaHR0cHM6Ly93d3cuamFpc2FsbWVybmV3cy5jb20vbmV3cy9uYXRpb25hbC9pbmRpYS1oYXMtcHJvZHVjZWQtb3Zlci00MC1xdWFudHVtLXRlY2hub2xvZ3ktc3RhcnQtdXBzLWluLXR3by15ZWFycy11bmlvbi1taW5pc3Rlci1kci1qaXRlbmRyYS1zaW5naC0yNDQxMjUvYW1wLw?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>Generating photon pairs from a liquid crystal source | Globe Echo</t>
+        </is>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>2024-06-15 14:05:28.346308</t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiS2h0dHBzOi8vZ2xvYmVlY2hvLmNvbS9nZW5lcmF0aW5nLXBob3Rvbi1wYWlycy1mcm9tLWEtbGlxdWlkLWNyeXN0YWwtc291cmNlL9IBT2h0dHBzOi8vZ2xvYmVlY2hvLmNvbS9nZW5lcmF0aW5nLXBob3Rvbi1wYWlycy1mcm9tLWEtbGlxdWlkLWNyeXN0YWwtc291cmNlL2FtcC8?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>IBM and Japan institute team up to develop next-gen quantum computer</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>2024-06-15 15:05:28.341672</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMicGh0dHBzOi8vYXNpYS5uaWtrZWkuY29tL0J1c2luZXNzL1RlY2hub2xvZ3kvSUJNLWFuZC1KYXBhbi1pbnN0aXR1dGUtdGVhbS11cC10by1kZXZlbG9wLW5leHQtZ2VuLXF1YW50dW0tY29tcHV0ZXLSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>Quantum Technology Flourishes in India with 40 New Startups in Two Years</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>2024-06-15 15:05:28.341672</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiZWh0dHBzOi8vd3d3LnRlY2hpZXhwZXJ0LmNvbS9xdWFudHVtLXRlY2hub2xvZ3ktZmxvdXJpc2hlcy1pbi1pbmRpYS13aXRoLTQwLW5ldy1zdGFydHVwcy1pbi10d28teWVhcnMv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>Quantum Block Share Chat (QBT)</t>
+        </is>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>2024-06-15 19:00:59.916918</t>
+        </is>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMidGh0dHBzOi8vd3d3LmxzZS5jby51ay9TaGFyZUNoYXQuaHRtbD9TaGFyZVRpY2tlcj1RQlQmc2hhcmU9UXVhbnR1bS1CbG9jayZ0aHJlYWQ9NjlCRjE3QTktQzM3MS00OTk5LUI0OTYtNjRGOTNGRTI4QkMy0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>Quantum Block Share Chat. Chat About QBT Shares - Stock Quote, Charts, Trade History, Share Chat, Financial Terms ...</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>2024-06-15 19:05:28.346308</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMidGh0dHBzOi8vd3d3LmxzZS5jby51ay9TaGFyZUNoYXQuaHRtbD9TaGFyZVRpY2tlcj1RQlQmc2hhcmU9UXVhbnR1bS1CbG9jayZ0aHJlYWQ9NjlCRjE3QTktQzM3MS00OTk5LUI0OTYtNjRGOTNGRTI4QkMy0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>India produced over 40 quantum technology startups in 2 years: Jitendra Singh</t>
+        </is>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>2024-06-15 20:05:28.346308</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMia2h0dHBzOi8vd3d3LmFwN2FtLmNvbS9lbi84MTY4NS9pbmRpYS1wcm9kdWNlZC1vdmVyLTQwLXF1YW50dW0tdGVjaG5vbG9neS1zdGFydHVwcy1pbi0yLXllYXJzLWppdGVuZHJhLXNpbmdo0gFvaHR0cHM6Ly93d3cuYXA3YW0uY29tL2VuL2FtcC84MTY4NS9pbmRpYS1wcm9kdWNlZC1vdmVyLTQwLXF1YW50dW0tdGVjaG5vbG9neS1zdGFydHVwcy1pbi0yLXllYXJzLWppdGVuZHJhLXNpbmdo?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>"Spooky action at a distance" confirmed to persist between top quarks</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>2024-06-15 21:00:59.912386</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiaGh0dHBzOi8vd3d3LmVhcnRoLmNvbS9uZXdzL3F1YW50dW0tZW50YW5nbGVtZW50LXNwb29reS1hY3Rpb24tYXQtYS1kaXN0YW5jZS1wZXJzaXN0cy1iZXR3ZWVuLXRvcC1xdWFya3Mv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>"Spooky action at a distance" confirmed in heaviest particles</t>
+        </is>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>2024-06-15 21:05:28.341672</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiaGh0dHBzOi8vd3d3LmVhcnRoLmNvbS9uZXdzL3F1YW50dW0tZW50YW5nbGVtZW50LXNwb29reS1hY3Rpb24tYXQtYS1kaXN0YW5jZS1wZXJzaXN0cy1iZXR3ZWVuLXRvcC1xdWFya3Mv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>Business News | India Produced over 40 Quantum Technology Startups in 2 Years: Jitendra Singh</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>2024-06-15 23:00:59.916918</t>
+        </is>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMijAFodHRwczovL3d3dy5sYXRlc3RseS5jb20vYWdlbmN5LW5ld3MvYnVzaW5lc3MtbmV3cy1pbmRpYS1wcm9kdWNlZC1vdmVyLTQwLXF1YW50dW0tdGVjaG5vbG9neS1zdGFydHVwcy1pbi0yLXllYXJzLWppdGVuZHJhLXNpbmdoLTYwNDExODQuaHRtbNIBkAFodHRwczovL3d3dy5sYXRlc3RseS5jb20vYWdlbmN5LW5ld3MvYnVzaW5lc3MtbmV3cy1pbmRpYS1wcm9kdWNlZC1vdmVyLTQwLXF1YW50dW0tdGVjaG5vbG9neS1zdGFydHVwcy1pbi0yLXllYXJzLWppdGVuZHJhLXNpbmdoLTYwNDExODQuaHRtbC9hbXA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>Development of optimization method for truss structure by quantum annealing | Scientific Reports</t>
+        </is>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>2024-06-15 23:05:28.341672</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiMmh0dHBzOi8vd3d3Lm5hdHVyZS5jb20vYXJ0aWNsZXMvczQxNTk4LTAyNC02NDU4OC0y0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>Jitendra Singh says over 40 quantum technology startups emerged in two years</t>
+        </is>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>2024-06-16 00:05:28.341672</t>
+        </is>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMijwFodHRwczovL3d3dy50aGVoaW5kdWJ1c2luZXNzbGluZS5jb20vaW5mby10ZWNoL2ppdGVuZHJhLXNpbmdoLXNheXMtb3Zlci00MC1xdWFudHVtLXRlY2hub2xvZ3ktc3RhcnR1cHMtZW1lcmdlZC1pbi10d28teWVhcnMvYXJ0aWNsZTY4Mjk2MDI3LmVjZdIBlAFodHRwczovL3d3dy50aGVoaW5kdWJ1c2luZXNzbGluZS5jb20vaW5mby10ZWNoL2ppdGVuZHJhLXNpbmdoLXNheXMtb3Zlci00MC1xdWFudHVtLXRlY2hub2xvZ3ktc3RhcnR1cHMtZW1lcmdlZC1pbi10d28teWVhcnMvYXJ0aWNsZTY4Mjk2MDI3LmVjZS9hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>Record 99.9% quantum computing accuracy achieved on existing silicon chips</t>
+        </is>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>2024-06-16 00:05:28.341672</t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMitgFodHRwczovL3d3dy5tc24uY29tL2VuLXVzL25ld3MvdGVjaG5vbG9neS9yZWNvcmQtOTktOS1xdWFudHVtLWNvbXB1dGluZy1hY2N1cmFjeS1hY2hpZXZlZC1vbi1leGlzdGluZy1zaWxpY29uLWNoaXBzL2FyLUJCMW9oN0VVP2l0ZW09dGhlbWVkX2ZlYXR1cmVkYXBwc19lbmFibGVEP2xvYWRJbj1kZWZhdWx0QnJvd3NlctIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>World News</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>2024-06-16 00:05:28.346308</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiogFodHRwczovL3d3dy5sYXRlc3RseS5jb20vYWdlbmN5LW5ld3Mvd29ybGQtbmV3cy1xdWFudHVtLWNvbXB1dGVycy1hcmUtbGlrZS1rYWxlaWRvc2NvcGVzLXdoeS11bnVzdWFsLW1ldGFwaG9ycy1oZWxwLWlsbHVzdHJhdGUtc2NpZW5jZS1hbmQtdGVjaG5vbG9neS02MDQxMjUwLmh0bWzSAaYBaHR0cHM6Ly93d3cubGF0ZXN0bHkuY29tL2FnZW5jeS1uZXdzL3dvcmxkLW5ld3MtcXVhbnR1bS1jb21wdXRlcnMtYXJlLWxpa2Uta2FsZWlkb3Njb3Blcy13aHktdW51c3VhbC1tZXRhcGhvcnMtaGVscC1pbGx1c3RyYXRlLXNjaWVuY2UtYW5kLXRlY2hub2xvZ3ktNjA0MTI1MC5odG1sL2FtcA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>Quantum Racing powered by American Magic on the cusp of hometown win…</t>
+        </is>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>2024-06-16 02:00:59.908773</t>
+        </is>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiYWh0dHBzOi8vd3d3LmxpdmVzYWlsZGllLmNvbS9xdWFudHVtLXJhY2luZy1wb3dlcmVkLWJ5LWFtZXJpY2FuLW1hZ2ljLW9uLXRoZS1jdXNwLW9mLWhvbWV0b3duLXdpbi_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
           <t>Quantum Racing powered by American Magic on the cusp of hometown win...</t>
         </is>
       </c>
-      <c r="B178" t="inlineStr">
-        <is>
-          <t>2024-06-16 01:31:21.538115</t>
-        </is>
-      </c>
-      <c r="C178" t="inlineStr">
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>2024-06-16 02:05:28.341672</t>
+        </is>
+      </c>
+      <c r="C231" t="inlineStr">
         <is>
           <t>news.google.com/articles/CBMiYWh0dHBzOi8vd3d3LmxpdmVzYWlsZGllLmNvbS9xdWFudHVtLXJhY2luZy1wb3dlcmVkLWJ5LWFtZXJpY2FuLW1hZ2ljLW9uLXRoZS1jdXNwLW9mLWhvbWV0b3duLXdpbi_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>Quantum entangled photons used to measure the Earth's rotation</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>2024-06-16 02:05:28.341672</t>
+        </is>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiV2h0dHBzOi8vd3d3LmVhcnRoLmNvbS9uZXdzL3F1YW50dW0tZW50YW5nbGVtZW50LXBob3RvbnMtdXNlZC10by1tZWFzdXJlLWVhcnRoLXJvdGF0aW9uL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update main.py, and datetime_column_inserter.py with demo sentiment CSV file
</commit_message>
<xml_diff>
--- a/quantum_articles.xlsx
+++ b/quantum_articles.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C275"/>
+  <dimension ref="A1:C276"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1439,7 +1439,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>First Quantum Minerals Ltd. stock rises Monday, outperforms market</t>
+          <t>InterQnet: a heterogeneous full-stack approach to co-designing scalable quantum networks</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -1449,14 +1449,14 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMijgFodHRwczovL3d3dy5tYXJrZXR3YXRjaC5jb20vZGF0YS1uZXdzL2ZpcnN0LXF1YW50dW0tbWluZXJhbHMtbHRkLXN0b2NrLXJpc2VzLW1vbmRheS1vdXRwZXJmb3Jtcy1tYXJrZXQtNDU2YzAzNTMtZjI0ZTI5MDI3OTk3P21vZD1td19xdW90ZV9uZXdz0gGAAWh0dHBzOi8vd3d3Lm1hcmtldHdhdGNoLmNvbS9hbXAvZGF0YS1uZXdzL2ZpcnN0LXF1YW50dW0tbWluZXJhbHMtbHRkLXN0b2NrLXJpc2VzLW1vbmRheS1vdXRwZXJmb3Jtcy1tYXJrZXQtNDU2YzAzNTMtZjI0ZTI5MDI3OTk3?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiaWh0dHBzOi8vd3d3LmFubC5nb3YvaW50ZXJxbmV0LWEtaGV0ZXJvZ2VuZW91cy1mdWxsc3RhY2stYXBwcm9hY2gtdG8tY29kZXNpZ25pbmctc2NhbGFibGUtcXVhbnR1bS1uZXR3b3Jrc9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>How a quantum scientist, a nurse, and an economist are joining the fight against global poverty</t>
+          <t>US Restricts Exports to Top Quantum Labs in China</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -1466,14 +1466,14 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiaWh0dHBzOi8vbmV3cy5taXQuZWR1LzIwMjQvaG93LXF1YW50dW0tc2NpZW50aXN0LW51cnNlLWVjb25vbWlzdC1qb2luaW5nLWZpZ2h0LWFnYWluc3QtZ2xvYmFsLXBvdmVydHktMDYxMNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiSWh0dHBzOi8vd3cyLmFpcC5vcmcvZnlpL3VzLXJlc3RyaWN0cy1leHBvcnRzLXRvLXRvcC1xdWFudHVtLWxhYnMtaW4tY2hpbmHSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>US Restricts Exports to Top Quantum Labs in China</t>
+          <t>How a quantum scientist, a nurse, and an economist are joining the fight against global poverty</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -1483,14 +1483,14 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiSWh0dHBzOi8vd3cyLmFpcC5vcmcvZnlpL3VzLXJlc3RyaWN0cy1leHBvcnRzLXRvLXRvcC1xdWFudHVtLWxhYnMtaW4tY2hpbmHSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiaWh0dHBzOi8vbmV3cy5taXQuZWR1LzIwMjQvaG93LXF1YW50dW0tc2NpZW50aXN0LW51cnNlLWVjb25vbWlzdC1qb2luaW5nLWZpZ2h0LWFnYWluc3QtZ2xvYmFsLXBvdmVydHktMDYxMNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>InterQnet: a heterogeneous full-stack approach to co-designing scalable quantum networks</t>
+          <t>First Quantum Minerals Ltd. stock rises Monday, outperforms market</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -1500,7 +1500,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiaWh0dHBzOi8vd3d3LmFubC5nb3YvaW50ZXJxbmV0LWEtaGV0ZXJvZ2VuZW91cy1mdWxsc3RhY2stYXBwcm9hY2gtdG8tY29kZXNpZ25pbmctc2NhbGFibGUtcXVhbnR1bS1uZXR3b3Jrc9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMijgFodHRwczovL3d3dy5tYXJrZXR3YXRjaC5jb20vZGF0YS1uZXdzL2ZpcnN0LXF1YW50dW0tbWluZXJhbHMtbHRkLXN0b2NrLXJpc2VzLW1vbmRheS1vdXRwZXJmb3Jtcy1tYXJrZXQtNDU2YzAzNTMtZjI0ZTI5MDI3OTk3P21vZD1td19xdW90ZV9uZXdz0gGAAWh0dHBzOi8vd3d3Lm1hcmtldHdhdGNoLmNvbS9hbXAvZGF0YS1uZXdzL2ZpcnN0LXF1YW50dW0tbWluZXJhbHMtbHRkLXN0b2NrLXJpc2VzLW1vbmRheS1vdXRwZXJmb3Jtcy1tYXJrZXQtNDU2YzAzNTMtZjI0ZTI5MDI3OTk3?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
@@ -1745,7 +1745,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>First Quantum Minerals Ltd. stock outperforms market despite losses on the day</t>
+          <t>SEALSQ to Launch Two New Quantum Resistant Chips</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -1755,14 +1755,14 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiiQFodHRwczovL3d3dy5tYXJrZXR3YXRjaC5jb20vZGF0YS1uZXdzL2ZpcnN0LXF1YW50dW0tbWluZXJhbHMtbHRkLXN0b2NrLW91dHBlcmZvcm1zLW1hcmtldC1kZXNwaXRlLWxvc3Nlcy1vbi10aGUtZGF5LTMyNmIzM2M1LWNiODQ5MWQxZDc4M9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMieGh0dHBzOi8vd3d3Lmdsb2JlbmV3c3dpcmUuY29tL25ld3MtcmVsZWFzZS8yMDI0LzA2LzExLzI4OTY5NDYvMC9lbi9TRUFMU1EtdG8tTGF1bmNoLVR3by1OZXctUXVhbnR1bS1SZXNpc3RhbnQtQ2hpcHMuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Quantum Computing Inc. Reports First Quarter 2024 Financial Results</t>
+          <t>Nvidia confirms worldwide acceleration in quantum computing using CUDA-Q</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -1772,14 +1772,14 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiemh0dHBzOi8vd3d3LnBybmV3c3dpcmUuY29tL25ld3MtcmVsZWFzZXMvcXVhbnR1bS1jb21wdXRpbmctaW5jLXJlcG9ydHMtZmlyc3QtcXVhcnRlci0yMDI0LWZpbmFuY2lhbC1yZXN1bHRzLTMwMjE2OTY1Ny5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiX2h0dHBzOi8vcmVhZHdyaXRlLmNvbS9udmlkaWEtY29uZmlybXMtd29ybGR3aWRlLWFjY2VsZXJhdGlvbi1pbi1xdWFudHVtLWNvbXB1dGluZy11c2luZy1jdWRhLXEv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>World's smallest quantum light detector now fits on a silicon chip</t>
+          <t>New Technique Could Help Build Quantum Computers of the Future</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -1789,14 +1789,14 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiW2h0dHBzOi8vd3d3LmVhcnRoLmNvbS9uZXdzL3dvcmxkcy1zbWFsbGVzdC1xdWFudHVtLWxpZ2h0LWRldGVjdG9yLW5vdy1maXRzLW9uLXNpbGljb24tY2hpcC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiZWh0dHBzOi8vbmV3c2NlbnRlci5sYmwuZ292LzIwMjQvMDYvMTEvbmV3LXRlY2huaXF1ZS1jb3VsZC1oZWxwLWJ1aWxkLXF1YW50dW0tY29tcHV0ZXJzLW9mLXRoZS1mdXR1cmUv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>UPDATE 1-Canadian miner First Quantum starts arbitration against Panama, says government</t>
+          <t>Quantum Computing Inc. Reports First Quarter 2024 Financial Results</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -1806,14 +1806,14 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiVmh0dHBzOi8vY2Euc3BvcnRzLnlhaG9vLmNvbS9uZXdzLzEtY2FuYWRpYW4tbWluZXItZmlyc3QtcXVhbnR1bS0xNjE1MjQ1NjkuaHRtbD9zcmM9cnNz0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiemh0dHBzOi8vd3d3LnBybmV3c3dpcmUuY29tL25ld3MtcmVsZWFzZXMvcXVhbnR1bS1jb21wdXRpbmctaW5jLXJlcG9ydHMtZmlyc3QtcXVhcnRlci0yMDI0LWZpbmFuY2lhbC1yZXN1bHRzLTMwMjE2OTY1Ny5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>New Technique Could Help Build Quantum Computers of the Future</t>
+          <t>World's smallest quantum light detector now fits on a silicon chip</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -1823,14 +1823,14 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiZWh0dHBzOi8vbmV3c2NlbnRlci5sYmwuZ292LzIwMjQvMDYvMTEvbmV3LXRlY2huaXF1ZS1jb3VsZC1oZWxwLWJ1aWxkLXF1YW50dW0tY29tcHV0ZXJzLW9mLXRoZS1mdXR1cmUv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiW2h0dHBzOi8vd3d3LmVhcnRoLmNvbS9uZXdzL3dvcmxkcy1zbWFsbGVzdC1xdWFudHVtLWxpZ2h0LWRldGVjdG9yLW5vdy1maXRzLW9uLXNpbGljb24tY2hpcC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Nvidia confirms worldwide acceleration in quantum computing using CUDA-Q</t>
+          <t>UPDATE 1-Canadian miner First Quantum starts arbitration against Panama, says government</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -1840,14 +1840,14 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiX2h0dHBzOi8vcmVhZHdyaXRlLmNvbS9udmlkaWEtY29uZmlybXMtd29ybGR3aWRlLWFjY2VsZXJhdGlvbi1pbi1xdWFudHVtLWNvbXB1dGluZy11c2luZy1jdWRhLXEv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiVmh0dHBzOi8vY2Euc3BvcnRzLnlhaG9vLmNvbS9uZXdzLzEtY2FuYWRpYW4tbWluZXItZmlyc3QtcXVhbnR1bS0xNjE1MjQ1NjkuaHRtbD9zcmM9cnNz0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>SEALSQ to Launch Two New Quantum Resistant Chips</t>
+          <t>First Quantum Minerals Ltd. stock outperforms market despite losses on the day</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -1857,7 +1857,7 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMieGh0dHBzOi8vd3d3Lmdsb2JlbmV3c3dpcmUuY29tL25ld3MtcmVsZWFzZS8yMDI0LzA2LzExLzI4OTY5NDYvMC9lbi9TRUFMU1EtdG8tTGF1bmNoLVR3by1OZXctUXVhbnR1bS1SZXNpc3RhbnQtQ2hpcHMuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiiQFodHRwczovL3d3dy5tYXJrZXR3YXRjaC5jb20vZGF0YS1uZXdzL2ZpcnN0LXF1YW50dW0tbWluZXJhbHMtbHRkLXN0b2NrLW91dHBlcmZvcm1zLW1hcmtldC1kZXNwaXRlLWxvc3Nlcy1vbi10aGUtZGF5LTMyNmIzM2M1LWNiODQ5MWQxZDc4M9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
@@ -2068,7 +2068,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>A Step toward Quantum Gases of Doubly Polar Molecules</t>
+          <t>Zero Point Cryogenics secures $2.67 million to help cool quantum computers</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -2078,14 +2078,14 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiKGh0dHBzOi8vcGh5c2ljcy5hcHMub3JnL2FydGljbGVzL3YxNy9zNzPSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiXmh0dHBzOi8vYmV0YWtpdC5jb20vemVyby1wb2ludC1jcnlvZ2VuaWNzLXNlY3VyZXMtMi02Ny1taWxsaW9uLXRvLWhlbHAtY29vbC1xdWFudHVtLWNvbXB1dGVycy_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Reflections of an IQC graduate, June 2024 | Institute for Quantum Computing</t>
+          <t>D-Wave, Photonic Inc. lead BC's charge in quantum tech race</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -2095,14 +2095,14 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiXGh0dHBzOi8vdXdhdGVybG9vLmNhL2luc3RpdHV0ZS1mb3ItcXVhbnR1bS1jb21wdXRpbmcvbmV3cy9yZWZsZWN0aW9ucy1pcWMtZ3JhZHVhdGUtanVuZS0yMDI00gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiZmh0dHBzOi8vd3d3LmJpdi5jb20vbmV3cy90ZWNobm9sb2d5L3doeS1iYy1pcy1wb2lzZWQtdG8tYmVjb21lLWEtcXVhbnR1bS10ZWNobm9sb2d5LXBvd2VyaG91c2UtOTA3NTE0N9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Zero Point Cryogenics secures $2.67 million to help cool quantum computers</t>
+          <t>A Step toward Quantum Gases of Doubly Polar Molecules</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -2112,14 +2112,14 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiXmh0dHBzOi8vYmV0YWtpdC5jb20vemVyby1wb2ludC1jcnlvZ2VuaWNzLXNlY3VyZXMtMi02Ny1taWxsaW9uLXRvLWhlbHAtY29vbC1xdWFudHVtLWNvbXB1dGVycy_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiKGh0dHBzOi8vcGh5c2ljcy5hcHMub3JnL2FydGljbGVzL3YxNy9zNzPSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>D-Wave, Photonic Inc. lead BC's charge in quantum tech race</t>
+          <t>Reflections of an IQC graduate, June 2024 | Institute for Quantum Computing</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2129,7 +2129,7 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiZmh0dHBzOi8vd3d3LmJpdi5jb20vbmV3cy90ZWNobm9sb2d5L3doeS1iYy1pcy1wb2lzZWQtdG8tYmVjb21lLWEtcXVhbnR1bS10ZWNobm9sb2d5LXBvd2VyaG91c2UtOTA3NTE0N9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiXGh0dHBzOi8vdXdhdGVybG9vLmNhL2luc3RpdHV0ZS1mb3ItcXVhbnR1bS1jb21wdXRpbmcvbmV3cy9yZWZsZWN0aW9ucy1pcWMtZ3JhZHVhdGUtanVuZS0yMDI00gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
@@ -2221,7 +2221,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>New method integrates quantum dots with metasurfaces for enhanced luminescence</t>
+          <t>OTI Lumionics Selects Nord Quantique to Test New Quantum Computing Applications for Materials Science</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -2231,14 +2231,14 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiUGh0dHBzOi8vcGh5cy5vcmcvbmV3cy8yMDI0LTA2LW1ldGhvZC1xdWFudHVtLWRvdHMtbWV0YXN1cmZhY2VzLWx1bWluZXNjZW5jZS5odG1s0gFPaHR0cHM6Ly9waHlzLm9yZy9uZXdzLzIwMjQtMDYtbWV0aG9kLXF1YW50dW0tZG90cy1tZXRhc3VyZmFjZXMtbHVtaW5lc2NlbmNlLmFtcA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMijwFodHRwczovL3RoZXF1YW50dW1pbnNpZGVyLmNvbS8yMDI0LzA2LzEyL290aS1sdW1pb25pY3Mtc2VsZWN0cy1ub3JkLXF1YW50aXF1ZS10by10ZXN0LW5ldy1xdWFudHVtLWNvbXB1dGluZy1hcHBsaWNhdGlvbnMtZm9yLW1hdGVyaWFscy1zY2llbmNlL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Are CBDCs quantum safe? | Amnon Samid | VOX Ep. 80</t>
+          <t>Liquid crystals could improve quantum communication devices</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -2248,14 +2248,14 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiMWh0dHBzOi8vd3d3LmRpZ2Zpbmdyb3VwLmNvbS9jYmRjLXF1YW50dW0tYml0bWludC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiaWh0dHBzOi8vd3d3Lm5ld3NjaWVudGlzdC5jb20vYXJ0aWNsZS8yNDM1MDEwLWxpcXVpZC1jcnlzdGFscy1jb3VsZC1pbXByb3ZlLXF1YW50dW0tY29tbXVuaWNhdGlvbi1kZXZpY2VzL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Liquid crystals could improve quantum communication devices</t>
+          <t>New method integrates quantum dots with metasurfaces for enhanced luminescence</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -2265,14 +2265,14 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiaWh0dHBzOi8vd3d3Lm5ld3NjaWVudGlzdC5jb20vYXJ0aWNsZS8yNDM1MDEwLWxpcXVpZC1jcnlzdGFscy1jb3VsZC1pbXByb3ZlLXF1YW50dW0tY29tbXVuaWNhdGlvbi1kZXZpY2VzL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiUGh0dHBzOi8vcGh5cy5vcmcvbmV3cy8yMDI0LTA2LW1ldGhvZC1xdWFudHVtLWRvdHMtbWV0YXN1cmZhY2VzLWx1bWluZXNjZW5jZS5odG1s0gFPaHR0cHM6Ly9waHlzLm9yZy9uZXdzLzIwMjQtMDYtbWV0aG9kLXF1YW50dW0tZG90cy1tZXRhc3VyZmFjZXMtbHVtaW5lc2NlbmNlLmFtcA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>OTI Lumionics Selects Nord Quantique to Test New Quantum Computing Applications for Materials Science</t>
+          <t>Are CBDCs quantum safe? | Amnon Samid | VOX Ep. 80</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -2282,7 +2282,7 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMijwFodHRwczovL3RoZXF1YW50dW1pbnNpZGVyLmNvbS8yMDI0LzA2LzEyL290aS1sdW1pb25pY3Mtc2VsZWN0cy1ub3JkLXF1YW50aXF1ZS10by10ZXN0LW5ldy1xdWFudHVtLWNvbXB1dGluZy1hcHBsaWNhdGlvbnMtZm9yLW1hdGVyaWFscy1zY2llbmNlL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiMWh0dHBzOi8vd3d3LmRpZ2Zpbmdyb3VwLmNvbS9jYmRjLXF1YW50dW0tYml0bWludC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
@@ -2459,721 +2459,721 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Quantum, AI Combine to Transform Energy Generation, AI Summit London</t>
+          <t>Quantum data assimilation offers new approach to weather prediction</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>2024-06-13 13:31:21.553304</t>
+          <t>2024-06-13 16:03:03.146646</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiaGh0dHBzOi8vd3d3LmlvdHdvcmxkdG9kYXkuY29tL3F1YW50dW0vcXVhbnR1bS1haS1jb21iaW5lLXRvLXRyYW5zZm9ybS1lbmVyZ3ktZ2VuZXJhdGlvbi1haS1zdW1taXQtbG9uZG9u0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiSGh0dHBzOi8vcGh5cy5vcmcvbmV3cy8yMDI0LTA2LXF1YW50dW0tYXNzaW1pbGF0aW9uLWFwcHJvYWNoLXdlYXRoZXIuaHRtbNIBR2h0dHBzOi8vcGh5cy5vcmcvbmV3cy8yMDI0LTA2LXF1YW50dW0tYXNzaW1pbGF0aW9uLWFwcHJvYWNoLXdlYXRoZXIuYW1w?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>IBM thinks it's ready to turn quantum computing into an actual business</t>
+          <t>Quantum Tech Sector Hiring Stays Soft</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>2024-06-13 13:31:21.553304</t>
+          <t>2024-06-13 16:03:03.147645</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiRmh0dHBzOi8vbnoubmV3cy55YWhvby5jb20vaWJtLXRoaW5rcy1yZWFkeS10dXJuLXF1YW50dW0tMDUwMTAwNTc0Lmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiSWh0dHBzOi8vd3d3LmhwY3dpcmUuY29tLzIwMjQvMDYvMTMvcXVhbnR1bS10ZWNoLXNlY3Rvci1oaXJpbmctc3RheXMtc29mdC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Quantum Computers May Break Bitcoin by 2030, But We Won't Know About It</t>
+          <t>Rethinking quantum orthodoxy</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>2024-06-13 13:31:21.553304</t>
+          <t>2024-06-13 16:03:03.147645</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMia2h0dHBzOi8vY3J5cHRvbmV3cy5jb20vZXhjbHVzaXZlcy9xdWFudHVtLWNvbXB1dGVycy1tYXktYnJlYWstYml0Y29pbi1ieS0yMDMwLWJ1dC13ZS13b250LWtub3ctYWJvdXQtaXQuaHRt0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiM2h0dHBzOi8vd3d3LnNjaWVuY2Uub3JnL2RvaS8xMC4xMTI2L3NjaWVuY2UuYWRxMTA4OdIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Unilever's Alberto Prado on Quantum Computing's Future, Impact on Emerging Tech</t>
+          <t>Quantum control's role in scaling quantum computing</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>2024-06-13 13:31:21.553304</t>
+          <t>2024-06-13 16:03:03.147645</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMib2h0dHBzOi8vYWlidXNpbmVzcy5jb20vdmVydGljYWxzL3VuaWxldmVyLXMtYWxiZXJ0by1wcmFkby1vbi1xdWFudHVtLWNvbXB1dGluZy1zLWZ1dHVyZS1pbXBhY3Qtb24tZW1lcmdpbmctdGVjaNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMikQFodHRwczovL3d3dy5tY2tpbnNleS5jb20vY2FwYWJpbGl0aWVzL21ja2luc2V5LWRpZ2l0YWwvb3VyLWluc2lnaHRzL3RlY2gtZm9yd2FyZC91bmRlcnN0YW5kaW5nLXF1YW50dW0tY29udHJvbHMtcm9sZS1pbi1zY2FsaW5nLXF1YW50dW0tY29tcHV0aW5n0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>The Techy ASICS GEL-Quantum 360 VIII Mints Two “Digitune” Pack Pairs</t>
+          <t>First Quantum Minerals Ltd. stock falls Thursday, underperforms market</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>2024-06-13 13:31:21.553304</t>
+          <t>2024-06-13 16:03:03.148645</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiVGh0dHBzOi8vc25lYWtlcm5ld3MuY29tLzIwMjQvMDYvMTMvYXNpY3MtZ2VsLXF1YW50dW0tMzYwLXZpaWktZGlnaXR1bmUtcmVsZWFzZS1kYXRlL9IBVGh0dHBzOi8vc25lYWtlcm5ld3MuY29tLzIwMjQvMDYvMTMvYXNpY3MtZ2VsLXF1YW50dW0tMzYwLXZpaWktZGlnaXR1bmUtcmVsZWFzZS1kYXRlLw?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMigAFodHRwczovL3d3dy5tYXJrZXR3YXRjaC5jb20vZGF0YS1uZXdzL2ZpcnN0LXF1YW50dW0tbWluZXJhbHMtbHRkLXN0b2NrLWZhbGxzLXRodXJzZGF5LXVuZGVycGVyZm9ybXMtbWFya2V0LWRjNjU1MmU5LTUwOWQyMjE0ZDUwZdIBhAFodHRwczovL3d3dy5tYXJrZXR3YXRjaC5jb20vYW1wL2RhdGEtbmV3cy9maXJzdC1xdWFudHVtLW1pbmVyYWxzLWx0ZC1zdG9jay1mYWxscy10aHVyc2RheS11bmRlcnBlcmZvcm1zLW1hcmtldC1kYzY1NTJlOS01MDlkMjIxNGQ1MGU?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Three team for quantum-safe IoT SIM tech ...</t>
+          <t>Semiconductor Quantum Light Sources</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>2024-06-13 13:31:21.553304</t>
+          <t>2024-06-13 16:03:03.148645</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiSWh0dHBzOi8vd3d3LmVlbmV3c2V1cm9wZS5jb20vZW4vdGhyZWUtdGVhbS1mb3ItcXVhbnR1bS1zYWZlLWlvdC1zaW0tdGVjaC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMigAFodHRwOi8vd3d3Lm9wdGljYS1vcG4ub3JnL2hvbWUvYm9va19yZXZpZXdzLzIwMjQvMDYyNC9zZW1pY29uZHVjdG9yX3F1YW50dW1fbGlnaHRfc291cmNlc19mdW5kYW1lbnRhbHNfdGVjaG5vbG9naWVzX2FuZF9kZXZpY2VzL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Startup Diraq taps GlobalFoundries to forge silicon-based quantum chips</t>
+          <t>Liquid crystal source of photon pairs opens path to new generation of quantum sources</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>2024-06-13 13:31:21.553304</t>
+          <t>2024-06-13 16:03:03.149646</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMimgFodHRwczovL3d3dy5tc24uY29tL2VuLXVzL25ld3MvdGVjaG5vbG9neS9zdGFydHVwLWRpcmFxLXRhcHMtZ2xvYmFsZm91bmRyaWVzLXRvLWZvcmdlLXNpbGljb24tYmFzZWQtcXVhbnR1bS1jaGlwcy9hci1CQjFvYUJrQj9pdGVtPWZsaWdodHNwcmctdGlwc3Vic2MtdjFh0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiRWh0dHBzOi8vcGh5cy5vcmcvbmV3cy8yMDI0LTA2LWxpcXVpZC1jcnlzdGFsLXNvdXJjZS1waG90b24tcGFpcnMuaHRtbNIBRGh0dHBzOi8vcGh5cy5vcmcvbmV3cy8yMDI0LTA2LWxpcXVpZC1jcnlzdGFsLXNvdXJjZS1waG90b24tcGFpcnMuYW1w?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Fermilab Opens Underground Facility for Quantum Information Science Research</t>
+          <t>Underground quantum criticality is hot right now</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>2024-06-13 13:31:21.553304</t>
+          <t>2024-06-13 16:03:03.149646</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMibmh0dHBzOi8vZXhlY3V0aXZlZ292LmNvbS8yMDI0LzA2L2Zlcm1pbGFiLW9wZW5zLXVuZGVyZ3JvdW5kLWZhY2lsaXR5LWZvci1xdWFudHVtLWluZm9ybWF0aW9uLXNjaWVuY2UtcmVzZWFyY2gv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiMmh0dHBzOi8vd3d3Lm5hdHVyZS5jb20vYXJ0aWNsZXMvczQxNTY3LTAyNC0wMjU2OS150gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>A common misunderstanding about wave-particle duality | Opinion</t>
+          <t>Estonia's Roadmap for Encryption in the Age of Quantum Computing</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>2024-06-13 13:31:21.553304</t>
+          <t>2024-06-13 16:03:03.149646</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMibGh0dHBzOi8vd3d3LmNoZW1pc3RyeXdvcmxkLmNvbS9vcGluaW9uL2EtY29tbW9uLW1pc3VuZGVyc3RhbmRpbmctYWJvdXQtd2F2ZS1wYXJ0aWNsZS1kdWFsaXR5LzQwMTk1ODUuYXJ0aWNsZdIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiaWh0dHBzOi8vdGhlcXVhbnR1bWluc2lkZXIuY29tLzIwMjQvMDYvMTMvZXN0b25pYXMtcm9hZG1hcC1mb3ItZW5jcnlwdGlvbi1pbi10aGUtYWdlLW9mLXF1YW50dW0tY29tcHV0aW5nL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>How Quantum Computing and Machine Learning are Shaping Cybersecurity</t>
+          <t>Quantum control and Berry phase of electron spins in rotating levitated diamonds in high vacuum</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>2024-06-13 13:31:21.553304</t>
+          <t>2024-06-13 16:03:03.150645</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiNWh0dHBzOi8vd3d3LnNpbXBsaWxlYXJuLmNvbS9xdWFudHVtLWNvbXB1dGluZy1hcnRpY2xl0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiMmh0dHBzOi8vd3d3Lm5hdHVyZS5jb20vYXJ0aWNsZXMvczQxNDY3LTAyNC00OTE3NS0z0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>3 Quantum Computing Stocks to Turn $100000 Into $1 Million: June Edition</t>
+          <t>Quantum Teleportation Just Got Real: Achieving 90% Fidelity Amidst Noise</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>2024-06-13 13:31:21.553304</t>
+          <t>2024-06-13 16:03:03.150645</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiaGh0dHBzOi8vaW52ZXN0b3JwbGFjZS5jb20vMjAyNC8wNi8zLXF1YW50dW0tY29tcHV0aW5nLXN0b2Nrcy10by10dXJuLTEwMDAwMC1pbnRvLTEtbWlsbGlvbi1qdW5lLWVkaXRpb24v0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiYGh0dHBzOi8vc2NpdGVjaGRhaWx5LmNvbS9xdWFudHVtLXRlbGVwb3J0YXRpb24tanVzdC1nb3QtcmVhbC1hY2hpZXZpbmctOTAtZmlkZWxpdHktYW1pZHN0LW5vaXNlL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>Chip-Scale Visible Sources Aim to Release Quantum Technology from the Lab</t>
+          <t>The Sphere in Las Vegas really is a 'quantum leap' for live music: Inside the first shows</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>2024-06-13 13:31:21.553304</t>
+          <t>2024-06-13 16:03:03.151646</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiXmh0dHBzOi8vd3d3LnBob3Rvbmljcy5jb20vQXJ0aWNsZXMvQ2hpcC1TY2FsZV9WaXNpYmxlX1NvdXJjZXNfQWltX3RvX1JlbGVhc2VfUXVhbnR1bS9wNS9hNjk5NjPSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiSGh0dHBzOi8vY2EubmV3cy55YWhvby5jb20vc3BoZXJlLWxhcy12ZWdhcy1yZWFsbHktcXVhbnR1bS0xNDIwMjYzNTcuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>Microsoft CEO says Azure Quantum will address the big challenges in computing</t>
+          <t>Diraq Achieves Record Accuracy For Quantum Computing Device Manufactured by Existing Semiconductor Infrastructure</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>2024-06-13 13:31:21.553304</t>
+          <t>2024-06-13 16:03:03.151646</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiUGh0dHBzOi8vdWsuc3R5bGUueWFob28uY29tL3N0eWxlL21pY3Jvc29mdC1jZW8tc2F5cy1henVyZS1xdWFudHVtLTE2MjYwMTAxOC5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMimwFodHRwczovL3RoZXF1YW50dW1pbnNpZGVyLmNvbS8yMDI0LzA2LzEzL2RpcmFxLWFjaGlldmVzLXJlY29yZC1hY2N1cmFjeS1mb3ItcXVhbnR1bS1jb21wdXRpbmctZGV2aWNlLW1hbnVmYWN0dXJlZC1ieS1leGlzdGluZy1zZW1pY29uZHVjdG9yLWluZnJhc3RydWN0dXJlL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>Quantum Revolution “Living up to Hype,” Quantum Summit London</t>
+          <t>Riverlane Joins the Quantum Energy Initiative</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>2024-06-13 13:31:21.553304</t>
+          <t>2024-06-13 16:03:03.151646</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiYGh0dHBzOi8vd3d3LmlvdHdvcmxkdG9kYXkuY29tL3F1YW50dW0vcXVhbnR1bS1yZXZvbHV0aW9uLWxpdmluZy11cC10by1oeXBlLXF1YW50dW0tc3VtbWl0LWxvbmRvbtIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiV2h0dHBzOi8vdGhlcXVhbnR1bWluc2lkZXIuY29tLzIwMjQvMDYvMTMvcml2ZXJsYW5lLWpvaW5zLXRoZS1xdWFudHVtLWVuZXJneS1pbml0aWF0aXZlL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Quantum data assimilation offers new approach to weather prediction</t>
+          <t>Unlock Generous Growth With These 3 Top Quantum Computing Stocks</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>2024-06-13 15:23:50.050461</t>
+          <t>2024-06-13 16:03:03.151646</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiSGh0dHBzOi8vcGh5cy5vcmcvbmV3cy8yMDI0LTA2LXF1YW50dW0tYXNzaW1pbGF0aW9uLWFwcHJvYWNoLXdlYXRoZXIuaHRtbNIBR2h0dHBzOi8vcGh5cy5vcmcvbmV3cy8yMDI0LTA2LXF1YW50dW0tYXNzaW1pbGF0aW9uLWFwcHJvYWNoLXdlYXRoZXIuYW1w?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMie2h0dHBzOi8vbWFya2V0cy5idXNpbmVzc2luc2lkZXIuY29tL25ld3Mvc3RvY2tzL3VubG9jay1nZW5lcm91cy1ncm93dGgtd2l0aC10aGVzZS0zLXRvcC1xdWFudHVtLWNvbXB1dGluZy1zdG9ja3MtMTAzMzQ3NzY0MNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>First Quantum Minerals Ltd. stock falls Thursday, underperforms market</t>
+          <t>Quantum data assimilation: A quantum leap in weather prediction</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>2024-06-13 15:23:50.050461</t>
+          <t>2024-06-13 16:03:03.151646</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMigAFodHRwczovL3d3dy5tYXJrZXR3YXRjaC5jb20vZGF0YS1uZXdzL2ZpcnN0LXF1YW50dW0tbWluZXJhbHMtbHRkLXN0b2NrLWZhbGxzLXRodXJzZGF5LXVuZGVycGVyZm9ybXMtbWFya2V0LWRjNjU1MmU5LTUwOWQyMjE0ZDUwZdIBhAFodHRwczovL3d3dy5tYXJrZXR3YXRjaC5jb20vYW1wL2RhdGEtbmV3cy9maXJzdC1xdWFudHVtLW1pbmVyYWxzLWx0ZC1zdG9jay1mYWxscy10aHVyc2RheS11bmRlcnBlcmZvcm1zLW1hcmtldC1kYzY1NTJlOS01MDlkMjIxNGQ1MGU?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiMGh0dHBzOi8vd3d3LmV1cmVrYWxlcnQub3JnL25ld3MtcmVsZWFzZXMvMTA0Nzk1NNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>Semiconductor Quantum Light Sources</t>
+          <t>Queen Mary Chooses Cryogenic Technology From Oxford Instruments NanoScience to Support Quantum Research</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>2024-06-13 15:23:50.050461</t>
+          <t>2024-06-13 16:03:03.152646</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMigAFodHRwOi8vd3d3Lm9wdGljYS1vcG4ub3JnL2hvbWUvYm9va19yZXZpZXdzLzIwMjQvMDYyNC9zZW1pY29uZHVjdG9yX3F1YW50dW1fbGlnaHRfc291cmNlc19mdW5kYW1lbnRhbHNfdGVjaG5vbG9naWVzX2FuZF9kZXZpY2VzL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMikQFodHRwczovL3RoZXF1YW50dW1pbnNpZGVyLmNvbS8yMDI0LzA2LzEzL3F1ZWVuLW1hcnktY2hvb3Nlcy1jcnlvZ2VuaWMtdGVjaG5vbG9neS1mcm9tLW94Zm9yZC1pbnN0cnVtZW50cy1uYW5vc2NpZW5jZS10by1zdXBwb3J0LXF1YW50dW0tcmVzZWFyY2gv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>Quantum Tech Sector Hiring Stays Soft</t>
+          <t>Fascinating behavior of 'super photons' in the quantum realm</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>2024-06-13 15:23:50.050461</t>
+          <t>2024-06-13 16:03:03.152646</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiSWh0dHBzOi8vd3d3LmhwY3dpcmUuY29tLzIwMjQvMDYvMTMvcXVhbnR1bS10ZWNoLXNlY3Rvci1oaXJpbmctc3RheXMtc29mdC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiT2h0dHBzOi8vd3d3LmVhcnRoLmNvbS9uZXdzL3N1cGVyLXBob3RvbnMtZmFzY2luYXRpbmctYmVoYXZpb3ItaW4tcXVhbnR1bS1yZWFsbS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>Quantum control's role in scaling quantum computing</t>
+          <t>Recurrent quantum embedding neural network and its application in vulnerability detection | Scientific Reports</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>2024-06-13 15:23:50.050461</t>
+          <t>2024-06-13 16:03:03.152646</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMikQFodHRwczovL3d3dy5tY2tpbnNleS5jb20vY2FwYWJpbGl0aWVzL21ja2luc2V5LWRpZ2l0YWwvb3VyLWluc2lnaHRzL3RlY2gtZm9yd2FyZC91bmRlcnN0YW5kaW5nLXF1YW50dW0tY29udHJvbHMtcm9sZS1pbi1zY2FsaW5nLXF1YW50dW0tY29tcHV0aW5n0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiMmh0dHBzOi8vd3d3Lm5hdHVyZS5jb20vYXJ0aWNsZXMvczQxNTk4LTAyNC02MzAyMS150gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>Rethinking quantum orthodoxy</t>
+          <t>Quantum Sensors market is projected to grow at a CAGR of 15.3% by 2034: Visiongain</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>2024-06-13 15:23:50.050461</t>
+          <t>2024-06-13 16:03:03.154258</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiM2h0dHBzOi8vd3d3LnNjaWVuY2Uub3JnL2RvaS8xMC4xMTI2L3NjaWVuY2UuYWRxMTA4OdIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMimAFodHRwczovL3d3dy5nbG9iZW5ld3N3aXJlLmNvbS9uZXdzLXJlbGVhc2UvMjAyNC8wNi8xMy8yODk4MDg4LzAvZW4vUXVhbnR1bS1TZW5zb3JzLW1hcmtldC1pcy1wcm9qZWN0ZWQtdG8tZ3Jvdy1hdC1hLUNBR1Itb2YtMTUtMy1ieS0yMDM0LVZpc2lvbmdhaW4uaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>Liquid crystal source of photon pairs opens path to new generation of quantum sources</t>
+          <t>United Nations Declares 2025 as International Year of Quantum Science and Technology</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>2024-06-13 15:23:50.060570</t>
+          <t>2024-06-13 16:03:03.155183</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiRWh0dHBzOi8vcGh5cy5vcmcvbmV3cy8yMDI0LTA2LWxpcXVpZC1jcnlzdGFsLXNvdXJjZS1waG90b24tcGFpcnMuaHRtbNIBRGh0dHBzOi8vcGh5cy5vcmcvbmV3cy8yMDI0LTA2LWxpcXVpZC1jcnlzdGFsLXNvdXJjZS1waG90b24tcGFpcnMuYW1w?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMieGh0dHBzOi8vcXVhbnR1bWNvbXB1dGluZ3JlcG9ydC5jb20vdW5pdGVkLW5hdGlvbnMtZGVjbGFyZXMtMjAyNS1hcy1pbnRlcm5hdGlvbmFsLXllYXItb2YtcXVhbnR1bS1zY2llbmNlLWFuZC10ZWNobm9sb2d5L9IBfGh0dHBzOi8vcXVhbnR1bWNvbXB1dGluZ3JlcG9ydC5jb20vdW5pdGVkLW5hdGlvbnMtZGVjbGFyZXMtMjAyNS1hcy1pbnRlcm5hdGlvbmFsLXllYXItb2YtcXVhbnR1bS1zY2llbmNlLWFuZC10ZWNobm9sb2d5L2FtcC8?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>Underground quantum criticality is hot right now</t>
+          <t>Diraq Reports 99.9% Qubit Control Accuracy with imec-Produced Silicon Quantum Dot</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>2024-06-13 15:23:50.060570</t>
+          <t>2024-06-13 16:03:03.155183</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiMmh0dHBzOi8vd3d3Lm5hdHVyZS5jb20vYXJ0aWNsZXMvczQxNTY3LTAyNC0wMjU2OS150gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMidmh0dHBzOi8vd3d3LmhwY3dpcmUuY29tL29mZi10aGUtd2lyZS9kaXJhcS1yZXBvcnRzLTk5LTktcXViaXQtY29udHJvbC1hY2N1cmFjeS13aXRoLWltZWMtcHJvZHVjZWQtc2lsaWNvbi1xdWFudHVtLWRvdC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>Estonia's Roadmap for Encryption in the Age of Quantum Computing</t>
+          <t>Diraq achieves record fidelity for single-qubit quantum computing | Electronics360</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>2024-06-13 15:23:50.060570</t>
+          <t>2024-06-13 16:03:03.155183</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiaWh0dHBzOi8vdGhlcXVhbnR1bWluc2lkZXIuY29tLzIwMjQvMDYvMTMvZXN0b25pYXMtcm9hZG1hcC1mb3ItZW5jcnlwdGlvbi1pbi10aGUtYWdlLW9mLXF1YW50dW0tY29tcHV0aW5nL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMidWh0dHBzOi8vZWxlY3Ryb25pY3MzNjAuZ2xvYmFsc3BlYy5jb20vYXJ0aWNsZS8yMTE3OC9kaXJhcS1hY2hpZXZlcy1yZWNvcmQtZmlkZWxpdHktZm9yLXNpbmdsZS1xdWJpdC1xdWFudHVtLWNvbXB1dGluZ9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>Quantum control and Berry phase of electron spins in rotating levitated diamonds in high vacuum</t>
+          <t>Quantum, AI Combine to Transform Energy Generation, AI Summit London</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>2024-06-13 15:23:50.061647</t>
+          <t>2024-06-13 16:03:03.156182</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiMmh0dHBzOi8vd3d3Lm5hdHVyZS5jb20vYXJ0aWNsZXMvczQxNDY3LTAyNC00OTE3NS0z0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiaGh0dHBzOi8vd3d3LmlvdHdvcmxkdG9kYXkuY29tL3F1YW50dW0vcXVhbnR1bS1haS1jb21iaW5lLXRvLXRyYW5zZm9ybS1lbmVyZ3ktZ2VuZXJhdGlvbi1haS1zdW1taXQtbG9uZG9u0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>Quantum Teleportation Just Got Real: Achieving 90% Fidelity Amidst Noise</t>
+          <t>Chip-Scale Visible Sources Aim to Release Quantum Technology from the Lab</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>2024-06-13 15:23:50.062710</t>
+          <t>2024-06-13 16:03:03.156182</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiYGh0dHBzOi8vc2NpdGVjaGRhaWx5LmNvbS9xdWFudHVtLXRlbGVwb3J0YXRpb24tanVzdC1nb3QtcmVhbC1hY2hpZXZpbmctOTAtZmlkZWxpdHktYW1pZHN0LW5vaXNlL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiXmh0dHBzOi8vd3d3LnBob3Rvbmljcy5jb20vQXJ0aWNsZXMvQ2hpcC1TY2FsZV9WaXNpYmxlX1NvdXJjZXNfQWltX3RvX1JlbGVhc2VfUXVhbnR1bS9wNS9hNjk5NjPSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>The Sphere in Las Vegas really is a 'quantum leap' for live music: Inside the first shows</t>
+          <t>IBM thinks it's ready to turn quantum computing into an actual business</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>2024-06-13 15:23:50.062710</t>
+          <t>2024-06-13 16:03:03.156182</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiSGh0dHBzOi8vY2EubmV3cy55YWhvby5jb20vc3BoZXJlLWxhcy12ZWdhcy1yZWFsbHktcXVhbnR1bS0xNDIwMjYzNTcuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiRmh0dHBzOi8vbnoubmV3cy55YWhvby5jb20vaWJtLXRoaW5rcy1yZWFkeS10dXJuLXF1YW50dW0tMDUwMTAwNTc0Lmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>Diraq Achieves Record Accuracy For Quantum Computing Device Manufactured by Existing Semiconductor Infrastructure</t>
+          <t>Microsoft CEO says Azure Quantum will address the big challenges in computing</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>2024-06-13 15:23:50.062710</t>
+          <t>2024-06-13 16:03:03.156182</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMimwFodHRwczovL3RoZXF1YW50dW1pbnNpZGVyLmNvbS8yMDI0LzA2LzEzL2RpcmFxLWFjaGlldmVzLXJlY29yZC1hY2N1cmFjeS1mb3ItcXVhbnR1bS1jb21wdXRpbmctZGV2aWNlLW1hbnVmYWN0dXJlZC1ieS1leGlzdGluZy1zZW1pY29uZHVjdG9yLWluZnJhc3RydWN0dXJlL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiUGh0dHBzOi8vdWsuc3R5bGUueWFob28uY29tL3N0eWxlL21pY3Jvc29mdC1jZW8tc2F5cy1henVyZS1xdWFudHVtLTE2MjYwMTAxOC5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>Riverlane Joins the Quantum Energy Initiative</t>
+          <t>Unilever's Alberto Prado on Quantum Computing's Future, Impact on Emerging Tech</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>2024-06-13 15:23:50.063739</t>
+          <t>2024-06-13 16:03:03.156182</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiV2h0dHBzOi8vdGhlcXVhbnR1bWluc2lkZXIuY29tLzIwMjQvMDYvMTMvcml2ZXJsYW5lLWpvaW5zLXRoZS1xdWFudHVtLWVuZXJneS1pbml0aWF0aXZlL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMib2h0dHBzOi8vYWlidXNpbmVzcy5jb20vdmVydGljYWxzL3VuaWxldmVyLXMtYWxiZXJ0by1wcmFkby1vbi1xdWFudHVtLWNvbXB1dGluZy1zLWZ1dHVyZS1pbXBhY3Qtb24tZW1lcmdpbmctdGVjaNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>Unlock Generous Growth With These 3 Top Quantum Computing Stocks</t>
+          <t>Quantum Computers May Break Bitcoin by 2030, But We Won't Know About It</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>2024-06-13 15:23:50.064735</t>
+          <t>2024-06-13 16:03:03.157180</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMie2h0dHBzOi8vbWFya2V0cy5idXNpbmVzc2luc2lkZXIuY29tL25ld3Mvc3RvY2tzL3VubG9jay1nZW5lcm91cy1ncm93dGgtd2l0aC10aGVzZS0zLXRvcC1xdWFudHVtLWNvbXB1dGluZy1zdG9ja3MtMTAzMzQ3NzY0MNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMia2h0dHBzOi8vY3J5cHRvbmV3cy5jb20vZXhjbHVzaXZlcy9xdWFudHVtLWNvbXB1dGVycy1tYXktYnJlYWstYml0Y29pbi1ieS0yMDMwLWJ1dC13ZS13b250LWtub3ctYWJvdXQtaXQuaHRt0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>Quantum data assimilation: A quantum leap in weather prediction</t>
+          <t>How Quantum Computing and Machine Learning are Shaping Cybersecurity</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>2024-06-13 15:23:50.064735</t>
+          <t>2024-06-13 16:03:03.157180</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiMGh0dHBzOi8vd3d3LmV1cmVrYWxlcnQub3JnL25ld3MtcmVsZWFzZXMvMTA0Nzk1NNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiNWh0dHBzOi8vd3d3LnNpbXBsaWxlYXJuLmNvbS9xdWFudHVtLWNvbXB1dGluZy1hcnRpY2xl0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>Fascinating behavior of 'super photons' in the quantum realm</t>
+          <t>The Techy ASICS GEL-Quantum 360 VIII Mints Two “Digitune” Pack Pairs</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>2024-06-13 15:23:50.064735</t>
+          <t>2024-06-13 16:03:03.157180</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiT2h0dHBzOi8vd3d3LmVhcnRoLmNvbS9uZXdzL3N1cGVyLXBob3RvbnMtZmFzY2luYXRpbmctYmVoYXZpb3ItaW4tcXVhbnR1bS1yZWFsbS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiVGh0dHBzOi8vc25lYWtlcm5ld3MuY29tLzIwMjQvMDYvMTMvYXNpY3MtZ2VsLXF1YW50dW0tMzYwLXZpaWktZGlnaXR1bmUtcmVsZWFzZS1kYXRlL9IBVGh0dHBzOi8vc25lYWtlcm5ld3MuY29tLzIwMjQvMDYvMTMvYXNpY3MtZ2VsLXF1YW50dW0tMzYwLXZpaWktZGlnaXR1bmUtcmVsZWFzZS1kYXRlLw?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>Queen Mary Chooses Cryogenic Technology From Oxford Instruments NanoScience to Support Quantum Research</t>
+          <t>Quantum Revolution “Living up to Hype,” Quantum Summit London</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>2024-06-13 15:23:50.065731</t>
+          <t>2024-06-13 16:03:03.157180</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMikQFodHRwczovL3RoZXF1YW50dW1pbnNpZGVyLmNvbS8yMDI0LzA2LzEzL3F1ZWVuLW1hcnktY2hvb3Nlcy1jcnlvZ2VuaWMtdGVjaG5vbG9neS1mcm9tLW94Zm9yZC1pbnN0cnVtZW50cy1uYW5vc2NpZW5jZS10by1zdXBwb3J0LXF1YW50dW0tcmVzZWFyY2gv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiYGh0dHBzOi8vd3d3LmlvdHdvcmxkdG9kYXkuY29tL3F1YW50dW0vcXVhbnR1bS1yZXZvbHV0aW9uLWxpdmluZy11cC10by1oeXBlLXF1YW50dW0tc3VtbWl0LWxvbmRvbtIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>Recurrent quantum embedding neural network and its application in vulnerability detection | Scientific Reports</t>
+          <t>3 Quantum Computing Stocks to Turn $100000 Into $1 Million: June Edition</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>2024-06-13 15:23:50.066730</t>
+          <t>2024-06-13 16:03:03.158181</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiMmh0dHBzOi8vd3d3Lm5hdHVyZS5jb20vYXJ0aWNsZXMvczQxNTk4LTAyNC02MzAyMS150gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiaGh0dHBzOi8vaW52ZXN0b3JwbGFjZS5jb20vMjAyNC8wNi8zLXF1YW50dW0tY29tcHV0aW5nLXN0b2Nrcy10by10dXJuLTEwMDAwMC1pbnRvLTEtbWlsbGlvbi1qdW5lLWVkaXRpb24v0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>Quantum Sensors market is projected to grow at a CAGR of 15.3% by 2034: Visiongain</t>
+          <t>A common misunderstanding about wave-particle duality | Opinion</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>2024-06-13 15:23:50.067730</t>
+          <t>2024-06-13 16:03:03.158181</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMimAFodHRwczovL3d3dy5nbG9iZW5ld3N3aXJlLmNvbS9uZXdzLXJlbGVhc2UvMjAyNC8wNi8xMy8yODk4MDg4LzAvZW4vUXVhbnR1bS1TZW5zb3JzLW1hcmtldC1pcy1wcm9qZWN0ZWQtdG8tZ3Jvdy1hdC1hLUNBR1Itb2YtMTUtMy1ieS0yMDM0LVZpc2lvbmdhaW4uaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMibGh0dHBzOi8vd3d3LmNoZW1pc3RyeXdvcmxkLmNvbS9vcGluaW9uL2EtY29tbW9uLW1pc3VuZGVyc3RhbmRpbmctYWJvdXQtd2F2ZS1wYXJ0aWNsZS1kdWFsaXR5LzQwMTk1ODUuYXJ0aWNsZdIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>Diraq Reports 99.9% Qubit Control Accuracy with imec-Produced Silicon Quantum Dot</t>
+          <t>Three team for quantum-safe IoT SIM tech ...</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>2024-06-13 15:23:50.068730</t>
+          <t>2024-06-13 16:03:03.158181</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMidmh0dHBzOi8vd3d3LmhwY3dpcmUuY29tL29mZi10aGUtd2lyZS9kaXJhcS1yZXBvcnRzLTk5LTktcXViaXQtY29udHJvbC1hY2N1cmFjeS13aXRoLWltZWMtcHJvZHVjZWQtc2lsaWNvbi1xdWFudHVtLWRvdC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiSWh0dHBzOi8vd3d3LmVlbmV3c2V1cm9wZS5jb20vZW4vdGhyZWUtdGVhbS1mb3ItcXVhbnR1bS1zYWZlLWlvdC1zaW0tdGVjaC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>United Nations Declares 2025 as International Year of Quantum Science and Technology</t>
+          <t>Startup Diraq taps GlobalFoundries to forge silicon-based quantum chips</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>2024-06-13 15:23:50.068730</t>
+          <t>2024-06-13 16:03:03.158181</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMieGh0dHBzOi8vcXVhbnR1bWNvbXB1dGluZ3JlcG9ydC5jb20vdW5pdGVkLW5hdGlvbnMtZGVjbGFyZXMtMjAyNS1hcy1pbnRlcm5hdGlvbmFsLXllYXItb2YtcXVhbnR1bS1zY2llbmNlLWFuZC10ZWNobm9sb2d5L9IBfGh0dHBzOi8vcXVhbnR1bWNvbXB1dGluZ3JlcG9ydC5jb20vdW5pdGVkLW5hdGlvbnMtZGVjbGFyZXMtMjAyNS1hcy1pbnRlcm5hdGlvbmFsLXllYXItb2YtcXVhbnR1bS1zY2llbmNlLWFuZC10ZWNobm9sb2d5L2FtcC8?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMimgFodHRwczovL3d3dy5tc24uY29tL2VuLXVzL25ld3MvdGVjaG5vbG9neS9zdGFydHVwLWRpcmFxLXRhcHMtZ2xvYmFsZm91bmRyaWVzLXRvLWZvcmdlLXNpbGljb24tYmFzZWQtcXVhbnR1bS1jaGlwcy9hci1CQjFvYUJrQj9pdGVtPWZsaWdodHNwcmctdGlwc3Vic2MtdjFh0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>Diraq achieves record fidelity for single-qubit quantum computing | Electronics360</t>
+          <t>Deloitte's Scott Buchholz gives a primer on quantum computing</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>2024-06-13 15:23:50.070288</t>
+          <t>2024-06-13 16:03:03.159180</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMidWh0dHBzOi8vZWxlY3Ryb25pY3MzNjAuZ2xvYmFsc3BlYy5jb20vYXJ0aWNsZS8yMTE3OC9kaXJhcS1hY2hpZXZlcy1yZWNvcmQtZmlkZWxpdHktZm9yLXNpbmdsZS1xdWJpdC1xdWFudHVtLWNvbXB1dGluZ9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMicWh0dHBzOi8vd3d3Mi5kZWxvaXR0ZS5jb20vdXMvZW4vcGFnZXMvY29uc3VsdGluZy9hcnRpY2xlcy9zY290dC1idWNoaG9sei1naXZlcy1hLXByaW1lci1vbi1xdWFudHVtLWNvbXB1dGluZy5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>Quantinuum AI Team's Advance Quickens Pace Toward Merging Quantum Computing And AI</t>
+          <t>Fermilab Opens Underground Facility for Quantum Information Science Research</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>2024-06-14 13:06:43.366610</t>
+          <t>2024-06-13 16:03:03.159180</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMie2h0dHBzOi8vdGhlcXVhbnR1bWluc2lkZXIuY29tLzIwMjQvMDYvMTQvcXVhbnRpbnV1bS1haS10ZWFtcy1hZHZhbmNlLXF1aWNrZW5zLXBhY2UtdG93YXJkLW1lcmdpbmctcXVhbnR1bS1jb21wdXRpbmctYW5kLWFpL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMibmh0dHBzOi8vZXhlY3V0aXZlZ292LmNvbS8yMDI0LzA2L2Zlcm1pbGFiLW9wZW5zLXVuZGVyZ3JvdW5kLWZhY2lsaXR5LWZvci1xdWFudHVtLWluZm9ybWF0aW9uLXNjaWVuY2UtcmVzZWFyY2gv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>Quantum entanglement measures Earth rotation</t>
+          <t>Quantinuum AI Team's Advance Quickens Pace Toward Merging Quantum Computing And AI</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>2024-06-14 13:06:43.373729</t>
+          <t>2024-06-14 13:06:43.366610</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiMGh0dHBzOi8vd3d3LmV1cmVrYWxlcnQub3JnL25ld3MtcmVsZWFzZXMvMTA0ODA5NdIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMie2h0dHBzOi8vdGhlcXVhbnR1bWluc2lkZXIuY29tLzIwMjQvMDYvMTQvcXVhbnRpbnV1bS1haS10ZWFtcy1hZHZhbmNlLXF1aWNrZW5zLXBhY2UtdG93YXJkLW1lcmdpbmctcXVhbnR1bS1jb21wdXRpbmctYW5kLWFpL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>SpaceX launches 'zero fuel' engine into space</t>
+          <t>Quantum entanglement measures Earth rotation</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>2024-06-14 13:31:21.545640</t>
+          <t>2024-06-14 13:06:43.373729</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiT2h0dHBzOi8vY2Euc3R5bGUueWFob28uY29tL25ld3Mvc3BhY2V4LWxhdW5jaGVzLXplcm8tZnVlbC1lbmdpbmUtMTQ1NDAzODYyLmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiMGh0dHBzOi8vd3d3LmV1cmVrYWxlcnQub3JnL25ld3MtcmVsZWFzZXMvMTA0ODA5NdIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>Scott Bakula Addresses 'Quantum Leap' Reboot Involvement Speculation, Says It Was “Very Difficult Decision” To Pass ...</t>
+          <t>IQC celebrates latest Dean of Science Award winners</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>2024-06-14 13:31:21.548290</t>
+          <t>2024-06-14 14:00:59.908773</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiTmh0dHBzOi8vY2EubW92aWVzLnlhaG9vLmNvbS9zY290dC1iYWt1bGEtYWRkcmVzc2VzLXF1YW50dW0tbGVhcC0yMjA5NDUzNzMuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiamh0dHBzOi8vdXdhdGVybG9vLmNhL2luc3RpdHV0ZS1mb3ItcXVhbnR1bS1jb21wdXRpbmcvbmV3cy9pcWMtY2VsZWJyYXRlcy1sYXRlc3QtZGVhbi1zY2llbmNlLWF3YXJkLXdpbm5lcnPSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>Diraq is going to make a hybrid chip combining quantum and classical processors</t>
+          <t>Midnight Sun Mining partners with KoBold Metals; First Quantum</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>2024-06-14 13:31:21.553304</t>
+          <t>2024-06-14 14:00:59.908773</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMihQFodHRwczovL3d3dy5zdGFydHVwZGFpbHkubmV0L3RvcGljL3F1YW50dW0tY29tcHV0aW5nL2RpcmFxLWlzLWdvaW5nLXRvLW1ha2UtYS1oeWJyaWQtY2hpcC1jb21iaW5pbmctcXVhbnR1bS1hbmQtY2xhc3NpY2FsLXByb2Nlc3NvcnMv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiZ2h0dHBzOi8vd3d3Lm1pbmluZy5jb20vc3BvbnNvcmVkLWNvbnRlbnQvbWlkbmlnaHQtc3VuLW1pbmluZy1wYXJ0bmVycy13aXRoLWtvYm9sZC1tZXRhbHMtZmlyc3QtcXVhbnR1bS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>Midnight Sun Mining partners with KoBold Metals; First Quantum</t>
+          <t>Experimental observation of Earth’s rotation with quantum entanglement</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -3183,14 +3183,14 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiZ2h0dHBzOi8vd3d3Lm1pbmluZy5jb20vc3BvbnNvcmVkLWNvbnRlbnQvbWlkbmlnaHQtc3VuLW1pbmluZy1wYXJ0bmVycy13aXRoLWtvYm9sZC1tZXRhbHMtZmlyc3QtcXVhbnR1bS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiMmh0dHBzOi8vd3d3LnNjaWVuY2Uub3JnL2RvaS8xMC4xMTI2L3NjaWFkdi5hZG8wMjE10gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>Experimental observation of Earth’s rotation with quantum entanglement</t>
+          <t>No Small Thing: Quantum Startups For The Here And Now</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
@@ -3200,14 +3200,14 @@
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiMmh0dHBzOi8vd3d3LnNjaWVuY2Uub3JnL2RvaS8xMC4xMTI2L3NjaWFkdi5hZG8wMjE10gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMia2h0dHBzOi8vd3d3LmZvcmJlcy5jb20vc2l0ZXMvdHJldm9yY2xhd3Nvbi8yMDI0LzA2LzE0L25vLXNtYWxsLXRoaW5nLXF1YW50dW0tc3RhcnR1cHMtZm9yLXRoZS1oZXJlLWFuZC1ub3cv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>No Small Thing: Quantum Startups For The Here And Now</t>
+          <t>First Quantum Minerals Ltd (FM-T) Quote - Press Release</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
@@ -3217,14 +3217,14 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMia2h0dHBzOi8vd3d3LmZvcmJlcy5jb20vc2l0ZXMvdHJldm9yY2xhd3Nvbi8yMDI0LzA2LzE0L25vLXNtYWxsLXRoaW5nLXF1YW50dW0tc3RhcnR1cHMtZm9yLXRoZS1oZXJlLWFuZC1ub3cv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMijQFodHRwczovL3d3dy50aGVnbG9iZWFuZG1haWwuY29tL2ludmVzdGluZy9tYXJrZXRzL3N0b2Nrcy9GTS1UL3ByZXNzcmVsZWFzZXMvMjY3MzQ1MTkvY2xvc2luZy1iZWxsLWZpcnN0LXF1YW50dW0tbWluZXJhbHMtbHRkLXVwLW9uLW1vbmRheS1mbS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>First Quantum Minerals Ltd (FM-T) Quote - Press Release</t>
+          <t>Physicists measured Earth’s rotation using quantum entanglement</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
@@ -3234,48 +3234,48 @@
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMijQFodHRwczovL3d3dy50aGVnbG9iZWFuZG1haWwuY29tL2ludmVzdGluZy9tYXJrZXRzL3N0b2Nrcy9GTS1UL3ByZXNzcmVsZWFzZXMvMjY3MzQ1MTkvY2xvc2luZy1iZWxsLWZpcnN0LXF1YW50dW0tbWluZXJhbHMtbHRkLXVwLW9uLW1vbmRheS1mbS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiR2h0dHBzOi8vd3d3LnNjaWVuY2VuZXdzLm9yZy9hcnRpY2xlL2VhcnRoLXJvdGF0aW9uLXF1YW50dW0tZW50YW5nbGVtZW500gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>Physicists measured Earth’s rotation using quantum entanglement</t>
+          <t>D-Wave Quantum Inc (QBTS-N) Quote - Press Release</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>2024-06-14 14:00:59.908773</t>
+          <t>2024-06-14 14:00:59.912386</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiR2h0dHBzOi8vd3d3LnNjaWVuY2VuZXdzLm9yZy9hcnRpY2xlL2VhcnRoLXJvdGF0aW9uLXF1YW50dW0tZW50YW5nbGVtZW500gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiwgFodHRwczovL3d3dy50aGVnbG9iZWFuZG1haWwuY29tL2ludmVzdGluZy9tYXJrZXRzL3N0b2Nrcy9RQlRTLU4vcHJlc3NyZWxlYXNlcy8yNjgyOTk2My9kLXdhdmUtbnlzZS1xYnRzLWV4dGVuZHMtcGFydG5lcnNoaXAtd2l0aC1hcmFtY28tcmVzZWFyY2gtY2VudGVyLXRvLWhlbHAtbWF4aW1pemUtcXVhbnR1bXMtcG9zaXRpdmUtaW1wYWN0L9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>IQC celebrates latest Dean of Science Award winners</t>
+          <t>The Growing Interest in On-Prem Quantum Computing</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>2024-06-14 14:00:59.908773</t>
+          <t>2024-06-14 14:00:59.912386</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiamh0dHBzOi8vdXdhdGVybG9vLmNhL2luc3RpdHV0ZS1mb3ItcXVhbnR1bS1jb21wdXRpbmcvbmV3cy9pcWMtY2VsZWJyYXRlcy1sYXRlc3QtZGVhbi1zY2llbmNlLWF3YXJkLXdpbm5lcnPSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiUGh0dHBzOi8vaW5zaWRlaHBjLmNvbS8yMDI0LzA2L3RoZS1ncm93aW5nLWludGVyZXN0LWluLW9uLXByZW0tcXVhbnR1bS1jb21wdXRpbmcv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>D-Wave Quantum Inc (QBTS-N) Quote - Press Release</t>
+          <t>How Classical AI is ‘Saving’ Quantum Computing: A Talk with IBM’s Ismael Faro</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
@@ -3285,48 +3285,48 @@
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiwgFodHRwczovL3d3dy50aGVnbG9iZWFuZG1haWwuY29tL2ludmVzdGluZy9tYXJrZXRzL3N0b2Nrcy9RQlRTLU4vcHJlc3NyZWxlYXNlcy8yNjgyOTk2My9kLXdhdmUtbnlzZS1xYnRzLWV4dGVuZHMtcGFydG5lcnNoaXAtd2l0aC1hcmFtY28tcmVzZWFyY2gtY2VudGVyLXRvLWhlbHAtbWF4aW1pemUtcXVhbnR1bXMtcG9zaXRpdmUtaW1wYWN0L9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMic2h0dHBzOi8vdGhlcXVhbnR1bWluc2lkZXIuY29tLzIwMjQvMDYvMTQvaG93LWNsYXNzaWNhbC1haS1pcy1zYXZpbmctcXVhbnR1bS1jb21wdXRpbmctYS10YWxrLXdpdGgtaWJtcy1pc21hZWwtZmFyby_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>The Growing Interest in On-Prem Quantum Computing</t>
+          <t>Advancements in Quantum Computing and Their Influence on</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>2024-06-14 14:00:59.912386</t>
+          <t>2024-06-14 14:00:59.916918</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiUGh0dHBzOi8vaW5zaWRlaHBjLmNvbS8yMDI0LzA2L3RoZS1ncm93aW5nLWludGVyZXN0LWluLW9uLXByZW0tcXVhbnR1bS1jb21wdXRpbmcv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiXGh0dHBzOi8vd3d3Lm9wZW5wci5jb20vbmV3cy8zNTM5NjkyL2FkdmFuY2VtZW50cy1pbi1xdWFudHVtLWNvbXB1dGluZy1hbmQtdGhlaXItaW5mbHVlbmNlLW9u0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>How Classical AI is ‘Saving’ Quantum Computing: A Talk with IBM’s Ismael Faro</t>
+          <t>Fraunhofer, EV team for 300mm 3D quantum chip ...</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>2024-06-14 14:00:59.912386</t>
+          <t>2024-06-14 14:00:59.916918</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMic2h0dHBzOi8vdGhlcXVhbnR1bWluc2lkZXIuY29tLzIwMjQvMDYvMTQvaG93LWNsYXNzaWNhbC1haS1pcy1zYXZpbmctcXVhbnR1bS1jb21wdXRpbmctYS10YWxrLXdpdGgtaWJtcy1pc21hZWwtZmFyby_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiTWh0dHBzOi8vd3d3LmVlbmV3c2V1cm9wZS5jb20vZW4vZnJhdW5ob2Zlci1ldi10ZWFtLWZvci0zMDBtbS0zZC1xdWFudHVtLWNoaXAv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>Government plans to work with TCS, HCL and other IT giants for quantum technology</t>
+          <t>Financial regulators need a ‘quantum’ leap</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
@@ -3336,14 +3336,14 @@
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiowFodHRwczovL3RpbWVzb2ZpbmRpYS5pbmRpYXRpbWVzLmNvbS90ZWNobm9sb2d5L3RlY2gtbmV3cy9nb3Zlcm5tZW50LXBsYW5zLXRvLXdvcmstd2l0aC10Y3MtaGNsLWFuZC1vdGhlci1pdC1naWFudHMtZm9yLXF1YW50dW0tdGVjaG5vbG9neS9hcnRpY2xlc2hvdy8xMTEwMDMwNDEuY21z0gGnAWh0dHBzOi8vdGltZXNvZmluZGlhLmluZGlhdGltZXMuY29tL3RlY2hub2xvZ3kvdGVjaC1uZXdzL2dvdmVybm1lbnQtcGxhbnMtdG8td29yay13aXRoLXRjcy1oY2wtYW5kLW90aGVyLWl0LWdpYW50cy1mb3ItcXVhbnR1bS10ZWNobm9sb2d5L2FtcF9hcnRpY2xlc2hvdy8xMTEwMDMwNDEuY21z?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMieWh0dHBzOi8vd3d3Lm1zbi5jb20vZW4taW4vbW9uZXkvdG9wc3Rvcmllcy9maW5hbmNpYWwtcmVndWxhdG9ycy1uZWVkLWEtcXVhbnR1bS1sZWFwL2FyLUJCMW9nNHhPP29jaWQ9ZmluYW5jZS12ZXJ0aHAtZmVlZHPSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>Soon, QDEL Screens Could Perfect What OLED Couldn't</t>
+          <t>First topological quantum simulator device in strong light-matter interaction regime to operate at room temperatures</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
@@ -3353,14 +3353,14 @@
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiTGh0dHBzOi8vd3d3Lmhvd3RvZ2Vlay5jb20vc29vbi1xZGVsLXNjcmVlbnMtY291bGQtcGVyZmVjdC13aGF0LW9sZWQtY291bGRudC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMi0wFodHRwczovL3d3dy5tc24uY29tL2VuLXVzL25ld3MvdGVjaG5vbG9neS9maXJzdC10b3BvbG9naWNhbC1xdWFudHVtLXNpbXVsYXRvci1kZXZpY2UtaW4tc3Ryb25nLWxpZ2h0LW1hdHRlci1pbnRlcmFjdGlvbi1yZWdpbWUtdG8tb3BlcmF0ZS1hdC1yb29tLXRlbXBlcmF0dXJlcy9hci1CQjFtWm5pYT9pdGVtPWZsaWdodHNwcmctdGlwc3Vic2MtdjFhP3NlYXNvbj0yMDI00gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>‘Escape From Shadow Physics’ Review: Quantum Weirdness</t>
+          <t>African traditional spirituality parallels quantum physics: Implications development</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
@@ -3370,14 +3370,14 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiaWh0dHBzOi8vd3d3Lm1zbi5jb20vZW4tdXMvbmV3cy90ZWNobm9sb2d5L2VzY2FwZS1mcm9tLXNoYWRvdy1waHlzaWNzLXJldmlldy1xdWFudHVtLXdlaXJkbmVzcy9hci1CQjFvZU5wUNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiiwFodHRwczovL3d3dy5naGFuYXdlYi5jb20vR2hhbmFIb21lUGFnZS9mZWF0dXJlcy9BZnJpY2FuLXRyYWRpdGlvbmFsLXNwaXJpdHVhbGl0eS1wYXJhbGxlbHMtcXVhbnR1bS1waHlzaWNzLUltcGxpY2F0aW9ucy1kZXZlbG9wbWVudC0xOTM1NjM50gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>New Dimensions in Quantum Computing: Majorana Particles Go 2D</t>
+          <t>Indian Government To Collaborate With IT Giants For Quantum Technology Development</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
@@ -3387,14 +3387,14 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiVmh0dHBzOi8vc2NpdGVjaGRhaWx5LmNvbS9uZXctZGltZW5zaW9ucy1pbi1xdWFudHVtLWNvbXB1dGluZy1tYWpvcmFuYS1wYXJ0aWNsZXMtZ28tMmQv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMilAFodHRwczovL3d3dy50aW1lc25vd25ld3MuY29tL3RlY2hub2xvZ3ktc2NpZW5jZS9pbmRpYW4tZ292ZXJubWVudC10by1jb2xsYWJvcmF0ZS13aXRoLWl0LWdpYW50cy1mb3ItcXVhbnR1bS10ZWNobm9sb2d5LWRldmVsb3BtZW50LWFydGljbGUtMTExMDAzNzkz0gGYAWh0dHBzOi8vd3d3LnRpbWVzbm93bmV3cy5jb20vdGVjaG5vbG9neS1zY2llbmNlL2luZGlhbi1nb3Zlcm5tZW50LXRvLWNvbGxhYm9yYXRlLXdpdGgtaXQtZ2lhbnRzLWZvci1xdWFudHVtLXRlY2hub2xvZ3ktZGV2ZWxvcG1lbnQtYXJ0aWNsZS0xMTEwMDM3OTMvYW1w?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>Daniel Oi</t>
+          <t>High-tech highway: US 36 corridor emerging as hotspot for quantum, aerospace, biotech – BizWest</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
@@ -3404,14 +3404,14 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiP2h0dHBzOi8vd3d3Lmxhc2VyZm9jdXN3b3JsZC5jb20vaG9tZS9jb250YWN0LzU1MDg4Mjk2L2RhbmllbC1vadIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMicmh0dHBzOi8vYml6d2VzdC5jb20vMjAyNC8wNi8xNC9oaWdoLXRlY2gtaGlnaHdheS11cy0zNi1jb3JyaWRvci1lbWVyZ2luZy1hcy1ob3RzcG90LWZvci1xdWFudHVtLWFlcm9zcGFjZS1iaW90ZWNoL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>High-tech highway: US 36 corridor emerging as hotspot for quantum, aerospace, biotech – BizWest</t>
+          <t>Daniel Oi</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
@@ -3421,14 +3421,14 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMicmh0dHBzOi8vYml6d2VzdC5jb20vMjAyNC8wNi8xNC9oaWdoLXRlY2gtaGlnaHdheS11cy0zNi1jb3JyaWRvci1lbWVyZ2luZy1hcy1ob3RzcG90LWZvci1xdWFudHVtLWFlcm9zcGFjZS1iaW90ZWNoL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiP2h0dHBzOi8vd3d3Lmxhc2VyZm9jdXN3b3JsZC5jb20vaG9tZS9jb250YWN0LzU1MDg4Mjk2L2RhbmllbC1vadIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>Best Internet Providers in Seattle, Washington</t>
+          <t>‘Escape From Shadow Physics’ Review: Quantum Weirdness</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -3438,14 +3438,14 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiSWh0dHBzOi8vd3d3LmNuZXQuY29tL2hvbWUvaW50ZXJuZXQvYmVzdC1pbnRlcm5ldC1wcm92aWRlcnMtaW4tc2VhdHRsZS13YS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiaWh0dHBzOi8vd3d3Lm1zbi5jb20vZW4tdXMvbmV3cy90ZWNobm9sb2d5L2VzY2FwZS1mcm9tLXNoYWRvdy1waHlzaWNzLXJldmlldy1xdWFudHVtLXdlaXJkbmVzcy9hci1CQjFvZU5wUNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>Indian Government To Collaborate With IT Giants For Quantum Technology Development</t>
+          <t>Government plans to work with TCS, HCL and other IT giants for quantum technology</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
@@ -3455,14 +3455,14 @@
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMilAFodHRwczovL3d3dy50aW1lc25vd25ld3MuY29tL3RlY2hub2xvZ3ktc2NpZW5jZS9pbmRpYW4tZ292ZXJubWVudC10by1jb2xsYWJvcmF0ZS13aXRoLWl0LWdpYW50cy1mb3ItcXVhbnR1bS10ZWNobm9sb2d5LWRldmVsb3BtZW50LWFydGljbGUtMTExMDAzNzkz0gGYAWh0dHBzOi8vd3d3LnRpbWVzbm93bmV3cy5jb20vdGVjaG5vbG9neS1zY2llbmNlL2luZGlhbi1nb3Zlcm5tZW50LXRvLWNvbGxhYm9yYXRlLXdpdGgtaXQtZ2lhbnRzLWZvci1xdWFudHVtLXRlY2hub2xvZ3ktZGV2ZWxvcG1lbnQtYXJ0aWNsZS0xMTEwMDM3OTMvYW1w?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiowFodHRwczovL3RpbWVzb2ZpbmRpYS5pbmRpYXRpbWVzLmNvbS90ZWNobm9sb2d5L3RlY2gtbmV3cy9nb3Zlcm5tZW50LXBsYW5zLXRvLXdvcmstd2l0aC10Y3MtaGNsLWFuZC1vdGhlci1pdC1naWFudHMtZm9yLXF1YW50dW0tdGVjaG5vbG9neS9hcnRpY2xlc2hvdy8xMTEwMDMwNDEuY21z0gGnAWh0dHBzOi8vdGltZXNvZmluZGlhLmluZGlhdGltZXMuY29tL3RlY2hub2xvZ3kvdGVjaC1uZXdzL2dvdmVybm1lbnQtcGxhbnMtdG8td29yay13aXRoLXRjcy1oY2wtYW5kLW90aGVyLWl0LWdpYW50cy1mb3ItcXVhbnR1bS10ZWNobm9sb2d5L2FtcF9hcnRpY2xlc2hvdy8xMTEwMDMwNDEuY21z?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>Bizarre device uses 'blind quantum computing' to let you access quantum computers from home</t>
+          <t>Best Internet Providers in Seattle, Washington</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
@@ -3472,150 +3472,150 @@
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMirQFodHRwczovL3d3dy5tc24uY29tL2VuLXVzL25ld3MvdGVjaG5vbG9neS9iaXphcnJlLWRldmljZS11c2VzLWJsaW5kLXF1YW50dW0tY29tcHV0aW5nLXRvLWxldC15b3UtYWNjZXNzLXF1YW50dW0tY29tcHV0ZXJzLWZyb20taG9tZS9hci1CQjFtekNwNT9pdGVtPWZsaWdodHNwcmctdGlwc3Vic2MtdjFhL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiSWh0dHBzOi8vd3d3LmNuZXQuY29tL2hvbWUvaW50ZXJuZXQvYmVzdC1pbnRlcm5ldC1wcm92aWRlcnMtaW4tc2VhdHRsZS13YS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>First topological quantum simulator device in strong light-matter interaction regime to operate at room temperatures</t>
+          <t>Ripple Issues Urgent Warning on Quantum Computing's Threat to Blockchain Security</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>2024-06-14 14:00:59.916918</t>
+          <t>2024-06-14 14:00:59.922033</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMi0wFodHRwczovL3d3dy5tc24uY29tL2VuLXVzL25ld3MvdGVjaG5vbG9neS9maXJzdC10b3BvbG9naWNhbC1xdWFudHVtLXNpbXVsYXRvci1kZXZpY2UtaW4tc3Ryb25nLWxpZ2h0LW1hdHRlci1pbnRlcmFjdGlvbi1yZWdpbWUtdG8tb3BlcmF0ZS1hdC1yb29tLXRlbXBlcmF0dXJlcy9hci1CQjFtWm5pYT9pdGVtPWZsaWdodHNwcmctdGlwc3Vic2MtdjFhP3NlYXNvbj0yMDI00gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMifWh0dHBzOi8vd3d3LmJpZ25ld3NuZXR3b3JrLmNvbS9uZXdzLzI3NDQxMDI2OS9yaXBwbGUtaXNzdWVzLXVyZ2VudC13YXJuaW5nLW9uLXF1YW50dW0tY29tcHV0aW5nLXRocmVhdC10by1ibG9ja2NoYWluLXNlY3VyaXR50gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>Advancements in Quantum Computing and Their Influence on</t>
+          <t>דף בית | Emirates News Agency</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>2024-06-14 14:00:59.916918</t>
+          <t>2024-06-14 14:00:59.922033</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiXGh0dHBzOi8vd3d3Lm9wZW5wci5jb20vbmV3cy8zNTM5NjkyL2FkdmFuY2VtZW50cy1pbi1xdWFudHVtLWNvbXB1dGluZy1hbmQtdGhlaXItaW5mbHVlbmNlLW9u0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiTmh0dHBzOi8vd3d3LndhbS5hZS9lbi9hcnRpY2xlL2IzbGZ5eW0tc29yYm9ubmUtdW5pdmVyc2l0eS1hYnUtZGhhYmktdGVjaG5vbG9nedIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>Financial regulators need a ‘quantum’ leap</t>
+          <t>TCS, HCLTech and Others Join Govt's INR 6000 Crore Quantum Tech Project – AIM</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>2024-06-14 14:00:59.916918</t>
+          <t>2024-06-14 14:00:59.922033</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMieWh0dHBzOi8vd3d3Lm1zbi5jb20vZW4taW4vbW9uZXkvdG9wc3Rvcmllcy9maW5hbmNpYWwtcmVndWxhdG9ycy1uZWVkLWEtcXVhbnR1bS1sZWFwL2FyLUJCMW9nNHhPP29jaWQ9ZmluYW5jZS12ZXJ0aHAtZmVlZHPSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiZGh0dHBzOi8vYW5hbHl0aWNzaW5kaWFtYWcuY29tL3Rjcy1oY2x0ZWNoLWFuZC1vdGhlcnMtam9pbi1nb3Z0cy1pbnItNjAwMC1jcm9yZS1xdWFudHVtLXRlY2gtcHJvamVjdC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>D-Wave quantum director Emil Michael sells over $27 million in warrants</t>
+          <t>Govt to work with IT majors for Rs 6,000 crore quantum tech scheme</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>2024-06-14 14:00:59.916918</t>
+          <t>2024-06-14 14:00:59.922033</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMifWh0dHBzOi8vaW4uaW52ZXN0aW5nLmNvbS9uZXdzL2NvbXBhbnktbmV3cy9kd2F2ZS1xdWFudHVtLWRpcmVjdG9yLWVtaWwtbWljaGFlbC1zZWxscy1vdmVyLTI3LW1pbGxpb24taW4td2FycmFudHMtOTNDSC00MjU1MTI00gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMieWh0dHBzOi8vd3d3Lm1zbi5jb20vZW4taW4vbW9uZXkvdG9wc3Rvcmllcy9nb3Z0LXRvLXdvcmstd2l0aC1pdC1tYWpvcnMtZm9yLXJzLTYtMDAwLWNyb3JlLXF1YW50dW0tdGVjaC1zY2hlbWUvYXItQkIxb2NVVG3SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>Lantronix Wins 2024 IoT Evolution Asset Tracking Award for FOX3 Telematic Gateway</t>
+          <t>Data Loading into Quantum: The Gateway to Quantum Computing Power</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>2024-06-14 14:00:59.916918</t>
+          <t>2024-06-14 14:00:59.922033</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMinAFodHRwczovL3d3dy5nbG9iZW5ld3N3aXJlLmNvbS9lbi9uZXdzLXJlbGVhc2UvMjAyNC8wNi8xMy8yODk4MTQ0LzAvZW4vTGFudHJvbml4LVdpbnMtMjAyNC1Jb1QtRXZvbHV0aW9uLUFzc2V0LVRyYWNraW5nLUF3YXJkLWZvci1GT1gzLVRlbGVtYXRpYy1HYXRld2F5Lmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiWWh0dHBzOi8vdGVjaGJ1bGxpb24uY29tL2RhdGEtbG9hZGluZy1pbnRvLXF1YW50dW0tdGhlLWdhdGV3YXktdG8tcXVhbnR1bS1jb21wdXRpbmctcG93ZXIv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>Fraunhofer, EV team for 300mm 3D quantum chip ...</t>
+          <t>52 Super Series : Back to reality for Quantum, the dream continues for Vayu</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>2024-06-14 14:00:59.916918</t>
+          <t>2024-06-14 14:00:59.922033</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiTWh0dHBzOi8vd3d3LmVlbmV3c2V1cm9wZS5jb20vZW4vZnJhdW5ob2Zlci1ldi10ZWFtLWZvci0zMDBtbS0zZC1xdWFudHVtLWNoaXAv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiXmh0dHBzOi8vbmF1dGljYS5uZXdzLzUyLXN1cGVyLXNlcmllcy1iYWNrLXRvLXJlYWxpdHktZm9yLXF1YW50dW0tdGhlLWRyZWFtLWNvbnRpbnVlcy1mb3ItdmF5dS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>African traditional spirituality parallels quantum physics: Implications development</t>
+          <t>Former Quantum House CEO Robi Jurney to serve as Palm Beach Chamber's new board chair</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>2024-06-14 14:00:59.916918</t>
+          <t>2024-06-14 14:00:59.922033</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiiwFodHRwczovL3d3dy5naGFuYXdlYi5jb20vR2hhbmFIb21lUGFnZS9mZWF0dXJlcy9BZnJpY2FuLXRyYWRpdGlvbmFsLXNwaXJpdHVhbGl0eS1wYXJhbGxlbHMtcXVhbnR1bS1waHlzaWNzLUltcGxpY2F0aW9ucy1kZXZlbG9wbWVudC0xOTM1NjM50gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiQGh0dHBzOi8vd3d3LmFvbC5jb20vZm9ybWVyLXF1YW50dW0taG91c2UtY2VvLXJvYmktMDkwMjI0MTg3Lmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>Femtosecond Lasers Spearhead the Quantum Computing Revolution</t>
+          <t>Indian Govt Mulls Working With TCS, HCL and Tech Mahindra to Develop Quantum Tech Software Under Rs 6000 ...</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>2024-06-14 14:00:59.916918</t>
+          <t>2024-06-14 14:00:59.922033</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiV2h0dHBzOi8vc2NpdGVjaGRhaWx5LmNvbS9mZW10b3NlY29uZC1sYXNlcnMtc3BlYXJoZWFkLXRoZS1xdWFudHVtLWNvbXB1dGluZy1yZXZvbHV0aW9uL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiTmh0dHBzOi8vd3d3LmluZGlhbndlYjIuY29tLzIwMjQvMDYvaW5kaWFuLWdvdnQtbXVsbHMtd29ya2luZy13aXRoLXRjcy1oY2wuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>דף בית | Emirates News Agency</t>
+          <t>Govt to work with TCS, HCL, others for Rs 6,000 crore quantum tech scheme</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -3625,14 +3625,14 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiTmh0dHBzOi8vd3d3LndhbS5hZS9lbi9hcnRpY2xlL2IzbGZ5eW0tc29yYm9ubmUtdW5pdmVyc2l0eS1hYnUtZGhhYmktdGVjaG5vbG9nedIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMif2h0dHBzOi8vd3d3Lm1vbmV5Y29udHJvbC5jb20vdGVjaG5vbG9neS9nb3Z0LXRvLXdvcmstd2l0aC1pdC1tYWpvcnMtZm9yLXJzLTYwMDAtY3JvcmUtcXVhbnR1bS10ZWNoLXNjaGVtZS1hcnRpY2xlLTEyNzQ4NjEzLmh0bWzSAYMBaHR0cHM6Ly93d3cubW9uZXljb250cm9sLmNvbS90ZWNobm9sb2d5L2dvdnQtdG8td29yay13aXRoLWl0LW1ham9ycy1mb3ItcnMtNjAwMC1jcm9yZS1xdWFudHVtLXRlY2gtc2NoZW1lLWFydGljbGUtMTI3NDg2MTMuaHRtbC9hbXA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>TCS, HCLTech and Others Join Govt's INR 6000 Crore Quantum Tech Project – AIM</t>
+          <t>Tech3 | Navi's UPI payments surge 10x in 2 months; IT majors to join govt's quantum mission; and more</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
@@ -3642,738 +3642,738 @@
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiZGh0dHBzOi8vYW5hbHl0aWNzaW5kaWFtYWcuY29tL3Rjcy1oY2x0ZWNoLWFuZC1vdGhlcnMtam9pbi1nb3Z0cy1pbnItNjAwMC1jcm9yZS1xdWFudHVtLXRlY2gtcHJvamVjdC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiqwFodHRwczovL3d3dy5tb25leWNvbnRyb2wuY29tL25ld3MvdGVjaG5vbG9neS1zdGFydHVwL25ld3NsZXR0ZXJzL01DVGVjaDMvdGVjaDMtbmF2aS1zLXVwaS1wYXltZW50cy1zdXJnZS0xMHgtaW4tMi1tb250aHMtaXQtbWFqb3JzLXRvLWpvaW4tZ292dC1zLXF1YW50dW0tbWlzc2lvbi1hbmQtbW9yZS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>Govt to work with IT majors for Rs 6,000 crore quantum tech scheme</t>
+          <t>Fresh Insights On D-Wave Quantum Inc (QBTS)</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>2024-06-14 14:00:59.922033</t>
+          <t>2024-06-14 14:00:59.924036</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMieWh0dHBzOi8vd3d3Lm1zbi5jb20vZW4taW4vbW9uZXkvdG9wc3Rvcmllcy9nb3Z0LXRvLXdvcmstd2l0aC1pdC1tYWpvcnMtZm9yLXJzLTYtMDAwLWNyb3JlLXF1YW50dW0tdGVjaC1zY2hlbWUvYXItQkIxb2NVVG3SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiVGh0dHBzOi8vd3d3LnN0b2Nrc3JlZ2lzdGVyLmNvbS8yMDI0LzA2LzE0L2ZyZXNoLWluc2lnaHRzLW9uLWQtd2F2ZS1xdWFudHVtLWluYy1xYnRzL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>Data Loading into Quantum: The Gateway to Quantum Computing Power</t>
+          <t>Investing in the Future: 3 Top Quantum Computing Stocks for Growth</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>2024-06-14 14:00:59.922033</t>
+          <t>2024-06-14 14:00:59.924036</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiWWh0dHBzOi8vdGVjaGJ1bGxpb24uY29tL2RhdGEtbG9hZGluZy1pbnRvLXF1YW50dW0tdGhlLWdhdGV3YXktdG8tcXVhbnR1bS1jb21wdXRpbmctcG93ZXIv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiYGh0dHBzOi8vd3d3LmZlYXR1cmV3ZWVrbHkuY29tL2ludmVzdGluZy1pbi10aGUtZnV0dXJlLTMtdG9wLXF1YW50dW0tY29tcHV0aW5nLXN0b2Nrcy1mb3ItZ3Jvd3RoL9IBZGh0dHBzOi8vd3d3LmZlYXR1cmV3ZWVrbHkuY29tL2ludmVzdGluZy1pbi10aGUtZnV0dXJlLTMtdG9wLXF1YW50dW0tY29tcHV0aW5nLXN0b2Nrcy1mb3ItZ3Jvd3RoL2FtcC8?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>52 Super Series : Back to reality for Quantum, the dream continues for Vayu</t>
+          <t>Physicists confirm quantum entanglement persists between top quarks, the heaviest known fundamental particles</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>2024-06-14 14:00:59.922033</t>
+          <t>2024-06-14 16:03:03.143083</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiXmh0dHBzOi8vbmF1dGljYS5uZXdzLzUyLXN1cGVyLXNlcmllcy1iYWNrLXRvLXJlYWxpdHktZm9yLXF1YW50dW0tdGhlLWRyZWFtLWNvbnRpbnVlcy1mb3ItdmF5dS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiUmh0dHBzOi8vcGh5cy5vcmcvbmV3cy8yMDI0LTA2LXBoeXNpY2lzdHMtcXVhbnR1bS1lbnRhbmdsZW1lbnQtcGVyc2lzdHMtcXVhcmtzLmh0bWzSAVFodHRwczovL3BoeXMub3JnL25ld3MvMjAyNC0wNi1waHlzaWNpc3RzLXF1YW50dW0tZW50YW5nbGVtZW50LXBlcnNpc3RzLXF1YXJrcy5hbXA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>Former Quantum House CEO Robi Jurney to serve as Palm Beach Chamber's new board chair</t>
+          <t>IQC celebrates latest Dean of Science Award winners | Institute for Quantum Computing</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>2024-06-14 14:00:59.922033</t>
+          <t>2024-06-14 16:03:03.144083</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiQGh0dHBzOi8vd3d3LmFvbC5jb20vZm9ybWVyLXF1YW50dW0taG91c2UtY2VvLXJvYmktMDkwMjI0MTg3Lmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiamh0dHBzOi8vdXdhdGVybG9vLmNhL2luc3RpdHV0ZS1mb3ItcXVhbnR1bS1jb21wdXRpbmcvbmV3cy9pcWMtY2VsZWJyYXRlcy1sYXRlc3QtZGVhbi1zY2llbmNlLWF3YXJkLXdpbm5lcnPSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>Indian Govt Mulls Working With TCS, HCL and Tech Mahindra to Develop Quantum Tech Software Under Rs 6000 ...</t>
+          <t>Closing Bell: First Quantum Minerals Ltd up on Monday (FM)</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>2024-06-14 14:00:59.922033</t>
+          <t>2024-06-14 16:03:03.144616</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiTmh0dHBzOi8vd3d3LmluZGlhbndlYjIuY29tLzIwMjQvMDYvaW5kaWFuLWdvdnQtbXVsbHMtd29ya2luZy13aXRoLXRjcy1oY2wuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMijQFodHRwczovL3d3dy50aGVnbG9iZWFuZG1haWwuY29tL2ludmVzdGluZy9tYXJrZXRzL3N0b2Nrcy9GTS1UL3ByZXNzcmVsZWFzZXMvMjY3MzQ1MTkvY2xvc2luZy1iZWxsLWZpcnN0LXF1YW50dW0tbWluZXJhbHMtbHRkLXVwLW9uLW1vbmRheS1mbS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>Tech3 | Navi's UPI payments surge 10x in 2 months; IT majors to join govt's quantum mission; and more</t>
+          <t>Midnight Sun Mining partners with KoBold Metals; First Quantum - MINING.COM</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>2024-06-14 14:00:59.922033</t>
+          <t>2024-06-14 16:03:03.144616</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiqwFodHRwczovL3d3dy5tb25leWNvbnRyb2wuY29tL25ld3MvdGVjaG5vbG9neS1zdGFydHVwL25ld3NsZXR0ZXJzL01DVGVjaDMvdGVjaDMtbmF2aS1zLXVwaS1wYXltZW50cy1zdXJnZS0xMHgtaW4tMi1tb250aHMtaXQtbWFqb3JzLXRvLWpvaW4tZ292dC1zLXF1YW50dW0tbWlzc2lvbi1hbmQtbW9yZS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiZ2h0dHBzOi8vd3d3Lm1pbmluZy5jb20vc3BvbnNvcmVkLWNvbnRlbnQvbWlkbmlnaHQtc3VuLW1pbmluZy1wYXJ0bmVycy13aXRoLWtvYm9sZC1tZXRhbHMtZmlyc3QtcXVhbnR1bS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>Ripple Issues Urgent Warning on Quantum Computing's Threat to Blockchain Security</t>
+          <t>No Small Thing: The U.K.'s Other Quantum Startups</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>2024-06-14 14:00:59.922033</t>
+          <t>2024-06-14 16:03:03.144616</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMifWh0dHBzOi8vd3d3LmJpZ25ld3NuZXR3b3JrLmNvbS9uZXdzLzI3NDQxMDI2OS9yaXBwbGUtaXNzdWVzLXVyZ2VudC13YXJuaW5nLW9uLXF1YW50dW0tY29tcHV0aW5nLXRocmVhdC10by1ibG9ja2NoYWluLXNlY3VyaXR50gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMia2h0dHBzOi8vd3d3LmZvcmJlcy5jb20vc2l0ZXMvdHJldm9yY2xhd3Nvbi8yMDI0LzA2LzE0L25vLXNtYWxsLXRoaW5nLXF1YW50dW0tc3RhcnR1cHMtZm9yLXRoZS1oZXJlLWFuZC1ub3cv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>Govt to work with TCS, HCL, others for Rs 6,000 crore quantum tech scheme</t>
+          <t>Experimental observation of Earth's rotation with quantum entanglement</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>2024-06-14 14:00:59.922033</t>
+          <t>2024-06-14 16:03:03.144616</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMif2h0dHBzOi8vd3d3Lm1vbmV5Y29udHJvbC5jb20vdGVjaG5vbG9neS9nb3Z0LXRvLXdvcmstd2l0aC1pdC1tYWpvcnMtZm9yLXJzLTYwMDAtY3JvcmUtcXVhbnR1bS10ZWNoLXNjaGVtZS1hcnRpY2xlLTEyNzQ4NjEzLmh0bWzSAYMBaHR0cHM6Ly93d3cubW9uZXljb250cm9sLmNvbS90ZWNobm9sb2d5L2dvdnQtdG8td29yay13aXRoLWl0LW1ham9ycy1mb3ItcnMtNjAwMC1jcm9yZS1xdWFudHVtLXRlY2gtc2NoZW1lLWFydGljbGUtMTI3NDg2MTMuaHRtbC9hbXA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiMmh0dHBzOi8vd3d3LnNjaWVuY2Uub3JnL2RvaS8xMC4xMTI2L3NjaWFkdi5hZG8wMjE10gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>Fresh Insights On D-Wave Quantum Inc (QBTS)</t>
+          <t>Quantum computers are like kaleidoscopes − why unusual metaphors help illustrate science and technology</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>2024-06-14 14:00:59.924036</t>
+          <t>2024-06-14 16:03:03.145649</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiVGh0dHBzOi8vd3d3LnN0b2Nrc3JlZ2lzdGVyLmNvbS8yMDI0LzA2LzE0L2ZyZXNoLWluc2lnaHRzLW9uLWQtd2F2ZS1xdWFudHVtLWluYy1xYnRzL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiiAFodHRwczovL3RoZWNvbnZlcnNhdGlvbi5jb20vcXVhbnR1bS1jb21wdXRlcnMtYXJlLWxpa2Uta2FsZWlkb3Njb3Blcy13aHktdW51c3VhbC1tZXRhcGhvcnMtaGVscC1pbGx1c3RyYXRlLXNjaWVuY2UtYW5kLXRlY2hub2xvZ3ktMjI4MTc40gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>Investing in the Future: 3 Top Quantum Computing Stocks for Growth</t>
+          <t>Physicists measured Earth's rotation using quantum entanglement</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>2024-06-14 14:00:59.924036</t>
+          <t>2024-06-14 16:03:03.145649</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiYGh0dHBzOi8vd3d3LmZlYXR1cmV3ZWVrbHkuY29tL2ludmVzdGluZy1pbi10aGUtZnV0dXJlLTMtdG9wLXF1YW50dW0tY29tcHV0aW5nLXN0b2Nrcy1mb3ItZ3Jvd3RoL9IBZGh0dHBzOi8vd3d3LmZlYXR1cmV3ZWVrbHkuY29tL2ludmVzdGluZy1pbi10aGUtZnV0dXJlLTMtdG9wLXF1YW50dW0tY29tcHV0aW5nLXN0b2Nrcy1mb3ItZ3Jvd3RoL2FtcC8?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiR2h0dHBzOi8vd3d3LnNjaWVuY2VuZXdzLm9yZy9hcnRpY2xlL2VhcnRoLXJvdGF0aW9uLXF1YW50dW0tZW50YW5nbGVtZW500gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>Closing Bell: First Quantum Minerals Ltd up on Monday (FM)</t>
+          <t>How Classical AI is 'Saving' Quantum Computing: A Talk with IBM's Ismael Faro</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>2024-06-14 15:00:16.903297</t>
+          <t>2024-06-14 16:03:03.145649</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMijQFodHRwczovL3d3dy50aGVnbG9iZWFuZG1haWwuY29tL2ludmVzdGluZy9tYXJrZXRzL3N0b2Nrcy9GTS1UL3ByZXNzcmVsZWFzZXMvMjY3MzQ1MTkvY2xvc2luZy1iZWxsLWZpcnN0LXF1YW50dW0tbWluZXJhbHMtbHRkLXVwLW9uLW1vbmRheS1mbS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMic2h0dHBzOi8vdGhlcXVhbnR1bWluc2lkZXIuY29tLzIwMjQvMDYvMTQvaG93LWNsYXNzaWNhbC1haS1pcy1zYXZpbmctcXVhbnR1bS1jb21wdXRpbmctYS10YWxrLXdpdGgtaWJtcy1pc21hZWwtZmFyby_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>European quantum computing startup takes its funding to €32M with fresh raise</t>
+          <t>Quantum entangled photons react to Earth's spin</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>2024-06-14 15:00:16.912991</t>
+          <t>2024-06-14 16:03:03.145649</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiWmh0dHBzOi8vY2EubW92aWVzLnlhaG9vLmNvbS9tb3ZpZXMvZXVyb3BlYW4tcXVhbnR1bS1jb21wdXRpbmctc3RhcnR1cC10YWtlcy0xMjMyNTEzNTIuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiSGh0dHBzOi8vcGh5cy5vcmcvbmV3cy8yMDI0LTA2LXF1YW50dW0tZW50YW5nbGVkLXBob3RvbnMtcmVhY3QtZWFydGguaHRtbNIBR2h0dHBzOi8vcGh5cy5vcmcvbmV3cy8yMDI0LTA2LXF1YW50dW0tZW50YW5nbGVkLXBob3RvbnMtcmVhY3QtZWFydGguYW1w?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>Physicists confirm quantum entanglement persists between top quarks, the heaviest known fundamental particles</t>
+          <t>D-Wave (NYSE: QBTS) Extends Partnership with Aramco Research Center to Help Maximize Quantum’s Positive Impact</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>2024-06-14 15:23:50.050461</t>
+          <t>2024-06-14 16:03:03.145649</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiUmh0dHBzOi8vcGh5cy5vcmcvbmV3cy8yMDI0LTA2LXBoeXNpY2lzdHMtcXVhbnR1bS1lbnRhbmdsZW1lbnQtcGVyc2lzdHMtcXVhcmtzLmh0bWzSAVFodHRwczovL3BoeXMub3JnL25ld3MvMjAyNC0wNi1waHlzaWNpc3RzLXF1YW50dW0tZW50YW5nbGVtZW50LXBlcnNpc3RzLXF1YXJrcy5hbXA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiwgFodHRwczovL3d3dy50aGVnbG9iZWFuZG1haWwuY29tL2ludmVzdGluZy9tYXJrZXRzL3N0b2Nrcy9RQlRTLU4vcHJlc3NyZWxlYXNlcy8yNjgyOTk2My9kLXdhdmUtbnlzZS1xYnRzLWV4dGVuZHMtcGFydG5lcnNoaXAtd2l0aC1hcmFtY28tcmVzZWFyY2gtY2VudGVyLXRvLWhlbHAtbWF4aW1pemUtcXVhbnR1bXMtcG9zaXRpdmUtaW1wYWN0L9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>IQC celebrates latest Dean of Science Award winners | Institute for Quantum Computing</t>
+          <t>European quantum computing startup takes its funding to €32M with fresh raise</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>2024-06-14 15:23:50.050461</t>
+          <t>2024-06-14 16:03:03.146646</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiamh0dHBzOi8vdXdhdGVybG9vLmNhL2luc3RpdHV0ZS1mb3ItcXVhbnR1bS1jb21wdXRpbmcvbmV3cy9pcWMtY2VsZWJyYXRlcy1sYXRlc3QtZGVhbi1zY2llbmNlLWF3YXJkLXdpbm5lcnPSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiWmh0dHBzOi8vY2EubW92aWVzLnlhaG9vLmNvbS9tb3ZpZXMvZXVyb3BlYW4tcXVhbnR1bS1jb21wdXRpbmctc3RhcnR1cC10YWtlcy0xMjMyNTEzNTIuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>No Small Thing: The U.K.'s Other Quantum Startups</t>
+          <t>Unlocking the Future of Quantum Computing: Insights from Paul Terry, CEO of Photonic Inc.</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>2024-06-14 15:23:50.050461</t>
+          <t>2024-06-14 16:03:03.146646</t>
         </is>
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMia2h0dHBzOi8vd3d3LmZvcmJlcy5jb20vc2l0ZXMvdHJldm9yY2xhd3Nvbi8yMDI0LzA2LzE0L25vLXNtYWxsLXRoaW5nLXF1YW50dW0tc3RhcnR1cHMtZm9yLXRoZS1oZXJlLWFuZC1ub3cv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMigAFodHRwczovL3RoZXF1YW50dW1pbnNpZGVyLmNvbS8yMDI0LzA2LzE0L3VubG9ja2luZy10aGUtZnV0dXJlLW9mLXF1YW50dW0tY29tcHV0aW5nLWluc2lnaHRzLWZyb20tcGF1bC10ZXJyeS1jZW8tb2YtcGhvdG9uaWMtaW5jL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>Experimental observation of Earth's rotation with quantum entanglement</t>
+          <t>When quantum dots meet blue phase liquid crystal elastomers</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>2024-06-14 15:23:50.050461</t>
+          <t>2024-06-14 16:03:03.146646</t>
         </is>
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiMmh0dHBzOi8vd3d3LnNjaWVuY2Uub3JnL2RvaS8xMC4xMTI2L3NjaWFkdi5hZG8wMjE10gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiQWh0dHBzOi8vcGh5cy5vcmcvbmV3cy8yMDI0LTA2LXF1YW50dW0tZG90cy1ibHVlLXBoYXNlLWxpcXVpZC5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>When quantum dots meet blue phase liquid crystal elastomers</t>
+          <t>Physicists Measure Earth’s Rotation Using Quantum Entanglement</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>2024-06-14 15:23:50.050461</t>
+          <t>2024-06-14 16:03:03.146646</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiQWh0dHBzOi8vcGh5cy5vcmcvbmV3cy8yMDI0LTA2LXF1YW50dW0tZG90cy1ibHVlLXBoYXNlLWxpcXVpZC5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiWGh0dHBzOi8vd3d3LnNjaS5uZXdzL3BoeXNpY3MvZWFydGhzLXJvdGF0aW9uLXF1YW50dW0tZW50YW5nbGVtZW50LW1lYXN1cmVtZW50LTEzMDIwLmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>D-Wave (NYSE: QBTS) Extends Partnership with Aramco Research Center to Help Maximize Quantum’s Positive Impact</t>
+          <t>Purified Silicon Makes Bigger, Faster Quantum Computers</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>2024-06-14 15:23:50.050461</t>
+          <t>2024-06-14 16:03:03.147645</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiwgFodHRwczovL3d3dy50aGVnbG9iZWFuZG1haWwuY29tL2ludmVzdGluZy9tYXJrZXRzL3N0b2Nrcy9RQlRTLU4vcHJlc3NyZWxlYXNlcy8yNjgyOTk2My9kLXdhdmUtbnlzZS1xYnRzLWV4dGVuZHMtcGFydG5lcnNoaXAtd2l0aC1hcmFtY28tcmVzZWFyY2gtY2VudGVyLXRvLWhlbHAtbWF4aW1pemUtcXVhbnR1bXMtcG9zaXRpdmUtaW1wYWN0L9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiP2h0dHBzOi8vc3BlY3RydW0uaWVlZS5vcmcvc2lsaWNvbi1xdWFudHVtLWNvbXB1dGluZy1wdXJpZmllZC1zadIBTmh0dHBzOi8vc3BlY3RydW0uaWVlZS5vcmcvYW1wL3NpbGljb24tcXVhbnR1bS1jb21wdXRpbmctcHVyaWZpZWQtc2ktMjY2ODQ4NzY3Mw?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>Midnight Sun Mining partners with KoBold Metals; First Quantum - MINING.COM</t>
+          <t>SpaceX launches 'zero fuel' engine into space</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>2024-06-14 15:23:50.050461</t>
+          <t>2024-06-14 16:03:03.147645</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiZ2h0dHBzOi8vd3d3Lm1pbmluZy5jb20vc3BvbnNvcmVkLWNvbnRlbnQvbWlkbmlnaHQtc3VuLW1pbmluZy1wYXJ0bmVycy13aXRoLWtvYm9sZC1tZXRhbHMtZmlyc3QtcXVhbnR1bS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiT2h0dHBzOi8vY2Euc3R5bGUueWFob28uY29tL25ld3Mvc3BhY2V4LWxhdW5jaGVzLXplcm8tZnVlbC1lbmdpbmUtMTQ1NDAzODYyLmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>Quantum computers are like kaleidoscopes − why unusual metaphors help illustrate science and technology</t>
+          <t>Innovation Lightbulb: Private Investment in Quantum Technology</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>2024-06-14 15:23:50.050461</t>
+          <t>2024-06-14 16:03:03.147645</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiiAFodHRwczovL3RoZWNvbnZlcnNhdGlvbi5jb20vcXVhbnR1bS1jb21wdXRlcnMtYXJlLWxpa2Uta2FsZWlkb3Njb3Blcy13aHktdW51c3VhbC1tZXRhcGhvcnMtaGVscC1pbGx1c3RyYXRlLXNjaWVuY2UtYW5kLXRlY2hub2xvZ3ktMjI4MTc40gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiWGh0dHBzOi8vd3d3LmNzaXMub3JnL2FuYWx5c2lzL2lubm92YXRpb24tbGlnaHRidWxiLXByaXZhdGUtaW52ZXN0bWVudC1xdWFudHVtLXRlY2hub2xvZ3nSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>Purified Silicon Makes Bigger, Faster Quantum Computers</t>
+          <t>First Quantum Minerals Ltd. stock rises Friday, outperforms market</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>2024-06-14 15:23:50.050461</t>
+          <t>2024-06-14 16:03:03.148645</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiP2h0dHBzOi8vc3BlY3RydW0uaWVlZS5vcmcvc2lsaWNvbi1xdWFudHVtLWNvbXB1dGluZy1wdXJpZmllZC1zadIBTmh0dHBzOi8vc3BlY3RydW0uaWVlZS5vcmcvYW1wL3NpbGljb24tcXVhbnR1bS1jb21wdXRpbmctcHVyaWZpZWQtc2ktMjY2ODQ4NzY3Mw?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMijgFodHRwczovL3d3dy5tYXJrZXR3YXRjaC5jb20vZGF0YS1uZXdzL2ZpcnN0LXF1YW50dW0tbWluZXJhbHMtbHRkLXN0b2NrLXJpc2VzLWZyaWRheS1vdXRwZXJmb3Jtcy1tYXJrZXQtNDIwMWM3NGEtZTk4OTFkYjhlNTBjP21vZD1td19xdW90ZV9uZXdz0gGAAWh0dHBzOi8vd3d3Lm1hcmtldHdhdGNoLmNvbS9hbXAvZGF0YS1uZXdzL2ZpcnN0LXF1YW50dW0tbWluZXJhbHMtbHRkLXN0b2NrLXJpc2VzLWZyaWRheS1vdXRwZXJmb3Jtcy1tYXJrZXQtNDIwMWM3NGEtZTk4OTFkYjhlNTBj?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>Physicists measured Earth's rotation using quantum entanglement</t>
+          <t>A portable quantum simulator on a silicon chip</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>2024-06-14 15:23:50.050461</t>
+          <t>2024-06-14 16:03:03.149646</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiR2h0dHBzOi8vd3d3LnNjaWVuY2VuZXdzLm9yZy9hcnRpY2xlL2VhcnRoLXJvdGF0aW9uLXF1YW50dW0tZW50YW5nbGVtZW500gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiY2h0dHBzOi8vd3d3Lm9wZW5hY2Nlc3Nnb3Zlcm5tZW50Lm9yZy9hcnRpY2xlL2EtcG9ydGFibGUtcXVhbnR1bS1zaW11bGF0b3Itb24tYS1zaWxpY29uLWNoaXAvMTc4MTYxL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>Unlocking the Future of Quantum Computing: Insights from Paul Terry, CEO of Photonic Inc.</t>
+          <t>Scott Bakula Addresses 'Quantum Leap' Reboot Involvement Speculation, Says It Was “Very Difficult Decision” To Pass ...</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>2024-06-14 15:23:50.050461</t>
+          <t>2024-06-14 16:03:03.150645</t>
         </is>
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMigAFodHRwczovL3RoZXF1YW50dW1pbnNpZGVyLmNvbS8yMDI0LzA2LzE0L3VubG9ja2luZy10aGUtZnV0dXJlLW9mLXF1YW50dW0tY29tcHV0aW5nLWluc2lnaHRzLWZyb20tcGF1bC10ZXJyeS1jZW8tb2YtcGhvdG9uaWMtaW5jL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiTmh0dHBzOi8vY2EubW92aWVzLnlhaG9vLmNvbS9zY290dC1iYWt1bGEtYWRkcmVzc2VzLXF1YW50dW0tbGVhcC0yMjA5NDUzNzMuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>Quantum entangled photons react to Earth's spin</t>
+          <t>The Growing Interest in On-Prem Quantum Computing - High-Performance Computing News Analysis</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>2024-06-14 15:23:50.050461</t>
+          <t>2024-06-14 16:03:03.150645</t>
         </is>
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiSGh0dHBzOi8vcGh5cy5vcmcvbmV3cy8yMDI0LTA2LXF1YW50dW0tZW50YW5nbGVkLXBob3RvbnMtcmVhY3QtZWFydGguaHRtbNIBR2h0dHBzOi8vcGh5cy5vcmcvbmV3cy8yMDI0LTA2LXF1YW50dW0tZW50YW5nbGVkLXBob3RvbnMtcmVhY3QtZWFydGguYW1w?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiUGh0dHBzOi8vaW5zaWRlaHBjLmNvbS8yMDI0LzA2L3RoZS1ncm93aW5nLWludGVyZXN0LWluLW9uLXByZW0tcXVhbnR1bS1jb21wdXRpbmcv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>Physicists Measure Earth’s Rotation Using Quantum Entanglement</t>
+          <t>Many-excitation removal of a transmon qubit using a single-junction quantum-circuit refrigerator and a two-tone ...</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>2024-06-14 15:23:50.050461</t>
+          <t>2024-06-14 16:03:03.150645</t>
         </is>
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiWGh0dHBzOi8vd3d3LnNjaS5uZXdzL3BoeXNpY3MvZWFydGhzLXJvdGF0aW9uLXF1YW50dW0tZW50YW5nbGVtZW50LW1lYXN1cmVtZW50LTEzMDIwLmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiMmh0dHBzOi8vd3d3Lm5hdHVyZS5jb20vYXJ0aWNsZXMvczQxNTk4LTAyNC02NDQ5Ni010gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>How Classical AI is 'Saving' Quantum Computing: A Talk with IBM's Ismael Faro</t>
+          <t>Quantum technologies take off!</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>2024-06-14 15:23:50.050461</t>
+          <t>2024-06-14 16:03:03.151646</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMic2h0dHBzOi8vdGhlcXVhbnR1bWluc2lkZXIuY29tLzIwMjQvMDYvMTQvaG93LWNsYXNzaWNhbC1haS1pcy1zYXZpbmctcXVhbnR1bS1jb21wdXRpbmctYS10YWxrLXdpdGgtaWJtcy1pc21hZWwtZmFyby_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiVmh0dHBzOi8vd3d3Lmxhc2VyZm9jdXN3b3JsZC5jb20vcXVhbnR1bS9hcnRpY2xlLzU1MDg4MzY2L3F1YW50dW0tdGVjaG5vbG9naWVzLXRha2Utb2Zm0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>Innovation Lightbulb: Private Investment in Quantum Technology</t>
+          <t>Earth's rotation measured 1000x better with quantum entanglement</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>2024-06-14 15:23:50.050461</t>
+          <t>2024-06-14 16:03:03.152646</t>
         </is>
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiWGh0dHBzOi8vd3d3LmNzaXMub3JnL2FuYWx5c2lzL2lubm92YXRpb24tbGlnaHRidWxiLXByaXZhdGUtaW52ZXN0bWVudC1xdWFudHVtLXRlY2hub2xvZ3nSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiVmh0dHBzOi8vaW50ZXJlc3RpbmdlbmdpbmVlcmluZy5jb20vc2NpZW5jZS9xdWFudHVtLWVudGFuZ2xlbWVudC1tZWFzdXJlLWVhcnRoLXJvdGF0aW9u0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>First Quantum Minerals Ltd. stock rises Friday, outperforms market</t>
+          <t>Quantum Computing Revolutionizes Data Assimilation</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>2024-06-14 15:23:50.060507</t>
+          <t>2024-06-14 16:03:03.152646</t>
         </is>
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMijgFodHRwczovL3d3dy5tYXJrZXR3YXRjaC5jb20vZGF0YS1uZXdzL2ZpcnN0LXF1YW50dW0tbWluZXJhbHMtbHRkLXN0b2NrLXJpc2VzLWZyaWRheS1vdXRwZXJmb3Jtcy1tYXJrZXQtNDIwMWM3NGEtZTk4OTFkYjhlNTBjP21vZD1td19xdW90ZV9uZXdz0gGAAWh0dHBzOi8vd3d3Lm1hcmtldHdhdGNoLmNvbS9hbXAvZGF0YS1uZXdzL2ZpcnN0LXF1YW50dW0tbWluZXJhbHMtbHRkLXN0b2NrLXJpc2VzLWZyaWRheS1vdXRwZXJmb3Jtcy1tYXJrZXQtNDIwMWM3NGEtZTk4OTFkYjhlNTBj?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiMWh0dHBzOi8vd3d3LmF6b3F1YW50dW0uY29tL05ld3MuYXNweD9uZXdzSUQ9MTAzMjHSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>A portable quantum simulator on a silicon chip</t>
+          <t>Programmable Approach to Fabricating Optical Qubits in Silicon Could Lead to Large-scale Manufacturing</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>2024-06-14 15:23:50.062710</t>
+          <t>2024-06-14 16:03:03.152646</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiY2h0dHBzOi8vd3d3Lm9wZW5hY2Nlc3Nnb3Zlcm5tZW50Lm9yZy9hcnRpY2xlL2EtcG9ydGFibGUtcXVhbnR1bS1zaW11bGF0b3Itb24tYS1zaWxpY29uLWNoaXAvMTc4MTYxL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMikAFodHRwczovL3RoZXF1YW50dW1pbnNpZGVyLmNvbS8yMDI0LzA2LzE0L3Byb2dyYW1tYWJsZS1hcHByb2FjaC10by1mYWJyaWNhdGluZy1vcHRpY2FsLXF1Yml0cy1pbi1zaWxpY29uLWNvdWxkLWxlYWQtdG8tbGFyZ2Utc2NhbGUtbWFudWZhY3R1cmluZy_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>Many-excitation removal of a transmon qubit using a single-junction quantum-circuit refrigerator and a two-tone ...</t>
+          <t>Quantum Computing and AI: A Perfect Match?</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>2024-06-14 15:23:50.062710</t>
+          <t>2024-06-14 16:03:03.152646</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiMmh0dHBzOi8vd3d3Lm5hdHVyZS5jb20vYXJ0aWNsZXMvczQxNTk4LTAyNC02NDQ5Ni010gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiXWh0dHBzOi8vd3d3LmluZm9ybWF0aW9ud2Vlay5jb20vbWFjaGluZS1sZWFybmluZy1haS9xdWFudHVtLWNvbXB1dGluZy1hbmQtYWktYS1wZXJmZWN0LW1hdGNoLdIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>The Growing Interest in On-Prem Quantum Computing - High-Performance Computing News Analysis</t>
+          <t>Quantum Computing Inc. Releases Preliminary Financial Results for Q1 2024</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>2024-06-14 15:23:50.063739</t>
+          <t>2024-06-14 16:03:03.152646</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiUGh0dHBzOi8vaW5zaWRlaHBjLmNvbS8yMDI0LzA2L3RoZS1ncm93aW5nLWludGVyZXN0LWluLW9uLXByZW0tcXVhbnR1bS1jb21wdXRpbmcv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMia2h0dHBzOi8vcXVhbnR1bWNvbXB1dGluZ3JlcG9ydC5jb20vcXVhbnR1bS1jb21wdXRpbmctaW5jLXJlbGVhc2UtcHJlbGltaW5hcnktZmluYW5jaWFsLXJlc3VsdHMtZm9yLXExLTIwMjQv0gFvaHR0cHM6Ly9xdWFudHVtY29tcHV0aW5ncmVwb3J0LmNvbS9xdWFudHVtLWNvbXB1dGluZy1pbmMtcmVsZWFzZS1wcmVsaW1pbmFyeS1maW5hbmNpYWwtcmVzdWx0cy1mb3ItcTEtMjAyNC9hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>Quantum technologies take off!</t>
+          <t>'Escape From Shadow Physics' Review: Quantum Weirdness</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>2024-06-14 15:23:50.065731</t>
+          <t>2024-06-14 16:03:03.154258</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiVmh0dHBzOi8vd3d3Lmxhc2VyZm9jdXN3b3JsZC5jb20vcXVhbnR1bS9hcnRpY2xlLzU1MDg4MzY2L3F1YW50dW0tdGVjaG5vbG9naWVzLXRha2Utb2Zm0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiaWh0dHBzOi8vd3d3Lm1zbi5jb20vZW4tdXMvbmV3cy90ZWNobm9sb2d5L2VzY2FwZS1mcm9tLXNoYWRvdy1waHlzaWNzLXJldmlldy1xdWFudHVtLXdlaXJkbmVzcy9hci1CQjFvZU5wUNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>Quantum Computing Inc. Releases Preliminary Financial Results for Q1 2024</t>
+          <t>When quantum dots meet blue phase liquid crystal elastomers: visualized full-color and mechanically-switchable ...</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>2024-06-14 15:23:50.066730</t>
+          <t>2024-06-14 16:03:03.154258</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMia2h0dHBzOi8vcXVhbnR1bWNvbXB1dGluZ3JlcG9ydC5jb20vcXVhbnR1bS1jb21wdXRpbmctaW5jLXJlbGVhc2UtcHJlbGltaW5hcnktZmluYW5jaWFsLXJlc3VsdHMtZm9yLXExLTIwMjQv0gFvaHR0cHM6Ly9xdWFudHVtY29tcHV0aW5ncmVwb3J0LmNvbS9xdWFudHVtLWNvbXB1dGluZy1pbmMtcmVsZWFzZS1wcmVsaW1pbmFyeS1maW5hbmNpYWwtcmVzdWx0cy1mb3ItcTEtMjAyNC9hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiMmh0dHBzOi8vd3d3Lm5hdHVyZS5jb20vYXJ0aWNsZXMvczQxMzc3LTAyNC0wMTQ3OS0x0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>Quantum Computing and AI: A Perfect Match?</t>
+          <t>Soon, QDEL Screens Could Perfect What OLED Couldn't</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>2024-06-14 15:23:50.066730</t>
+          <t>2024-06-14 16:03:03.155183</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiXWh0dHBzOi8vd3d3LmluZm9ybWF0aW9ud2Vlay5jb20vbWFjaGluZS1sZWFybmluZy1haS9xdWFudHVtLWNvbXB1dGluZy1hbmQtYWktYS1wZXJmZWN0LW1hdGNoLdIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiTGh0dHBzOi8vd3d3Lmhvd3RvZ2Vlay5jb20vc29vbi1xZGVsLXNjcmVlbnMtY291bGQtcGVyZmVjdC13aGF0LW9sZWQtY291bGRudC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>Quantum Computing Revolutionizes Data Assimilation</t>
+          <t>Quantum Defies Fossil Fuel Flight with $5.8B Target</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>2024-06-14 15:23:50.067730</t>
+          <t>2024-06-14 16:03:03.155183</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiMWh0dHBzOi8vd3d3LmF6b3F1YW50dW0uY29tL05ld3MuYXNweD9uZXdzSUQ9MTAzMjHSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiYGh0dHBzOi8vd3d3LnRoZW1pZGRsZW1hcmtldC5jb20vbmV3cy1hbmFseXNpcy9xdWFudHVtLWRlZmllcy1mb3NzaWwtZnVlbC1mbGlnaHQtd2l0aC01LThiLXRhcmdldNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>Earth's rotation measured 1000x better with quantum entanglement</t>
+          <t>New Dimensions in Quantum Computing: Majorana Particles Go 2D</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>2024-06-14 15:23:50.067730</t>
+          <t>2024-06-14 16:03:03.156182</t>
         </is>
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiVmh0dHBzOi8vaW50ZXJlc3RpbmdlbmdpbmVlcmluZy5jb20vc2NpZW5jZS9xdWFudHVtLWVudGFuZ2xlbWVudC1tZWFzdXJlLWVhcnRoLXJvdGF0aW9u0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiVmh0dHBzOi8vc2NpdGVjaGRhaWx5LmNvbS9uZXctZGltZW5zaW9ucy1pbi1xdWFudHVtLWNvbXB1dGluZy1tYWpvcmFuYS1wYXJ0aWNsZXMtZ28tMmQv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>Programmable Approach to Fabricating Optical Qubits in Silicon Could Lead to Large-scale Manufacturing</t>
+          <t>Femtosecond Lasers Spearhead the Quantum Computing Revolution</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>2024-06-14 15:23:50.067730</t>
+          <t>2024-06-14 16:03:03.157180</t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMikAFodHRwczovL3RoZXF1YW50dW1pbnNpZGVyLmNvbS8yMDI0LzA2LzE0L3Byb2dyYW1tYWJsZS1hcHByb2FjaC10by1mYWJyaWNhdGluZy1vcHRpY2FsLXF1Yml0cy1pbi1zaWxpY29uLWNvdWxkLWxlYWQtdG8tbGFyZ2Utc2NhbGUtbWFudWZhY3R1cmluZy_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiV2h0dHBzOi8vc2NpdGVjaGRhaWx5LmNvbS9mZW10b3NlY29uZC1sYXNlcnMtc3BlYXJoZWFkLXRoZS1xdWFudHVtLWNvbXB1dGluZy1yZXZvbHV0aW9uL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>'Escape From Shadow Physics' Review: Quantum Weirdness</t>
+          <t>Diraq is going to make a hybrid chip combining quantum and classical processors</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>2024-06-14 15:23:50.068730</t>
+          <t>2024-06-14 16:03:03.158181</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiaWh0dHBzOi8vd3d3Lm1zbi5jb20vZW4tdXMvbmV3cy90ZWNobm9sb2d5L2VzY2FwZS1mcm9tLXNoYWRvdy1waHlzaWNzLXJldmlldy1xdWFudHVtLXdlaXJkbmVzcy9hci1CQjFvZU5wUNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMihQFodHRwczovL3d3dy5zdGFydHVwZGFpbHkubmV0L3RvcGljL3F1YW50dW0tY29tcHV0aW5nL2RpcmFxLWlzLWdvaW5nLXRvLW1ha2UtYS1oeWJyaWQtY2hpcC1jb21iaW5pbmctcXVhbnR1bS1hbmQtY2xhc3NpY2FsLXByb2Nlc3NvcnMv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>When quantum dots meet blue phase liquid crystal elastomers: visualized full-color and mechanically-switchable ...</t>
+          <t>Lantronix Wins 2024 IoT Evolution Asset Tracking Award for FOX3 Telematic Gateway</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>2024-06-14 15:23:50.068730</t>
+          <t>2024-06-14 16:03:03.158181</t>
         </is>
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiMmh0dHBzOi8vd3d3Lm5hdHVyZS5jb20vYXJ0aWNsZXMvczQxMzc3LTAyNC0wMTQ3OS0x0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMinAFodHRwczovL3d3dy5nbG9iZW5ld3N3aXJlLmNvbS9lbi9uZXdzLXJlbGVhc2UvMjAyNC8wNi8xMy8yODk4MTQ0LzAvZW4vTGFudHJvbml4LVdpbnMtMjAyNC1Jb1QtRXZvbHV0aW9uLUFzc2V0LVRyYWNraW5nLUF3YXJkLWZvci1GT1gzLVRlbGVtYXRpYy1HYXRld2F5Lmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>Quantum Defies Fossil Fuel Flight with $5.8B Target</t>
+          <t>Bizarre device uses 'blind quantum computing' to let you access quantum computers from home</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>2024-06-14 15:23:50.070288</t>
+          <t>2024-06-14 16:03:03.158181</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiYGh0dHBzOi8vd3d3LnRoZW1pZGRsZW1hcmtldC5jb20vbmV3cy1hbmFseXNpcy9xdWFudHVtLWRlZmllcy1mb3NzaWwtZnVlbC1mbGlnaHQtd2l0aC01LThiLXRhcmdldNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMirQFodHRwczovL3d3dy5tc24uY29tL2VuLXVzL25ld3MvdGVjaG5vbG9neS9iaXphcnJlLWRldmljZS11c2VzLWJsaW5kLXF1YW50dW0tY29tcHV0aW5nLXRvLWxldC15b3UtYWNjZXNzLXF1YW50dW0tY29tcHV0ZXJzLWZyb20taG9tZS9hci1CQjFtekNwNT9pdGVtPWZsaWdodHNwcmctdGlwc3Vic2MtdjFhL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>Earth's rotation is measured using quantum entanglement | Globe Echo</t>
+          <t>D-Wave quantum director Emil Michael sells over $27 million in warrants</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>2024-06-15 14:00:59.924683</t>
+          <t>2024-06-14 16:03:03.159180</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiTWh0dHBzOi8vZ2xvYmVlY2hvLmNvbS9lYXJ0aHMtcm90YXRpb24taXMtbWVhc3VyZWQtdXNpbmctcXVhbnR1bS1lbnRhbmdsZW1lbnQv0gFRaHR0cHM6Ly9nbG9iZWVjaG8uY29tL2VhcnRocy1yb3RhdGlvbi1pcy1tZWFzdXJlZC11c2luZy1xdWFudHVtLWVudGFuZ2xlbWVudC9hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMifWh0dHBzOi8vaW4uaW52ZXN0aW5nLmNvbS9uZXdzL2NvbXBhbnktbmV3cy9kd2F2ZS1xdWFudHVtLWRpcmVjdG9yLWVtaWwtbWljaGFlbC1zZWxscy1vdmVyLTI3LW1pbGxpb24taW4td2FycmFudHMtOTNDSC00MjU1MTI00gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>There's a way to lessen your chances of getting booted from an overbooked cruise: pay more</t>
+          <t>Earth's rotation is measured using quantum entanglement | Globe Echo</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>2024-06-15 14:05:28.346308</t>
+          <t>2024-06-15 14:00:59.924683</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiSmh0dHBzOi8vc2cubmV3cy55YWhvby5jb20vdGhlcmVzLXdheS1sZXNzZW4tY2hhbmNlcy1nZXR0aW5nLTEwMDAwMTkwMy5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiTWh0dHBzOi8vZ2xvYmVlY2hvLmNvbS9lYXJ0aHMtcm90YXRpb24taXMtbWVhc3VyZWQtdXNpbmctcXVhbnR1bS1lbnRhbmdsZW1lbnQv0gFRaHR0cHM6Ly9nbG9iZWVjaG8uY29tL2VhcnRocy1yb3RhdGlvbi1pcy1tZWFzdXJlZC11c2luZy1xdWFudHVtLWVudGFuZ2xlbWVudC9hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>“India has produced over 40 Quantum Technology start-ups in 2 years, few of them with global potential,” says Dr ...</t>
+          <t>There's a way to lessen your chances of getting booted from an overbooked cruise: pay more</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>2024-06-15 14:51:30.298139</t>
+          <t>2024-06-15 14:05:28.346308</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiO2h0dHBzOi8vcGliLmdvdi5pbi9QcmVzc1JlbGVhc2VJZnJhbWVQYWdlLmFzcHg_UFJJRD0yMDI1NTY00gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiSmh0dHBzOi8vc2cubmV3cy55YWhvby5jb20vdGhlcmVzLXdheS1sZXNzZW4tY2hhbmNlcy1nZXR0aW5nLTEwMDAwMTkwMy5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
@@ -4397,7 +4397,7 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>Guest Post — The Road to the Proclamation of IYQ2025</t>
+          <t>HDK questions ₹3.2 crore subsidy to chip manufacturer by Gujarat govt, then backtracks</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
@@ -4407,14 +4407,14 @@
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiXGh0dHBzOi8vdGhlcXVhbnR1bWluc2lkZXIuY29tLzIwMjQvMDYvMTUvZ3Vlc3QtcG9zdC10aGUtcm9hZC10by10aGUtcHJvY2xhbWF0aW9uLW9mLWl5cTIwMjUv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMisgFodHRwczovL3d3dy50aGVoaW5kdS5jb20vYnVzaW5lc3MvdW5pb24tbWluaXN0ZXItaGQta3VtYXJhc3dhbXktcmV0cmFjdHMtc3RhdGVtZW50LW9uLXNlbWljb25kdWN0b3ItdW5pdC1pbi1ndWphcmF0LWEtZGF5LWFmdGVyLXF1ZXN0aW9uaW5nLXF1YW50dW0tb2Ytc3Vic2lkeS9hcnRpY2xlNjgyOTI3NTUuZWNl0gG3AWh0dHBzOi8vd3d3LnRoZWhpbmR1LmNvbS9idXNpbmVzcy91bmlvbi1taW5pc3Rlci1oZC1rdW1hcmFzd2FteS1yZXRyYWN0cy1zdGF0ZW1lbnQtb24tc2VtaWNvbmR1Y3Rvci11bml0LWluLWd1amFyYXQtYS1kYXktYWZ0ZXItcXVlc3Rpb25pbmctcXVhbnR1bS1vZi1zdWJzaWR5L2FydGljbGU2ODI5Mjc1NS5lY2UvYW1wLw?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>Modi 3.0 to team up with TCS, HCL and other IT giants – Know why</t>
+          <t>A liquid crystal source of photon pairs</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
@@ -4424,14 +4424,14 @@
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMie2h0dHBzOi8vd3d3Lm1zbi5jb20vZW4taW4vbGlmZXN0eWxlL3JlbGF0aW9uc2hpcHMvbW9kaS0zLTAtdG8tdGVhbS11cC13aXRoLXRjcy1oY2wtYW5kLW90aGVyLWl0LWdpYW50cy1rbm93LXdoeS9hci1CQjFvZ1lFb9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiMGh0dHBzOi8vd3d3LmV1cmVrYWxlcnQub3JnL25ld3MtcmVsZWFzZXMvMTA0ODMwMtIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>Gemma Arterton Says She Gets 'Criticism' for Quantum of Solace : There's 'So Much Wrong with Bond Women'</t>
+          <t>Scientists Create Multi-Node Entanglement in Metropolitan Quantum Network</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
@@ -4441,14 +4441,14 @@
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiR2h0dHBzOi8vdWsubW92aWVzLnlhaG9vLmNvbS9nZW1tYS1hcnRlcnRvbi1zYXlzLXNoZS1nZXRzLTE2MTkzMDYzNy5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiZWh0dHBzOi8vYW5hLmlyL2VuL25ld3MvNjIyMy9zY2llbnRpc3RzLWNyZWF0ZS1tdWx0aS1ub2RlLWVudGFuZ2xlbWVudC1pbi1tZXRyb3BvbGl0YW4tcXVhbnR1bS1uZXR3b3Jr0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>Quantum Encryption &amp; the Rise of Cybersecuritys Superhero ‍♂️ | Tech News with Comed-AI-n</t>
+          <t>Guest Post — The Road to the Proclamation of IYQ2025</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
@@ -4458,14 +4458,14 @@
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMirwFodHRwczovL21lZGl1bS5jb20vQENvbWVkX0FJX24vcXVhbnR1bS1lbmNyeXB0aW9uLXRoZS1yaXNlLW9mLWN5YmVyc2VjdXJpdHlzLXN1cGVyaGVyby0lRUYlQjglOEYtdGVjaC1uZXdzLXdpdGgtY29tZWQtYWktbi01ZTUxODc1YzRmYzA_cmVzcG9uc2VzT3Blbj10cnVlJnNvcnRCeT1SRVZFUlNFX0NIUk9O0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiXGh0dHBzOi8vdGhlcXVhbnR1bWluc2lkZXIuY29tLzIwMjQvMDYvMTUvZ3Vlc3QtcG9zdC10aGUtcm9hZC10by10aGUtcHJvY2xhbWF0aW9uLW9mLWl5cTIwMjUv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>Quantum Technology Flourishes in India with 40 New Startups in Two Years</t>
+          <t>“India has produced over 40 Quantum Technology start-ups in 2 years, few of them with global potential,” says Dr ...</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
@@ -4475,7 +4475,7 @@
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiZWh0dHBzOi8vd3d3LnRlY2hpZXhwZXJ0LmNvbS9xdWFudHVtLXRlY2hub2xvZ3ktZmxvdXJpc2hlcy1pbi1pbmRpYS13aXRoLTQwLW5ldy1zdGFydHVwcy1pbi10d28teWVhcnMv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiO2h0dHBzOi8vcGliLmdvdi5pbi9QcmVzc1JlbGVhc2VJZnJhbWVQYWdlLmFzcHg_UFJJRD0yMDI1NTY00gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
@@ -4499,7 +4499,7 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>Scientists Create Multi-Node Entanglement in Metropolitan Quantum Network</t>
+          <t>Quantum Technology Flourishes in India with 40 New Startups in Two Years</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
@@ -4509,14 +4509,14 @@
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiZWh0dHBzOi8vYW5hLmlyL2VuL25ld3MvNjIyMy9zY2llbnRpc3RzLWNyZWF0ZS1tdWx0aS1ub2RlLWVudGFuZ2xlbWVudC1pbi1tZXRyb3BvbGl0YW4tcXVhbnR1bS1uZXR3b3Jr0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiZWh0dHBzOi8vd3d3LnRlY2hpZXhwZXJ0LmNvbS9xdWFudHVtLXRlY2hub2xvZ3ktZmxvdXJpc2hlcy1pbi1pbmRpYS13aXRoLTQwLW5ldy1zdGFydHVwcy1pbi10d28teWVhcnMv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>A liquid crystal source of photon pairs</t>
+          <t>Modi 3.0 to team up with TCS, HCL and other IT giants – Know why</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -4526,48 +4526,48 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiMGh0dHBzOi8vd3d3LmV1cmVrYWxlcnQub3JnL25ld3MtcmVsZWFzZXMvMTA0ODMwMtIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMie2h0dHBzOi8vd3d3Lm1zbi5jb20vZW4taW4vbGlmZXN0eWxlL3JlbGF0aW9uc2hpcHMvbW9kaS0zLTAtdG8tdGVhbS11cC13aXRoLXRjcy1oY2wtYW5kLW90aGVyLWl0LWdpYW50cy1rbm93LXdoeS9hci1CQjFvZ1lFb9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>HDK questions ₹3.2 crore subsidy to chip manufacturer by Gujarat govt, then backtracks</t>
+          <t>Generating photon pairs from a liquid crystal source | Globe Echo</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>2024-06-15 14:51:30.298139</t>
+          <t>2024-06-15 14:51:30.303962</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMisgFodHRwczovL3d3dy50aGVoaW5kdS5jb20vYnVzaW5lc3MvdW5pb24tbWluaXN0ZXItaGQta3VtYXJhc3dhbXktcmV0cmFjdHMtc3RhdGVtZW50LW9uLXNlbWljb25kdWN0b3ItdW5pdC1pbi1ndWphcmF0LWEtZGF5LWFmdGVyLXF1ZXN0aW9uaW5nLXF1YW50dW0tb2Ytc3Vic2lkeS9hcnRpY2xlNjgyOTI3NTUuZWNl0gG3AWh0dHBzOi8vd3d3LnRoZWhpbmR1LmNvbS9idXNpbmVzcy91bmlvbi1taW5pc3Rlci1oZC1rdW1hcmFzd2FteS1yZXRyYWN0cy1zdGF0ZW1lbnQtb24tc2VtaWNvbmR1Y3Rvci11bml0LWluLWd1amFyYXQtYS1kYXktYWZ0ZXItcXVlc3Rpb25pbmctcXVhbnR1bS1vZi1zdWJzaWR5L2FydGljbGU2ODI5Mjc1NS5lY2UvYW1wLw?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiS2h0dHBzOi8vZ2xvYmVlY2hvLmNvbS9nZW5lcmF0aW5nLXBob3Rvbi1wYWlycy1mcm9tLWEtbGlxdWlkLWNyeXN0YWwtc291cmNlL9IBT2h0dHBzOi8vZ2xvYmVlY2hvLmNvbS9nZW5lcmF0aW5nLXBob3Rvbi1wYWlycy1mcm9tLWEtbGlxdWlkLWNyeXN0YWwtc291cmNlL2FtcC8?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>Quantum entanglement measures Earth's spin with never-before-seen accuracy</t>
+          <t>India Has Produced Over 40 Quantum Technology Start-Ups In Two Years: Union Minister Dr. Jitendra Singh |</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>2024-06-15 14:51:30.298139</t>
+          <t>2024-06-15 14:51:30.303962</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMingFodHRwczovL3d3dy5tc24uY29tL2VuLXVzL25ld3MvdGVjaG5vbG9neS9xdWFudHVtLWVudGFuZ2xlbWVudC1tZWFzdXJlcy1lYXJ0aC1zLXNwaW4td2l0aC1uZXZlci1iZWZvcmUtc2Vlbi1hY2N1cmFjeS9hci1CQjFvZjZWZj9pdGVtPWZsaWdodHNwcmctdGlwc3Vic2MtdjFhL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMimQFodHRwczovL3d3dy5qYWlzYWxtZXJuZXdzLmNvbS9uZXdzL25hdGlvbmFsL2luZGlhLWhhcy1wcm9kdWNlZC1vdmVyLTQwLXF1YW50dW0tdGVjaG5vbG9neS1zdGFydC11cHMtaW4tdHdvLXllYXJzLXVuaW9uLW1pbmlzdGVyLWRyLWppdGVuZHJhLXNpbmdoLTI0NDEyNS_SAZ0BaHR0cHM6Ly93d3cuamFpc2FsbWVybmV3cy5jb20vbmV3cy9uYXRpb25hbC9pbmRpYS1oYXMtcHJvZHVjZWQtb3Zlci00MC1xdWFudHVtLXRlY2hub2xvZ3ktc3RhcnQtdXBzLWluLXR3by15ZWFycy11bmlvbi1taW5pc3Rlci1kci1qaXRlbmRyYS1zaW5naC0yNDQxMjUvYW1wLw?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>Generating photon pairs from a liquid crystal source | Globe Echo</t>
+          <t>From Uncommon White Powder to Quantum Innovation: Discovering Nearly Noiseless Qubits is a valuable resource for learning about quantum computing</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
@@ -4577,7 +4577,7 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiS2h0dHBzOi8vZ2xvYmVlY2hvLmNvbS9nZW5lcmF0aW5nLXBob3Rvbi1wYWlycy1mcm9tLWEtbGlxdWlkLWNyeXN0YWwtc291cmNlL9IBT2h0dHBzOi8vZ2xvYmVlY2hvLmNvbS9nZW5lcmF0aW5nLXBob3Rvbi1wYWlycy1mcm9tLWEtbGlxdWlkLWNyeXN0YWwtc291cmNlL2FtcC8?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMigAFodHRwczovL2xpc3QyMy5jb20vMzgwMTU2NS1mcm9tLXVuY29tbW9uLXdoaXRlLXBvd2Rlci10by1xdWFudHVtLWlubm92YXRpb24tZGlzY292ZXJpbmctbmVhcmx5LW5vaXNlbGVzcy1xdWJpdHMtaXMtYS12YWx1YWJsZS1yL9IBhAFodHRwczovL2xpc3QyMy5jb20vMzgwMTU2NS1mcm9tLXVuY29tbW9uLXdoaXRlLXBvd2Rlci10by1xdWFudHVtLWlubm92YXRpb24tZGlzY292ZXJpbmctbmVhcmx5LW5vaXNlbGVzcy1xdWJpdHMtaXMtYS12YWx1YWJsZS1yL2FtcC8?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
@@ -4618,51 +4618,51 @@
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>From Uncommon White Powder to Quantum Innovation: Discovering Nearly Noiseless Qubits is a valuable resource for learning about quantum computing</t>
+          <t>From Common White Powder to Quantum Innovation: Unlocking Nearly Noiseless Qubits</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>2024-06-15 14:51:30.303962</t>
+          <t>2024-06-15 15:23:50.061647</t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMigAFodHRwczovL2xpc3QyMy5jb20vMzgwMTU2NS1mcm9tLXVuY29tbW9uLXdoaXRlLXBvd2Rlci10by1xdWFudHVtLWlubm92YXRpb24tZGlzY292ZXJpbmctbmVhcmx5LW5vaXNlbGVzcy1xdWJpdHMtaXMtYS12YWx1YWJsZS1yL9IBhAFodHRwczovL2xpc3QyMy5jb20vMzgwMTU2NS1mcm9tLXVuY29tbW9uLXdoaXRlLXBvd2Rlci10by1xdWFudHVtLWlubm92YXRpb24tZGlzY292ZXJpbmctbmVhcmx5LW5vaXNlbGVzcy1xdWJpdHMtaXMtYS12YWx1YWJsZS1yL2FtcC8?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiamh0dHBzOi8vc2NpdGVjaGRhaWx5LmNvbS9mcm9tLWNvbW1vbi13aGl0ZS1wb3dkZXItdG8tcXVhbnR1bS1pbm5vdmF0aW9uLXVubG9ja2luZy1uZWFybHktbm9pc2VsZXNzLXF1Yml0cy_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>India Has Produced Over 40 Quantum Technology Start-Ups In Two Years: Union Minister Dr. Jitendra Singh |</t>
+          <t>Panama and Canada's First Quantum agree details for copper mine contract</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>2024-06-15 14:51:30.303962</t>
+          <t>2024-06-15 16:03:03.143083</t>
         </is>
       </c>
       <c r="C248" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMimQFodHRwczovL3d3dy5qYWlzYWxtZXJuZXdzLmNvbS9uZXdzL25hdGlvbmFsL2luZGlhLWhhcy1wcm9kdWNlZC1vdmVyLTQwLXF1YW50dW0tdGVjaG5vbG9neS1zdGFydC11cHMtaW4tdHdvLXllYXJzLXVuaW9uLW1pbmlzdGVyLWRyLWppdGVuZHJhLXNpbmdoLTI0NDEyNS_SAZ0BaHR0cHM6Ly93d3cuamFpc2FsbWVybmV3cy5jb20vbmV3cy9uYXRpb25hbC9pbmRpYS1oYXMtcHJvZHVjZWQtb3Zlci00MC1xdWFudHVtLXRlY2hub2xvZ3ktc3RhcnQtdXBzLWluLXR3by15ZWFycy11bmlvbi1taW5pc3Rlci1kci1qaXRlbmRyYS1zaW5naC0yNDQxMjUvYW1wLw?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiWmh0dHBzOi8vY2EubW92aWVzLnlhaG9vLmNvbS9maW5hbmNlL25ld3MvcGFuYW1hLWNhbmFkYXMtZmlyc3QtcXVhbnR1bS1hZ3JlZS0xNTI2MTgxNzQuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>Panama and Canada's First Quantum agree details for copper mine contract</t>
+          <t>Huge fault-tolerant quantum computers on the agenda at Commercialising Quantum 2024 conference – Physics World</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>2024-06-15 15:00:16.898297</t>
+          <t>2024-06-15 16:03:03.144616</t>
         </is>
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiWmh0dHBzOi8vY2EubW92aWVzLnlhaG9vLmNvbS9maW5hbmNlL25ld3MvcGFuYW1hLWNhbmFkYXMtZmlyc3QtcXVhbnR1bS1hZ3JlZS0xNTI2MTgxNzQuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiemh0dHBzOi8vcGh5c2ljc3dvcmxkLmNvbS9hL2h1Z2UtZmF1bHQtdG9sZXJhbnQtcXVhbnR1bS1jb21wdXRlcnMtb24tdGhlLWFnZW5kYS1hdC1jb21tZXJjaWFsaXNpbmctcXVhbnR1bS0yMDI0LWNvbmZlcmVuY2Uv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
@@ -4674,7 +4674,7 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>2024-06-15 15:23:50.050461</t>
+          <t>2024-06-15 16:03:03.144616</t>
         </is>
       </c>
       <c r="C250" t="inlineStr">
@@ -4686,221 +4686,221 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>Huge fault-tolerant quantum computers on the agenda at Commercialising Quantum 2024 conference – Physics World</t>
+          <t>Anyon quantum dimensions from an arbitrary ground state wave function</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>2024-06-15 15:23:50.050461</t>
+          <t>2024-06-15 16:03:03.145649</t>
         </is>
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiemh0dHBzOi8vcGh5c2ljc3dvcmxkLmNvbS9hL2h1Z2UtZmF1bHQtdG9sZXJhbnQtcXVhbnR1bS1jb21wdXRlcnMtb24tdGhlLWFnZW5kYS1hdC1jb21tZXJjaWFsaXNpbmctcXVhbnR1bS0yMDI0LWNvbmZlcmVuY2Uv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiMmh0dHBzOi8vd3d3Lm5hdHVyZS5jb20vYXJ0aWNsZXMvczQxNDY3LTAyNC00Nzg1Ni030gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>Anyon quantum dimensions from an arbitrary ground state wave function</t>
+          <t>Zero Point Cryogenics Secures $2.67 Million (CAD) in Funding to Fuel Growth</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>2024-06-15 15:23:50.050461</t>
+          <t>2024-06-15 16:03:03.146646</t>
         </is>
       </c>
       <c r="C252" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiMmh0dHBzOi8vd3d3Lm5hdHVyZS5jb20vYXJ0aWNsZXMvczQxNDY3LTAyNC00Nzg1Ni030gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMicmh0dHBzOi8vdGhlcXVhbnR1bWluc2lkZXIuY29tLzIwMjQvMDYvMTUvemVyby1wb2ludC1jcnlvZ2VuaWNzLXNlY3VyZXMtMi02Ny1taWxsaW9uLWNhZC1pbi1mdW5kaW5nLXRvLWZ1ZWwtZ3Jvd3RoL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>Zero Point Cryogenics Secures $2.67 Million (CAD) in Funding to Fuel Growth</t>
+          <t>Superposition Guy's Podcast -- Dominik Ulmer, Chief Quantum Solutions officer at ParTec The Superposition Guy's ...</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>2024-06-15 15:23:50.050461</t>
+          <t>2024-06-15 16:03:03.148645</t>
         </is>
       </c>
       <c r="C253" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMicmh0dHBzOi8vdGhlcXVhbnR1bWluc2lkZXIuY29tLzIwMjQvMDYvMTUvemVyby1wb2ludC1jcnlvZ2VuaWNzLXNlY3VyZXMtMi02Ny1taWxsaW9uLWNhZC1pbi1mdW5kaW5nLXRvLWZ1ZWwtZ3Jvd3RoL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMifGh0dHBzOi8vdGhlcXVhbnR1bWluc2lkZXIuY29tLzIwMjQvMDYvMTUvc3VwZXJwb3NpdGlvbi1ndXlzLXBvZGNhc3QtZG9taW5pay11bG1lci1jaGllZi1xdWFudHVtLXNvbHV0aW9ucy1vZmZpY2VyLWF0LXBhcnRlYy_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>Superposition Guy's Podcast -- Dominik Ulmer, Chief Quantum Solutions officer at ParTec The Superposition Guy's ...</t>
+          <t>Nonlocal correlations transmitted between quantum dots via short topological superconductor | Scientific Reports</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>2024-06-15 15:23:50.060570</t>
+          <t>2024-06-15 16:03:03.149646</t>
         </is>
       </c>
       <c r="C254" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMifGh0dHBzOi8vdGhlcXVhbnR1bWluc2lkZXIuY29tLzIwMjQvMDYvMTUvc3VwZXJwb3NpdGlvbi1ndXlzLXBvZGNhc3QtZG9taW5pay11bG1lci1jaGllZi1xdWFudHVtLXNvbHV0aW9ucy1vZmZpY2VyLWF0LXBhcnRlYy_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiMmh0dHBzOi8vd3d3Lm5hdHVyZS5jb20vYXJ0aWNsZXMvczQxNTk4LTAyNC02NDU3OC000gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>From Common White Powder to Quantum Innovation: Unlocking Nearly Noiseless Qubits</t>
+          <t>What Is a Quantum Battery? And When Will It Power My Laptop?</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>2024-06-15 15:23:50.061647</t>
+          <t>2024-06-15 16:03:03.149646</t>
         </is>
       </c>
       <c r="C255" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiamh0dHBzOi8vc2NpdGVjaGRhaWx5LmNvbS9mcm9tLWNvbW1vbi13aGl0ZS1wb3dkZXItdG8tcXVhbnR1bS1pbm5vdmF0aW9uLXVubG9ja2luZy1uZWFybHktbm9pc2VsZXNzLXF1Yml0cy_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiVWh0dHBzOi8vZ2l6bW9kby5jb20vd2hhdC1pcy1hLXF1YW50dW0tYmF0dGVyeS1hbmQtd2hlbi13aWxsLWl0LXBvd2VyLW15LWxhLTE4NTE1MjIwNjLSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>Nonlocal correlations transmitted between quantum dots via short topological superconductor | Scientific Reports</t>
+          <t>Guest Post -- The Road to the Proclamation of IYQ2025</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>2024-06-15 15:23:50.061647</t>
+          <t>2024-06-15 16:03:03.150645</t>
         </is>
       </c>
       <c r="C256" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiMmh0dHBzOi8vd3d3Lm5hdHVyZS5jb20vYXJ0aWNsZXMvczQxNTk4LTAyNC02NDU3OC000gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiXGh0dHBzOi8vdGhlcXVhbnR1bWluc2lkZXIuY29tLzIwMjQvMDYvMTUvZ3Vlc3QtcG9zdC10aGUtcm9hZC10by10aGUtcHJvY2xhbWF0aW9uLW9mLWl5cTIwMjUv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>What Is a Quantum Battery? And When Will It Power My Laptop?</t>
+          <t>An Improved Method for Quantum Matrix Multiplication: Main Procedure</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>2024-06-15 15:23:50.062710</t>
+          <t>2024-06-15 16:03:03.152646</t>
         </is>
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiVWh0dHBzOi8vZ2l6bW9kby5jb20vd2hhdC1pcy1hLXF1YW50dW0tYmF0dGVyeS1hbmQtd2hlbi13aWxsLWl0LXBvd2VyLW15LWxhLTE4NTE1MjIwNjLSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiWmh0dHBzOi8vaGFja2Vybm9vbi5jb20vYW4taW1wcm92ZWQtbWV0aG9kLWZvci1xdWFudHVtLW1hdHJpeC1tdWx0aXBsaWNhdGlvbi1tYWluLXByb2NlZHVyZdIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>Record 99.9% quantum computing accuracy achieved on existing silicon chips</t>
+          <t>What if a nonmagnetic material could be magnetic?</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>2024-06-15 15:23:50.063739</t>
+          <t>2024-06-15 16:03:03.152646</t>
         </is>
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiYGh0dHBzOi8vaW50ZXJlc3RpbmdlbmdpbmVlcmluZy5jb20vaW5ub3ZhdGlvbi9yZWNvcmQtcXVhbnR1bS1jb21wdXRpbmctYWNjdXJhY3ktZXhpc3Rpbmctc2lsaWNvbtIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiMGh0dHBzOi8vd3d3LmV1cmVrYWxlcnQub3JnL25ld3MtcmVsZWFzZXMvMTA0ODM1MtIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>Guest Post -- The Road to the Proclamation of IYQ2025</t>
+          <t>IBM and Japan institute team up to develop next-gen quantum computer</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>2024-06-15 15:23:50.064735</t>
+          <t>2024-06-15 16:03:03.154258</t>
         </is>
       </c>
       <c r="C259" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiXGh0dHBzOi8vdGhlcXVhbnR1bWluc2lkZXIuY29tLzIwMjQvMDYvMTUvZ3Vlc3QtcG9zdC10aGUtcm9hZC10by10aGUtcHJvY2xhbWF0aW9uLW9mLWl5cTIwMjUv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMicGh0dHBzOi8vYXNpYS5uaWtrZWkuY29tL0J1c2luZXNzL1RlY2hub2xvZ3kvSUJNLWFuZC1KYXBhbi1pbnN0aXR1dGUtdGVhbS11cC10by1kZXZlbG9wLW5leHQtZ2VuLXF1YW50dW0tY29tcHV0ZXLSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>An Improved Method for Quantum Matrix Multiplication: Main Procedure</t>
+          <t>Everyone Missed 1 Detail In The MCU's Most Recent Movie, But I Can't Wait To See What It Means</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>2024-06-15 15:23:50.067730</t>
+          <t>2024-06-15 16:03:03.154258</t>
         </is>
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiWmh0dHBzOi8vaGFja2Vybm9vbi5jb20vYW4taW1wcm92ZWQtbWV0aG9kLWZvci1xdWFudHVtLW1hdHJpeC1tdWx0aXBsaWNhdGlvbi1tYWluLXByb2NlZHVyZdIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiTWh0dHBzOi8vc2NyZWVucmFudC5jb20vdGhlLW1hcnZlbHMtbWlzc2VkLWRldGFpbC1xdWFudHVtLWJhbmRzLW1hcmlhLXJhbWJlYXUv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>What if a nonmagnetic material could be magnetic?</t>
+          <t>Gemma Arterton Says She Gets 'Criticism' for Quantum of Solace : There's 'So Much Wrong with Bond Women'</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>2024-06-15 15:23:50.068730</t>
+          <t>2024-06-15 16:03:03.155183</t>
         </is>
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiMGh0dHBzOi8vd3d3LmV1cmVrYWxlcnQub3JnL25ld3MtcmVsZWFzZXMvMTA0ODM1MtIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiR2h0dHBzOi8vdWsubW92aWVzLnlhaG9vLmNvbS9nZW1tYS1hcnRlcnRvbi1zYXlzLXNoZS1nZXRzLTE2MTkzMDYzNy5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>IBM and Japan institute team up to develop next-gen quantum computer</t>
+          <t>Quantum entanglement measures Earth's spin with never-before-seen accuracy</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>2024-06-15 15:23:50.068730</t>
+          <t>2024-06-15 16:03:03.156182</t>
         </is>
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMicGh0dHBzOi8vYXNpYS5uaWtrZWkuY29tL0J1c2luZXNzL1RlY2hub2xvZ3kvSUJNLWFuZC1KYXBhbi1pbnN0aXR1dGUtdGVhbS11cC10by1kZXZlbG9wLW5leHQtZ2VuLXF1YW50dW0tY29tcHV0ZXLSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMingFodHRwczovL3d3dy5tc24uY29tL2VuLXVzL25ld3MvdGVjaG5vbG9neS9xdWFudHVtLWVudGFuZ2xlbWVudC1tZWFzdXJlcy1lYXJ0aC1zLXNwaW4td2l0aC1uZXZlci1iZWZvcmUtc2Vlbi1hY2N1cmFjeS9hci1CQjFvZjZWZj9pdGVtPWZsaWdodHNwcmctdGlwc3Vic2MtdjFhL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>Everyone Missed 1 Detail In The MCU's Most Recent Movie, But I Can't Wait To See What It Means</t>
+          <t>Quantum Encryption &amp; the Rise of Cybersecuritys Superhero ‍♂️ | Tech News with Comed-AI-n</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>2024-06-15 15:23:50.070288</t>
+          <t>2024-06-15 16:03:03.157180</t>
         </is>
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiTWh0dHBzOi8vc2NyZWVucmFudC5jb20vdGhlLW1hcnZlbHMtbWlzc2VkLWRldGFpbC1xdWFudHVtLWJhbmRzLW1hcmlhLXJhbWJlYXUv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMirwFodHRwczovL21lZGl1bS5jb20vQENvbWVkX0FJX24vcXVhbnR1bS1lbmNyeXB0aW9uLXRoZS1yaXNlLW9mLWN5YmVyc2VjdXJpdHlzLXN1cGVyaGVyby0lRUYlQjglOEYtdGVjaC1uZXdzLXdpdGgtY29tZWQtYWktbi01ZTUxODc1YzRmYzA_cmVzcG9uc2VzT3Blbj10cnVlJnNvcnRCeT1SRVZFUlNFX0NIUk9O0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
@@ -4958,12 +4958,12 @@
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>"Spooky action at a distance" confirmed in heaviest particles</t>
+          <t>"Spooky action at a distance" confirmed to persist between top quarks</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>2024-06-15 20:23:50.060570</t>
+          <t>2024-06-15 20:51:30.298139</t>
         </is>
       </c>
       <c r="C267" t="inlineStr">
@@ -4975,12 +4975,12 @@
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>"Spooky action at a distance" confirmed to persist between top quarks</t>
+          <t>"Spooky action at a distance" confirmed in heaviest particles</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>2024-06-15 20:51:30.298139</t>
+          <t>2024-06-15 21:03:03.148645</t>
         </is>
       </c>
       <c r="C268" t="inlineStr">
@@ -5014,7 +5014,7 @@
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>2024-06-15 23:23:50.050461</t>
+          <t>2024-06-15 23:03:03.143083</t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
@@ -5043,66 +5043,83 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>Jitendra Singh says over 40 quantum technology startups emerged in two years</t>
+          <t>Record 99.9% quantum computing accuracy achieved on existing silicon chips</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>2024-06-16 00:51:30.298139</t>
+          <t>2024-06-16 00:03:03.148645</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMijwFodHRwczovL3d3dy50aGVoaW5kdWJ1c2luZXNzbGluZS5jb20vaW5mby10ZWNoL2ppdGVuZHJhLXNpbmdoLXNheXMtb3Zlci00MC1xdWFudHVtLXRlY2hub2xvZ3ktc3RhcnR1cHMtZW1lcmdlZC1pbi10d28teWVhcnMvYXJ0aWNsZTY4Mjk2MDI3LmVjZdIBlAFodHRwczovL3d3dy50aGVoaW5kdWJ1c2luZXNzbGluZS5jb20vaW5mby10ZWNoL2ppdGVuZHJhLXNpbmdoLXNheXMtb3Zlci00MC1xdWFudHVtLXRlY2hub2xvZ3ktc3RhcnR1cHMtZW1lcmdlZC1pbi10d28teWVhcnMvYXJ0aWNsZTY4Mjk2MDI3LmVjZS9hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMitgFodHRwczovL3d3dy5tc24uY29tL2VuLXVzL25ld3MvdGVjaG5vbG9neS9yZWNvcmQtOTktOS1xdWFudHVtLWNvbXB1dGluZy1hY2N1cmFjeS1hY2hpZXZlZC1vbi1leGlzdGluZy1zaWxpY29uLWNoaXBzL2FyLUJCMW9oN0VVP2l0ZW09dGhlbWVkX2ZlYXR1cmVkYXBwc19lbmFibGVEP2xvYWRJbj1kZWZhdWx0QnJvd3NlctIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>Quantum Racing powered by American Magic on the cusp of hometown win...</t>
+          <t>Jitendra Singh says over 40 quantum technology startups emerged in two years</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>2024-06-16 01:23:50.050461</t>
+          <t>2024-06-16 00:03:03.156182</t>
         </is>
       </c>
       <c r="C273" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiYWh0dHBzOi8vd3d3LmxpdmVzYWlsZGllLmNvbS9xdWFudHVtLXJhY2luZy1wb3dlcmVkLWJ5LWFtZXJpY2FuLW1hZ2ljLW9uLXRoZS1jdXNwLW9mLWhvbWV0b3duLXdpbi_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMijwFodHRwczovL3d3dy50aGVoaW5kdWJ1c2luZXNzbGluZS5jb20vaW5mby10ZWNoL2ppdGVuZHJhLXNpbmdoLXNheXMtb3Zlci00MC1xdWFudHVtLXRlY2hub2xvZ3ktc3RhcnR1cHMtZW1lcmdlZC1pbi10d28teWVhcnMvYXJ0aWNsZTY4Mjk2MDI3LmVjZdIBlAFodHRwczovL3d3dy50aGVoaW5kdWJ1c2luZXNzbGluZS5jb20vaW5mby10ZWNoL2ppdGVuZHJhLXNpbmdoLXNheXMtb3Zlci00MC1xdWFudHVtLXRlY2hub2xvZ3ktc3RhcnR1cHMtZW1lcmdlZC1pbi10d28teWVhcnMvYXJ0aWNsZTY4Mjk2MDI3LmVjZS9hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>Quantum entangled photons used to measure the Earth's rotation</t>
+          <t>Quantum Racing powered by American Magic on the cusp of hometown win…</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>2024-06-16 01:23:50.050461</t>
+          <t>2024-06-16 01:51:30.298139</t>
         </is>
       </c>
       <c r="C274" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiV2h0dHBzOi8vd3d3LmVhcnRoLmNvbS9uZXdzL3F1YW50dW0tZW50YW5nbGVtZW50LXBob3RvbnMtdXNlZC10by1tZWFzdXJlLWVhcnRoLXJvdGF0aW9uL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiYWh0dHBzOi8vd3d3LmxpdmVzYWlsZGllLmNvbS9xdWFudHVtLXJhY2luZy1wb3dlcmVkLWJ5LWFtZXJpY2FuLW1hZ2ljLW9uLXRoZS1jdXNwLW9mLWhvbWV0b3duLXdpbi_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>Quantum Racing powered by American Magic on the cusp of hometown win…</t>
+          <t>Quantum entangled photons used to measure the Earth's rotation</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>2024-06-16 01:51:30.298139</t>
+          <t>2024-06-16 02:03:03.144083</t>
         </is>
       </c>
       <c r="C275" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiV2h0dHBzOi8vd3d3LmVhcnRoLmNvbS9uZXdzL3F1YW50dW0tZW50YW5nbGVtZW50LXBob3RvbnMtdXNlZC10by1tZWFzdXJlLWVhcnRoLXJvdGF0aW9uL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>Quantum Racing powered by American Magic on the cusp of hometown win...</t>
+        </is>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>2024-06-16 02:03:03.144083</t>
+        </is>
+      </c>
+      <c r="C276" t="inlineStr">
         <is>
           <t>news.google.com/articles/CBMiYWh0dHBzOi8vd3d3LmxpdmVzYWlsZGllLmNvbS9xdWFudHVtLXJhY2luZy1wb3dlcmVkLWJ5LWFtZXJpY2FuLW1hZ2ljLW9uLXRoZS1jdXNwLW9mLWhvbWV0b3duLXdpbi_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>

</xml_diff>